<commit_message>
Update Clean_Data and Label
</commit_message>
<xml_diff>
--- a/Label.xlsx
+++ b/Label.xlsx
@@ -31,7 +31,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="402" uniqueCount="180">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="430" uniqueCount="181">
   <si>
     <t>Note</t>
   </si>
@@ -732,6 +732,9 @@
   <si>
     <t>Pt13Eb</t>
   </si>
+  <si>
+    <t>NaN</t>
+  </si>
 </sst>
 </file>
 
@@ -756,6 +759,14 @@
       <color theme="1"/>
       <name val="Times New Roman"/>
       <charset val="134"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="等线"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
     </font>
     <font>
       <sz val="9"/>
@@ -859,14 +870,6 @@
     <font>
       <sz val="11"/>
       <color rgb="FFFA7D00"/>
-      <name val="等线"/>
-      <charset val="134"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <color theme="1"/>
       <name val="等线"/>
       <charset val="134"/>
       <scheme val="minor"/>
@@ -1229,16 +1232,13 @@
     <xf numFmtId="42" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="1" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="1" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
@@ -1247,34 +1247,37 @@
     <xf numFmtId="0" fontId="7" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="2" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="3" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="2" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="4" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="3" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="4" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="11" fillId="3" borderId="5" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="12" fillId="4" borderId="6" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="12" fillId="3" borderId="5" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="13" fillId="4" borderId="5" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="13" fillId="4" borderId="6" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="14" fillId="5" borderId="7" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="14" fillId="4" borderId="5" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="15" fillId="0" borderId="8" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="15" fillId="5" borderId="7" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="16" fillId="0" borderId="9" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="16" fillId="0" borderId="8" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="9" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="17" fillId="6" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
@@ -1359,12 +1362,18 @@
       <alignment vertical="center"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="5">
+  <cellXfs count="7">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1">
       <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
@@ -1372,7 +1381,7 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1">
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1">
       <alignment vertical="center"/>
     </xf>
   </cellXfs>
@@ -1445,16 +1454,16 @@
 <xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
   <xdr:twoCellAnchor editAs="oneCell">
     <xdr:from>
-      <xdr:col>5</xdr:col>
-      <xdr:colOff>311150</xdr:colOff>
-      <xdr:row>18</xdr:row>
-      <xdr:rowOff>88900</xdr:rowOff>
+      <xdr:col>8</xdr:col>
+      <xdr:colOff>342900</xdr:colOff>
+      <xdr:row>0</xdr:row>
+      <xdr:rowOff>107950</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>10</xdr:col>
-      <xdr:colOff>247650</xdr:colOff>
-      <xdr:row>30</xdr:row>
-      <xdr:rowOff>114300</xdr:rowOff>
+      <xdr:col>13</xdr:col>
+      <xdr:colOff>279400</xdr:colOff>
+      <xdr:row>12</xdr:row>
+      <xdr:rowOff>133350</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
@@ -1471,7 +1480,7 @@
       </xdr:blipFill>
       <xdr:spPr>
         <a:xfrm>
-          <a:off x="3441700" y="3632200"/>
+          <a:off x="5454650" y="107950"/>
           <a:ext cx="3238500" cy="2387600"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
@@ -1748,12 +1757,12 @@
   <sheetPr/>
   <dimension ref="A1:KB66"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="110" zoomScaleNormal="110" workbookViewId="0">
-      <pane xSplit="3" ySplit="1" topLeftCell="R2" activePane="bottomRight" state="frozen"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <pane xSplit="3" ySplit="1" topLeftCell="O2" activePane="bottomRight" state="frozen"/>
       <selection/>
       <selection pane="topRight"/>
       <selection pane="bottomLeft"/>
-      <selection pane="bottomRight" activeCell="W6" sqref="W6"/>
+      <selection pane="bottomRight" activeCell="T8" sqref="T8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9" defaultRowHeight="14"/>
@@ -1773,12 +1782,12 @@
     <col min="14" max="14" width="12.9166666666667" customWidth="1"/>
     <col min="15" max="15" width="12.75" customWidth="1"/>
     <col min="16" max="16" width="9" customWidth="1"/>
-    <col min="17" max="17" width="37" customWidth="1"/>
+    <col min="17" max="17" width="41.6666666666667" customWidth="1"/>
     <col min="18" max="18" width="29" customWidth="1"/>
     <col min="20" max="20" width="13.25" customWidth="1"/>
     <col min="21" max="21" width="17.4166666666667" customWidth="1"/>
     <col min="22" max="22" width="8.66666666666667" customWidth="1"/>
-    <col min="23" max="23" width="23.8333333333333" style="2" customWidth="1"/>
+    <col min="23" max="23" width="23.8333333333333" style="4" customWidth="1"/>
     <col min="24" max="24" width="14.5" customWidth="1"/>
   </cols>
   <sheetData>
@@ -1789,7 +1798,7 @@
       <c r="B1" s="1" t="s">
         <v>1</v>
       </c>
-      <c r="C1" s="3" t="s">
+      <c r="C1" s="5" t="s">
         <v>2</v>
       </c>
       <c r="D1" s="1" t="s">
@@ -1849,7 +1858,7 @@
       <c r="V1" t="s">
         <v>21</v>
       </c>
-      <c r="W1" s="2" t="s">
+      <c r="W1" s="4" t="s">
         <v>22</v>
       </c>
       <c r="X1" t="s">
@@ -1923,7 +1932,7 @@
         <v>0</v>
       </c>
       <c r="W2" s="1"/>
-      <c r="X2" s="4" t="s">
+      <c r="X2" s="6" t="s">
         <v>33</v>
       </c>
       <c r="Y2" s="1">
@@ -2256,7 +2265,7 @@
         <v>0</v>
       </c>
       <c r="W3" s="1"/>
-      <c r="X3" s="4" t="s">
+      <c r="X3" s="6" t="s">
         <v>33</v>
       </c>
       <c r="Y3" s="1">
@@ -2589,7 +2598,7 @@
         <v>0</v>
       </c>
       <c r="W4" s="1"/>
-      <c r="X4" s="4" t="s">
+      <c r="X4" s="6" t="s">
         <v>33</v>
       </c>
       <c r="Y4" s="1">
@@ -2922,7 +2931,7 @@
         <v>0</v>
       </c>
       <c r="W5" s="1"/>
-      <c r="X5" s="4" t="s">
+      <c r="X5" s="6" t="s">
         <v>33</v>
       </c>
       <c r="Y5" s="1">
@@ -3259,7 +3268,7 @@
         <v>0</v>
       </c>
       <c r="W6" s="1"/>
-      <c r="X6" s="4" t="s">
+      <c r="X6" s="6" t="s">
         <v>33</v>
       </c>
       <c r="Y6" s="1">
@@ -21925,224 +21934,380 @@
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:etc="http://www.wps.cn/officeDocument/2017/etCustomData">
   <sheetPr/>
-  <dimension ref="A1:B66"/>
+  <dimension ref="A1:E66"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="A48" sqref="A48"/>
+      <selection activeCell="I17" sqref="I17"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.66666666666667" defaultRowHeight="14" outlineLevelCol="1"/>
+  <sheetFormatPr defaultColWidth="8.66666666666667" defaultRowHeight="14" outlineLevelCol="4"/>
   <cols>
     <col min="1" max="1" width="6.08333333333333" customWidth="1"/>
     <col min="2" max="2" width="9" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" ht="15.5" spans="1:2">
+    <row r="1" ht="15.5" spans="1:5">
       <c r="A1" s="1" t="s">
         <v>3</v>
       </c>
       <c r="B1" s="1" t="s">
         <v>5</v>
       </c>
+      <c r="D1" s="2" t="s">
+        <v>3</v>
+      </c>
+      <c r="E1" s="2" t="s">
+        <v>5</v>
+      </c>
     </row>
-    <row r="2" ht="15.5" spans="1:2">
+    <row r="2" ht="15.5" spans="1:5">
       <c r="A2" s="1" t="s">
         <v>28</v>
       </c>
       <c r="B2" s="1">
         <v>2019</v>
       </c>
+      <c r="D2" s="3" t="s">
+        <v>28</v>
+      </c>
+      <c r="E2" s="3">
+        <v>2019</v>
+      </c>
     </row>
-    <row r="3" ht="15.5" spans="1:2">
+    <row r="3" ht="15.5" spans="1:5">
       <c r="A3" s="1" t="s">
         <v>28</v>
       </c>
       <c r="B3" s="1">
         <v>2019</v>
       </c>
+      <c r="D3" s="3" t="s">
+        <v>41</v>
+      </c>
+      <c r="E3" s="3">
+        <v>2020</v>
+      </c>
     </row>
-    <row r="4" ht="15.5" spans="1:2">
+    <row r="4" ht="15.5" spans="1:5">
       <c r="A4" s="1" t="s">
         <v>28</v>
       </c>
       <c r="B4" s="1">
         <v>2019</v>
       </c>
+      <c r="D4" s="3" t="s">
+        <v>49</v>
+      </c>
+      <c r="E4" s="3">
+        <v>2020</v>
+      </c>
     </row>
-    <row r="5" ht="15.5" spans="1:2">
+    <row r="5" ht="15.5" spans="1:5">
       <c r="A5" s="1" t="s">
         <v>28</v>
       </c>
       <c r="B5" s="1">
         <v>2019</v>
       </c>
+      <c r="D5" s="3" t="s">
+        <v>54</v>
+      </c>
+      <c r="E5" s="3">
+        <v>2020</v>
+      </c>
     </row>
-    <row r="6" ht="15.5" spans="1:2">
+    <row r="6" ht="15.5" spans="1:5">
       <c r="A6" s="1" t="s">
         <v>41</v>
       </c>
       <c r="B6" s="1">
         <v>2020</v>
       </c>
+      <c r="D6" s="3" t="s">
+        <v>58</v>
+      </c>
+      <c r="E6" s="3">
+        <v>2020</v>
+      </c>
     </row>
-    <row r="7" ht="15.5" spans="1:2">
+    <row r="7" ht="15.5" spans="1:5">
       <c r="A7" s="1" t="s">
         <v>49</v>
       </c>
       <c r="B7" s="1">
         <v>2020</v>
       </c>
+      <c r="D7" s="3" t="s">
+        <v>67</v>
+      </c>
+      <c r="E7" s="3">
+        <v>2019</v>
+      </c>
     </row>
-    <row r="8" ht="15.5" spans="1:2">
+    <row r="8" ht="15.5" spans="1:5">
       <c r="A8" s="1" t="s">
         <v>54</v>
       </c>
       <c r="B8" s="1">
         <v>2020</v>
       </c>
+      <c r="D8" s="3" t="s">
+        <v>76</v>
+      </c>
+      <c r="E8" s="3">
+        <v>2018</v>
+      </c>
     </row>
-    <row r="9" ht="15.5" spans="1:2">
+    <row r="9" ht="15.5" spans="1:5">
       <c r="A9" s="1" t="s">
         <v>58</v>
       </c>
       <c r="B9" s="1">
         <v>2020</v>
       </c>
+      <c r="D9" s="3" t="s">
+        <v>83</v>
+      </c>
+      <c r="E9" s="3">
+        <v>2021</v>
+      </c>
     </row>
-    <row r="10" ht="15.5" spans="1:2">
+    <row r="10" ht="15.5" spans="1:5">
       <c r="A10" s="1" t="s">
         <v>58</v>
       </c>
       <c r="B10" s="1">
         <v>2020</v>
       </c>
+      <c r="D10" s="3" t="s">
+        <v>87</v>
+      </c>
+      <c r="E10" s="3">
+        <v>2021</v>
+      </c>
     </row>
-    <row r="11" ht="15.5" spans="1:2">
+    <row r="11" ht="15.5" spans="1:5">
       <c r="A11" s="1" t="s">
         <v>67</v>
       </c>
       <c r="B11" s="1">
         <v>2019</v>
       </c>
+      <c r="D11" s="3" t="s">
+        <v>93</v>
+      </c>
+      <c r="E11" s="3">
+        <v>2022</v>
+      </c>
     </row>
-    <row r="12" ht="15.5" spans="1:2">
+    <row r="12" ht="15.5" spans="1:5">
       <c r="A12" s="1" t="s">
         <v>67</v>
       </c>
       <c r="B12" s="1">
         <v>2019</v>
       </c>
+      <c r="D12" s="3" t="s">
+        <v>101</v>
+      </c>
+      <c r="E12" s="3">
+        <v>2021</v>
+      </c>
     </row>
-    <row r="13" ht="15.5" spans="1:2">
+    <row r="13" ht="15.5" spans="1:5">
       <c r="A13" s="1" t="s">
         <v>76</v>
       </c>
       <c r="B13" s="1">
         <v>2018</v>
       </c>
+      <c r="D13" s="3" t="s">
+        <v>106</v>
+      </c>
+      <c r="E13" s="3">
+        <v>2023</v>
+      </c>
     </row>
-    <row r="14" ht="15.5" spans="1:2">
+    <row r="14" ht="15.5" spans="1:5">
       <c r="A14" s="1" t="s">
         <v>76</v>
       </c>
       <c r="B14" s="1">
         <v>2018</v>
       </c>
+      <c r="D14" s="3" t="s">
+        <v>111</v>
+      </c>
+      <c r="E14" s="3">
+        <v>2023</v>
+      </c>
     </row>
-    <row r="15" ht="15.5" spans="1:2">
+    <row r="15" ht="15.5" spans="1:5">
       <c r="A15" s="1" t="s">
         <v>83</v>
       </c>
       <c r="B15" s="1">
         <v>2021</v>
       </c>
+      <c r="D15" s="3" t="s">
+        <v>116</v>
+      </c>
+      <c r="E15" s="3">
+        <v>2014</v>
+      </c>
     </row>
-    <row r="16" ht="15.5" spans="1:2">
+    <row r="16" ht="15.5" spans="1:5">
       <c r="A16" s="1" t="s">
         <v>87</v>
       </c>
       <c r="B16" s="1">
         <v>2021</v>
       </c>
+      <c r="D16" s="3" t="s">
+        <v>120</v>
+      </c>
+      <c r="E16" s="3">
+        <v>2015</v>
+      </c>
     </row>
-    <row r="17" ht="15.5" spans="1:2">
+    <row r="17" ht="15.5" spans="1:5">
       <c r="A17" s="1" t="s">
         <v>87</v>
       </c>
       <c r="B17" s="1">
         <v>2021</v>
       </c>
+      <c r="D17" s="3" t="s">
+        <v>124</v>
+      </c>
+      <c r="E17" s="3">
+        <v>2014</v>
+      </c>
     </row>
-    <row r="18" ht="15.5" spans="1:2">
+    <row r="18" ht="15.5" spans="1:5">
       <c r="A18" s="1" t="s">
         <v>87</v>
       </c>
       <c r="B18" s="1">
         <v>2021</v>
       </c>
+      <c r="D18" s="3" t="s">
+        <v>138</v>
+      </c>
+      <c r="E18" s="3">
+        <v>2023</v>
+      </c>
     </row>
-    <row r="19" ht="15.5" spans="1:2">
+    <row r="19" ht="15.5" spans="1:5">
       <c r="A19" s="1" t="s">
         <v>93</v>
       </c>
       <c r="B19" s="1">
         <v>2022</v>
       </c>
+      <c r="D19" s="3" t="s">
+        <v>142</v>
+      </c>
+      <c r="E19" s="3">
+        <v>2023</v>
+      </c>
     </row>
-    <row r="20" ht="15.5" spans="1:2">
+    <row r="20" ht="15.5" spans="1:5">
       <c r="A20" s="1" t="s">
         <v>93</v>
       </c>
       <c r="B20" s="1">
         <v>2022</v>
       </c>
+      <c r="D20" s="3" t="s">
+        <v>146</v>
+      </c>
+      <c r="E20" s="3">
+        <v>2021</v>
+      </c>
     </row>
-    <row r="21" ht="15.5" spans="1:2">
+    <row r="21" ht="15.5" spans="1:5">
       <c r="A21" s="1" t="s">
         <v>93</v>
       </c>
       <c r="B21" s="1">
         <v>2022</v>
       </c>
+      <c r="D21" s="3" t="s">
+        <v>153</v>
+      </c>
+      <c r="E21" s="3">
+        <v>2023</v>
+      </c>
     </row>
-    <row r="22" ht="15.5" spans="1:2">
+    <row r="22" ht="15.5" spans="1:5">
       <c r="A22" s="1" t="s">
         <v>101</v>
       </c>
       <c r="B22" s="1">
         <v>2021</v>
       </c>
+      <c r="D22" s="3" t="s">
+        <v>157</v>
+      </c>
+      <c r="E22" s="3">
+        <v>2022</v>
+      </c>
     </row>
-    <row r="23" ht="15.5" spans="1:2">
+    <row r="23" ht="15.5" spans="1:5">
       <c r="A23" s="1" t="s">
         <v>106</v>
       </c>
       <c r="B23" s="1">
         <v>2023</v>
       </c>
+      <c r="D23" s="3" t="s">
+        <v>163</v>
+      </c>
+      <c r="E23" s="3">
+        <v>2022</v>
+      </c>
     </row>
-    <row r="24" ht="15.5" spans="1:2">
+    <row r="24" ht="15.5" spans="1:5">
       <c r="A24" s="1" t="s">
         <v>111</v>
       </c>
       <c r="B24" s="1">
         <v>2023</v>
       </c>
+      <c r="D24" s="3" t="s">
+        <v>167</v>
+      </c>
+      <c r="E24" s="3">
+        <v>2020</v>
+      </c>
     </row>
-    <row r="25" ht="15.5" spans="1:2">
+    <row r="25" ht="15.5" spans="1:5">
       <c r="A25" s="1" t="s">
         <v>116</v>
       </c>
       <c r="B25" s="1">
         <v>2014</v>
       </c>
+      <c r="D25" s="3" t="s">
+        <v>171</v>
+      </c>
+      <c r="E25" s="3">
+        <v>2023</v>
+      </c>
     </row>
-    <row r="26" ht="15.5" spans="1:2">
+    <row r="26" ht="15.5" spans="1:5">
       <c r="A26" s="1" t="s">
         <v>120</v>
       </c>
       <c r="B26" s="1">
         <v>2015</v>
+      </c>
+      <c r="D26" s="3" t="s">
+        <v>177</v>
+      </c>
+      <c r="E26" s="3" t="s">
+        <v>180</v>
       </c>
     </row>
     <row r="27" ht="15.5" spans="1:2">

</xml_diff>

<commit_message>
Update Clean_Data & label
</commit_message>
<xml_diff>
--- a/Label.xlsx
+++ b/Label.xlsx
@@ -11,7 +11,7 @@
     <sheet name="Sheet1" sheetId="2" r:id="rId2"/>
   </sheets>
   <definedNames>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">Label!$A$1:$S$54</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">Label!$A$1:$S$56</definedName>
     <definedName name="_xlnm._FilterDatabase" localSheetId="1" hidden="1">Sheet1!$A$1:$A$68</definedName>
   </definedNames>
   <calcPr calcId="191029"/>
@@ -32,7 +32,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="554" uniqueCount="213">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="580" uniqueCount="218">
   <si>
     <t>Note</t>
   </si>
@@ -438,7 +438,22 @@
     <t>Pn13E4</t>
   </si>
   <si>
+    <t>Pn14E1</t>
+  </si>
+  <si>
     <t>Pn14</t>
+  </si>
+  <si>
+    <t>G Orellana-Corrales et al.</t>
+  </si>
+  <si>
+    <t>Experimental Psychology</t>
+  </si>
+  <si>
+    <t>Pn14E2</t>
+  </si>
+  <si>
+    <t>Pn14E3</t>
   </si>
   <si>
     <t>Pn16E1</t>
@@ -511,6 +526,9 @@
   </si>
   <si>
     <t>Citation()</t>
+  </si>
+  <si>
+    <t>unpublished</t>
   </si>
   <si>
     <t>Ps3E1</t>
@@ -681,9 +699,6 @@
   </si>
   <si>
     <t>Schäfer et al.</t>
-  </si>
-  <si>
-    <t>Experimental Psychology</t>
   </si>
   <si>
     <t>Pt6E1</t>
@@ -1865,14 +1880,14 @@
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:etc="http://www.wps.cn/officeDocument/2017/etCustomData">
   <sheetPr/>
-  <dimension ref="A1:KB70"/>
+  <dimension ref="A1:KB72"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane xSplit="3" ySplit="1" topLeftCell="D11" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="3" ySplit="1" topLeftCell="T2" activePane="bottomRight" state="frozen"/>
       <selection/>
       <selection pane="topRight"/>
       <selection pane="bottomLeft"/>
-      <selection pane="bottomRight" activeCell="C32" sqref="C32"/>
+      <selection pane="bottomRight" activeCell="Y29" sqref="Y29:Z29"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9" defaultRowHeight="14"/>
@@ -1881,7 +1896,7 @@
     <col min="2" max="2" width="3.625" customWidth="1"/>
     <col min="3" max="3" width="9.16666666666667" customWidth="1"/>
     <col min="4" max="4" width="6.08333333333333" customWidth="1"/>
-    <col min="5" max="5" width="19.75" customWidth="1"/>
+    <col min="5" max="5" width="23.4166666666667" customWidth="1"/>
     <col min="6" max="6" width="9" customWidth="1"/>
     <col min="7" max="7" width="67.0833333333333" customWidth="1"/>
     <col min="8" max="8" width="4.625" customWidth="1"/>
@@ -4685,7 +4700,7 @@
         <v>1</v>
       </c>
       <c r="P10" s="1">
-        <f t="shared" ref="P10:P19" si="1">M10-O10</f>
+        <f t="shared" ref="P10:P24" si="1">M10-O10</f>
         <v>55</v>
       </c>
       <c r="Q10" s="1"/>
@@ -8019,7 +8034,7 @@
       </c>
       <c r="O20" s="1"/>
       <c r="P20" s="1">
-        <f>M20-O20</f>
+        <f t="shared" si="1"/>
         <v>27</v>
       </c>
       <c r="Q20" s="1"/>
@@ -8350,7 +8365,7 @@
       </c>
       <c r="O21" s="1"/>
       <c r="P21" s="1">
-        <f>M21-O21</f>
+        <f t="shared" si="1"/>
         <v>26</v>
       </c>
       <c r="Q21" s="1"/>
@@ -8642,33 +8657,74 @@
     </row>
     <row r="22" ht="15.5" spans="1:288">
       <c r="A22" s="1"/>
-      <c r="B22" s="1"/>
+      <c r="B22" s="1">
+        <v>21</v>
+      </c>
       <c r="C22" s="1" t="s">
         <v>108</v>
       </c>
-      <c r="D22" s="1"/>
-      <c r="E22" s="1"/>
-      <c r="F22" s="1"/>
-      <c r="G22" s="1"/>
-      <c r="H22" s="1"/>
-      <c r="I22" s="1"/>
-      <c r="J22" s="1"/>
+      <c r="D22" s="1" t="s">
+        <v>109</v>
+      </c>
+      <c r="E22" s="1" t="s">
+        <v>110</v>
+      </c>
+      <c r="F22" s="1">
+        <v>2020</v>
+      </c>
+      <c r="G22" s="1" t="s">
+        <v>111</v>
+      </c>
+      <c r="H22" s="1">
+        <v>1</v>
+      </c>
+      <c r="I22" s="1">
+        <v>1</v>
+      </c>
+      <c r="J22" s="1" t="s">
+        <v>9</v>
+      </c>
       <c r="K22" s="1"/>
-      <c r="L22" s="1"/>
-      <c r="M22" s="1"/>
-      <c r="N22" s="1"/>
-      <c r="O22" s="1"/>
-      <c r="P22" s="1"/>
+      <c r="L22" s="1" t="s">
+        <v>45</v>
+      </c>
+      <c r="M22" s="1">
+        <v>38</v>
+      </c>
+      <c r="N22" s="1">
+        <v>128</v>
+      </c>
+      <c r="O22" s="1">
+        <v>4</v>
+      </c>
+      <c r="P22" s="1">
+        <f t="shared" si="1"/>
+        <v>34</v>
+      </c>
       <c r="Q22" s="1"/>
       <c r="R22" s="1"/>
       <c r="S22" s="1"/>
-      <c r="T22" s="7"/>
-      <c r="U22" s="8"/>
-      <c r="V22" s="8"/>
-      <c r="W22" s="1"/>
-      <c r="X22" s="1"/>
-      <c r="Y22" s="1"/>
-      <c r="Z22" s="1"/>
+      <c r="T22" s="7">
+        <v>1</v>
+      </c>
+      <c r="U22" s="8">
+        <v>0</v>
+      </c>
+      <c r="V22" s="8">
+        <v>0</v>
+      </c>
+      <c r="W22" s="1" t="s">
+        <v>66</v>
+      </c>
+      <c r="X22" s="1" t="s">
+        <v>87</v>
+      </c>
+      <c r="Y22" s="1">
+        <v>9</v>
+      </c>
+      <c r="Z22" s="1">
+        <v>29</v>
+      </c>
       <c r="AA22" s="1"/>
       <c r="AB22" s="1"/>
       <c r="AC22" s="1"/>
@@ -8935,46 +8991,48 @@
     <row r="23" ht="15.5" spans="1:288">
       <c r="A23" s="1"/>
       <c r="B23" s="1">
-        <v>21</v>
+        <v>22</v>
       </c>
       <c r="C23" s="1" t="s">
+        <v>112</v>
+      </c>
+      <c r="D23" s="1" t="s">
         <v>109</v>
       </c>
-      <c r="D23" s="1" t="s">
+      <c r="E23" s="1" t="s">
         <v>110</v>
       </c>
-      <c r="E23" s="1" t="s">
+      <c r="F23" s="1">
+        <v>2020</v>
+      </c>
+      <c r="G23" s="1" t="s">
         <v>111</v>
       </c>
-      <c r="F23" s="1">
-        <v>2022</v>
-      </c>
-      <c r="G23" s="1" t="s">
-        <v>112</v>
-      </c>
       <c r="H23" s="1">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="I23" s="1">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="J23" s="1" t="s">
         <v>9</v>
       </c>
-      <c r="K23" s="1" t="s">
-        <v>59</v>
-      </c>
-      <c r="L23" s="1"/>
+      <c r="K23" s="1"/>
+      <c r="L23" s="1" t="s">
+        <v>45</v>
+      </c>
       <c r="M23" s="1">
-        <v>20</v>
+        <v>33</v>
       </c>
       <c r="N23" s="1">
-        <v>200</v>
-      </c>
-      <c r="O23" s="1"/>
+        <v>128</v>
+      </c>
+      <c r="O23" s="1">
+        <v>2</v>
+      </c>
       <c r="P23" s="1">
-        <f t="shared" ref="P23:P46" si="2">M23-O23</f>
-        <v>20</v>
+        <f t="shared" si="1"/>
+        <v>31</v>
       </c>
       <c r="Q23" s="1"/>
       <c r="R23" s="1"/>
@@ -8988,13 +9046,17 @@
       <c r="V23" s="8">
         <v>0</v>
       </c>
-      <c r="W23" s="1"/>
-      <c r="X23" s="1"/>
+      <c r="W23" s="1" t="s">
+        <v>66</v>
+      </c>
+      <c r="X23" s="1" t="s">
+        <v>87</v>
+      </c>
       <c r="Y23" s="1">
-        <v>6</v>
+        <v>7</v>
       </c>
       <c r="Z23" s="1">
-        <v>14</v>
+        <v>26</v>
       </c>
       <c r="AA23" s="1"/>
       <c r="AB23" s="1"/>
@@ -9262,50 +9324,50 @@
     <row r="24" ht="15.5" spans="1:288">
       <c r="A24" s="1"/>
       <c r="B24" s="1">
-        <v>22</v>
+        <v>23</v>
       </c>
       <c r="C24" s="1" t="s">
         <v>113</v>
       </c>
       <c r="D24" s="1" t="s">
+        <v>109</v>
+      </c>
+      <c r="E24" s="1" t="s">
         <v>110</v>
       </c>
-      <c r="E24" s="1" t="s">
+      <c r="F24" s="1">
+        <v>2020</v>
+      </c>
+      <c r="G24" s="1" t="s">
         <v>111</v>
       </c>
-      <c r="F24" s="1">
-        <v>2022</v>
-      </c>
-      <c r="G24" s="1" t="s">
-        <v>112</v>
-      </c>
       <c r="H24" s="1">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="I24" s="1">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="J24" s="1" t="s">
         <v>9</v>
       </c>
-      <c r="K24" s="1" t="s">
-        <v>59</v>
-      </c>
-      <c r="L24" s="1"/>
+      <c r="K24" s="1"/>
+      <c r="L24" s="1" t="s">
+        <v>45</v>
+      </c>
       <c r="M24" s="1">
-        <v>24</v>
+        <v>36</v>
       </c>
       <c r="N24" s="1">
-        <v>200</v>
-      </c>
-      <c r="O24" s="1"/>
+        <v>128</v>
+      </c>
+      <c r="O24" s="1">
+        <v>1</v>
+      </c>
       <c r="P24" s="1">
-        <f t="shared" si="2"/>
-        <v>24</v>
-      </c>
-      <c r="Q24" s="1" t="s">
-        <v>114</v>
-      </c>
+        <f t="shared" si="1"/>
+        <v>35</v>
+      </c>
+      <c r="Q24" s="1"/>
       <c r="R24" s="1"/>
       <c r="S24" s="1"/>
       <c r="T24" s="7">
@@ -9317,13 +9379,17 @@
       <c r="V24" s="8">
         <v>0</v>
       </c>
-      <c r="W24" s="1"/>
-      <c r="X24" s="1"/>
+      <c r="W24" s="1" t="s">
+        <v>66</v>
+      </c>
+      <c r="X24" s="1" t="s">
+        <v>87</v>
+      </c>
       <c r="Y24" s="1">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="Z24" s="1">
-        <v>16</v>
+        <v>29</v>
       </c>
       <c r="AA24" s="1"/>
       <c r="AB24" s="1"/>
@@ -9591,28 +9657,28 @@
     <row r="25" ht="15.5" spans="1:288">
       <c r="A25" s="1"/>
       <c r="B25" s="1">
-        <v>23</v>
+        <v>24</v>
       </c>
       <c r="C25" s="1" t="s">
+        <v>114</v>
+      </c>
+      <c r="D25" s="1" t="s">
         <v>115</v>
       </c>
-      <c r="D25" s="1" t="s">
-        <v>110</v>
-      </c>
       <c r="E25" s="1" t="s">
-        <v>111</v>
+        <v>116</v>
       </c>
       <c r="F25" s="1">
         <v>2022</v>
       </c>
       <c r="G25" s="1" t="s">
-        <v>112</v>
+        <v>117</v>
       </c>
       <c r="H25" s="1">
-        <v>3</v>
+        <v>1</v>
       </c>
       <c r="I25" s="1">
-        <v>3</v>
+        <v>1</v>
       </c>
       <c r="J25" s="1" t="s">
         <v>9</v>
@@ -9622,19 +9688,17 @@
       </c>
       <c r="L25" s="1"/>
       <c r="M25" s="1">
-        <v>25</v>
+        <v>20</v>
       </c>
       <c r="N25" s="1">
-        <v>100</v>
+        <v>200</v>
       </c>
       <c r="O25" s="1"/>
       <c r="P25" s="1">
-        <f t="shared" si="2"/>
-        <v>25</v>
-      </c>
-      <c r="Q25" s="1" t="s">
-        <v>116</v>
-      </c>
+        <f t="shared" ref="P25:P48" si="2">M25-O25</f>
+        <v>20</v>
+      </c>
+      <c r="Q25" s="1"/>
       <c r="R25" s="1"/>
       <c r="S25" s="1"/>
       <c r="T25" s="7">
@@ -9649,10 +9713,10 @@
       <c r="W25" s="1"/>
       <c r="X25" s="1"/>
       <c r="Y25" s="1">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="Z25" s="1">
-        <v>18</v>
+        <v>14</v>
       </c>
       <c r="AA25" s="1"/>
       <c r="AB25" s="1"/>
@@ -9920,28 +9984,28 @@
     <row r="26" ht="15.5" spans="1:288">
       <c r="A26" s="1"/>
       <c r="B26" s="1">
-        <v>24</v>
+        <v>25</v>
       </c>
       <c r="C26" s="1" t="s">
+        <v>118</v>
+      </c>
+      <c r="D26" s="1" t="s">
+        <v>115</v>
+      </c>
+      <c r="E26" s="1" t="s">
+        <v>116</v>
+      </c>
+      <c r="F26" s="1">
+        <v>2022</v>
+      </c>
+      <c r="G26" s="1" t="s">
         <v>117</v>
       </c>
-      <c r="D26" s="1" t="s">
-        <v>118</v>
-      </c>
-      <c r="E26" s="1" t="s">
-        <v>119</v>
-      </c>
-      <c r="F26" s="1">
-        <v>2021</v>
-      </c>
-      <c r="G26" s="1" t="s">
-        <v>120</v>
-      </c>
       <c r="H26" s="1">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="I26" s="1">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="J26" s="1" t="s">
         <v>9</v>
@@ -9949,22 +10013,20 @@
       <c r="K26" s="1" t="s">
         <v>59</v>
       </c>
-      <c r="L26" s="1" t="s">
-        <v>45</v>
-      </c>
+      <c r="L26" s="1"/>
       <c r="M26" s="1">
-        <v>105</v>
+        <v>24</v>
       </c>
       <c r="N26" s="1">
-        <v>360</v>
+        <v>200</v>
       </c>
       <c r="O26" s="1"/>
       <c r="P26" s="1">
         <f t="shared" si="2"/>
-        <v>105</v>
-      </c>
-      <c r="Q26" s="10" t="s">
-        <v>121</v>
+        <v>24</v>
+      </c>
+      <c r="Q26" s="1" t="s">
+        <v>119</v>
       </c>
       <c r="R26" s="1"/>
       <c r="S26" s="1"/>
@@ -9977,17 +10039,13 @@
       <c r="V26" s="8">
         <v>0</v>
       </c>
-      <c r="W26" s="1" t="s">
-        <v>66</v>
-      </c>
-      <c r="X26" s="1" t="s">
-        <v>54</v>
-      </c>
+      <c r="W26" s="1"/>
+      <c r="X26" s="1"/>
       <c r="Y26" s="1">
-        <v>51</v>
+        <v>8</v>
       </c>
       <c r="Z26" s="1">
-        <v>54</v>
+        <v>16</v>
       </c>
       <c r="AA26" s="1"/>
       <c r="AB26" s="1"/>
@@ -10253,71 +10311,71 @@
       <c r="KB26" s="1"/>
     </row>
     <row r="27" ht="15.5" spans="1:288">
-      <c r="A27" s="1" t="s">
-        <v>88</v>
-      </c>
+      <c r="A27" s="1"/>
       <c r="B27" s="1">
-        <v>25</v>
+        <v>26</v>
       </c>
       <c r="C27" s="1" t="s">
-        <v>122</v>
+        <v>120</v>
       </c>
       <c r="D27" s="1" t="s">
-        <v>123</v>
+        <v>115</v>
       </c>
       <c r="E27" s="1" t="s">
-        <v>124</v>
+        <v>116</v>
       </c>
       <c r="F27" s="1">
-        <v>2023</v>
+        <v>2022</v>
       </c>
       <c r="G27" s="1" t="s">
-        <v>125</v>
+        <v>117</v>
       </c>
       <c r="H27" s="1">
-        <v>1</v>
+        <v>3</v>
       </c>
       <c r="I27" s="1">
-        <v>1</v>
+        <v>3</v>
       </c>
       <c r="J27" s="1" t="s">
         <v>9</v>
       </c>
-      <c r="K27" s="1"/>
-      <c r="L27" s="1" t="s">
-        <v>45</v>
-      </c>
+      <c r="K27" s="1" t="s">
+        <v>59</v>
+      </c>
+      <c r="L27" s="1"/>
       <c r="M27" s="1">
-        <v>302</v>
+        <v>25</v>
       </c>
       <c r="N27" s="1">
-        <v>16</v>
-      </c>
-      <c r="O27" s="1">
-        <v>3</v>
-      </c>
+        <v>100</v>
+      </c>
+      <c r="O27" s="1"/>
       <c r="P27" s="1">
         <f t="shared" si="2"/>
-        <v>299</v>
-      </c>
-      <c r="Q27" s="1"/>
+        <v>25</v>
+      </c>
+      <c r="Q27" s="1" t="s">
+        <v>121</v>
+      </c>
       <c r="R27" s="1"/>
       <c r="S27" s="1"/>
       <c r="T27" s="7">
         <v>1</v>
       </c>
-      <c r="U27" t="s">
-        <v>86</v>
+      <c r="U27" s="8">
+        <v>0</v>
       </c>
       <c r="V27" s="8">
         <v>0</v>
       </c>
-      <c r="W27" s="11" t="s">
-        <v>126</v>
-      </c>
+      <c r="W27" s="1"/>
       <c r="X27" s="1"/>
-      <c r="Y27" s="1"/>
-      <c r="Z27" s="1"/>
+      <c r="Y27" s="1">
+        <v>7</v>
+      </c>
+      <c r="Z27" s="1">
+        <v>18</v>
+      </c>
       <c r="AA27" s="1"/>
       <c r="AB27" s="1"/>
       <c r="AC27" s="1"/>
@@ -10582,71 +10640,77 @@
       <c r="KB27" s="1"/>
     </row>
     <row r="28" ht="15.5" spans="1:288">
-      <c r="A28" s="1" t="s">
-        <v>127</v>
-      </c>
+      <c r="A28" s="1"/>
       <c r="B28" s="1">
-        <v>26</v>
+        <v>27</v>
       </c>
       <c r="C28" s="1" t="s">
-        <v>128</v>
+        <v>122</v>
       </c>
       <c r="D28" s="1" t="s">
-        <v>129</v>
+        <v>123</v>
       </c>
       <c r="E28" s="1" t="s">
-        <v>50</v>
+        <v>124</v>
       </c>
       <c r="F28" s="1">
-        <v>2023</v>
-      </c>
-      <c r="G28" s="1"/>
+        <v>2021</v>
+      </c>
+      <c r="G28" s="1" t="s">
+        <v>125</v>
+      </c>
       <c r="H28" s="1">
         <v>1</v>
       </c>
-      <c r="I28" s="1" t="s">
-        <v>130</v>
+      <c r="I28" s="1">
+        <v>1</v>
       </c>
       <c r="J28" s="1" t="s">
         <v>9</v>
       </c>
-      <c r="K28" s="1"/>
+      <c r="K28" s="1" t="s">
+        <v>59</v>
+      </c>
       <c r="L28" s="1" t="s">
         <v>45</v>
       </c>
       <c r="M28" s="1">
-        <v>23</v>
+        <v>105</v>
       </c>
       <c r="N28" s="1">
-        <v>90</v>
-      </c>
-      <c r="O28" s="1">
-        <v>3</v>
-      </c>
+        <v>360</v>
+      </c>
+      <c r="O28" s="1"/>
       <c r="P28" s="1">
         <f t="shared" si="2"/>
-        <v>20</v>
-      </c>
-      <c r="Q28" s="1" t="s">
-        <v>131</v>
+        <v>105</v>
+      </c>
+      <c r="Q28" s="10" t="s">
+        <v>126</v>
       </c>
       <c r="R28" s="1"/>
-      <c r="S28" s="1" t="s">
-        <v>132</v>
-      </c>
+      <c r="S28" s="1"/>
       <c r="T28" s="7">
         <v>1</v>
       </c>
       <c r="U28" s="8">
         <v>0</v>
       </c>
-      <c r="V28" s="7">
-        <v>1</v>
-      </c>
-      <c r="W28" s="11"/>
-      <c r="X28" s="1"/>
-      <c r="Y28" s="1"/>
-      <c r="Z28" s="1"/>
+      <c r="V28" s="8">
+        <v>0</v>
+      </c>
+      <c r="W28" s="1" t="s">
+        <v>66</v>
+      </c>
+      <c r="X28" s="1" t="s">
+        <v>54</v>
+      </c>
+      <c r="Y28" s="1">
+        <v>51</v>
+      </c>
+      <c r="Z28" s="1">
+        <v>54</v>
+      </c>
       <c r="AA28" s="1"/>
       <c r="AB28" s="1"/>
       <c r="AC28" s="1"/>
@@ -10911,59 +10975,77 @@
       <c r="KB28" s="1"/>
     </row>
     <row r="29" ht="15.5" spans="1:288">
-      <c r="A29" s="1"/>
+      <c r="A29" s="1" t="s">
+        <v>88</v>
+      </c>
       <c r="B29" s="1">
-        <v>27</v>
+        <v>28</v>
       </c>
       <c r="C29" s="1" t="s">
-        <v>133</v>
+        <v>127</v>
       </c>
       <c r="D29" s="1" t="s">
-        <v>134</v>
+        <v>128</v>
       </c>
       <c r="E29" s="1" t="s">
-        <v>135</v>
+        <v>129</v>
       </c>
       <c r="F29" s="1">
-        <v>2014</v>
-      </c>
-      <c r="G29" s="1"/>
+        <v>2023</v>
+      </c>
+      <c r="G29" s="1" t="s">
+        <v>130</v>
+      </c>
       <c r="H29" s="1">
         <v>1</v>
       </c>
-      <c r="I29" s="1" t="s">
-        <v>136</v>
+      <c r="I29" s="1">
+        <v>1</v>
       </c>
       <c r="J29" s="1" t="s">
         <v>9</v>
       </c>
-      <c r="K29" s="1" t="s">
-        <v>59</v>
-      </c>
+      <c r="K29" s="1"/>
       <c r="L29" s="1" t="s">
         <v>45</v>
       </c>
       <c r="M29" s="1">
-        <v>24</v>
+        <v>302</v>
       </c>
       <c r="N29" s="1">
-        <v>40</v>
-      </c>
-      <c r="O29" s="1"/>
+        <v>16</v>
+      </c>
+      <c r="O29" s="1">
+        <v>3</v>
+      </c>
       <c r="P29" s="1">
         <f t="shared" si="2"/>
-        <v>24</v>
+        <v>299</v>
       </c>
       <c r="Q29" s="1"/>
       <c r="R29" s="1"/>
       <c r="S29" s="1"/>
-      <c r="T29" s="1"/>
-      <c r="U29" s="1"/>
-      <c r="V29" s="1"/>
-      <c r="W29" s="1"/>
+      <c r="T29" s="7">
+        <v>1</v>
+      </c>
+      <c r="U29" t="s">
+        <v>86</v>
+      </c>
+      <c r="V29" s="8">
+        <v>0</v>
+      </c>
+      <c r="W29" s="11" t="s">
+        <v>131</v>
+      </c>
       <c r="X29" s="1"/>
-      <c r="Y29" s="1"/>
-      <c r="Z29" s="1"/>
+      <c r="Y29" s="1">
+        <f>SUM(Y2:Y28)</f>
+        <v>321</v>
+      </c>
+      <c r="Z29" s="1">
+        <f>SUM(Z2:Z28)</f>
+        <v>676</v>
+      </c>
       <c r="AA29" s="1"/>
       <c r="AB29" s="1"/>
       <c r="AC29" s="1"/>
@@ -11228,56 +11310,68 @@
       <c r="KB29" s="1"/>
     </row>
     <row r="30" ht="15.5" spans="1:288">
-      <c r="A30" s="1"/>
+      <c r="A30" s="1" t="s">
+        <v>132</v>
+      </c>
       <c r="B30" s="1">
-        <v>28</v>
+        <v>29</v>
       </c>
       <c r="C30" s="1" t="s">
-        <v>137</v>
+        <v>133</v>
       </c>
       <c r="D30" s="1" t="s">
-        <v>138</v>
+        <v>134</v>
       </c>
       <c r="E30" s="1" t="s">
-        <v>135</v>
+        <v>50</v>
       </c>
       <c r="F30" s="1">
-        <v>2015</v>
+        <v>2023</v>
       </c>
       <c r="G30" s="1"/>
       <c r="H30" s="1">
         <v>1</v>
       </c>
       <c r="I30" s="1" t="s">
-        <v>136</v>
+        <v>135</v>
       </c>
       <c r="J30" s="1" t="s">
         <v>9</v>
       </c>
-      <c r="K30" s="1" t="s">
-        <v>59</v>
-      </c>
+      <c r="K30" s="1"/>
       <c r="L30" s="1" t="s">
         <v>45</v>
       </c>
       <c r="M30" s="1">
-        <v>20</v>
+        <v>23</v>
       </c>
       <c r="N30" s="1">
-        <v>40</v>
-      </c>
-      <c r="O30" s="1"/>
+        <v>90</v>
+      </c>
+      <c r="O30" s="1">
+        <v>3</v>
+      </c>
       <c r="P30" s="1">
         <f t="shared" si="2"/>
         <v>20</v>
       </c>
-      <c r="Q30" s="1"/>
+      <c r="Q30" s="1" t="s">
+        <v>136</v>
+      </c>
       <c r="R30" s="1"/>
-      <c r="S30" s="1"/>
-      <c r="T30" s="1"/>
-      <c r="U30" s="1"/>
-      <c r="V30" s="1"/>
-      <c r="W30" s="1"/>
+      <c r="S30" s="1" t="s">
+        <v>137</v>
+      </c>
+      <c r="T30" s="7">
+        <v>1</v>
+      </c>
+      <c r="U30" s="8">
+        <v>0</v>
+      </c>
+      <c r="V30" s="7">
+        <v>1</v>
+      </c>
+      <c r="W30" s="11"/>
       <c r="X30" s="1"/>
       <c r="Y30" s="1"/>
       <c r="Z30" s="1"/>
@@ -11545,28 +11639,30 @@
       <c r="KB30" s="1"/>
     </row>
     <row r="31" ht="15.5" spans="1:288">
-      <c r="A31" s="1"/>
+      <c r="A31" s="1" t="s">
+        <v>138</v>
+      </c>
       <c r="B31" s="1">
-        <v>29</v>
+        <v>30</v>
       </c>
       <c r="C31" s="1" t="s">
         <v>139</v>
       </c>
       <c r="D31" s="1" t="s">
-        <v>138</v>
+        <v>140</v>
       </c>
       <c r="E31" s="1" t="s">
-        <v>135</v>
+        <v>141</v>
       </c>
       <c r="F31" s="1">
-        <v>2015</v>
+        <v>2014</v>
       </c>
       <c r="G31" s="1"/>
       <c r="H31" s="1">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="I31" s="1" t="s">
-        <v>136</v>
+        <v>142</v>
       </c>
       <c r="J31" s="1" t="s">
         <v>9</v>
@@ -11578,7 +11674,7 @@
         <v>45</v>
       </c>
       <c r="M31" s="1">
-        <v>21</v>
+        <v>24</v>
       </c>
       <c r="N31" s="1">
         <v>40</v>
@@ -11586,7 +11682,7 @@
       <c r="O31" s="1"/>
       <c r="P31" s="1">
         <f t="shared" si="2"/>
-        <v>21</v>
+        <v>24</v>
       </c>
       <c r="Q31" s="1"/>
       <c r="R31" s="1"/>
@@ -11863,55 +11959,51 @@
     </row>
     <row r="32" ht="15.5" spans="1:288">
       <c r="A32" s="1" t="s">
-        <v>140</v>
+        <v>138</v>
       </c>
       <c r="B32" s="1">
-        <v>30</v>
+        <v>31</v>
       </c>
       <c r="C32" s="1" t="s">
+        <v>143</v>
+      </c>
+      <c r="D32" s="1" t="s">
+        <v>144</v>
+      </c>
+      <c r="E32" s="1" t="s">
         <v>141</v>
       </c>
-      <c r="D32" s="1" t="s">
-        <v>142</v>
-      </c>
-      <c r="E32" s="1" t="s">
-        <v>143</v>
-      </c>
       <c r="F32" s="1">
-        <v>2014</v>
-      </c>
-      <c r="G32" s="1" t="s">
-        <v>144</v>
-      </c>
+        <v>2015</v>
+      </c>
+      <c r="G32" s="1"/>
       <c r="H32" s="1">
         <v>1</v>
       </c>
-      <c r="I32" s="1">
-        <v>1</v>
+      <c r="I32" s="1" t="s">
+        <v>142</v>
       </c>
       <c r="J32" s="1" t="s">
         <v>9</v>
       </c>
       <c r="K32" s="1" t="s">
-        <v>145</v>
+        <v>59</v>
       </c>
       <c r="L32" s="1" t="s">
         <v>45</v>
       </c>
       <c r="M32" s="1">
-        <v>24</v>
+        <v>20</v>
       </c>
       <c r="N32" s="1">
-        <v>60</v>
+        <v>40</v>
       </c>
       <c r="O32" s="1"/>
       <c r="P32" s="1">
         <f t="shared" si="2"/>
-        <v>24</v>
-      </c>
-      <c r="Q32" s="1" t="s">
-        <v>146</v>
-      </c>
+        <v>20</v>
+      </c>
+      <c r="Q32" s="1"/>
       <c r="R32" s="1"/>
       <c r="S32" s="1"/>
       <c r="T32" s="1"/>
@@ -12186,55 +12278,51 @@
     </row>
     <row r="33" ht="15.5" spans="1:288">
       <c r="A33" s="1" t="s">
-        <v>147</v>
+        <v>138</v>
       </c>
       <c r="B33" s="1">
-        <v>31</v>
+        <v>32</v>
       </c>
       <c r="C33" s="1" t="s">
-        <v>148</v>
+        <v>145</v>
       </c>
       <c r="D33" s="1" t="s">
-        <v>142</v>
+        <v>144</v>
       </c>
       <c r="E33" s="1" t="s">
-        <v>143</v>
+        <v>141</v>
       </c>
       <c r="F33" s="1">
-        <v>2014</v>
-      </c>
-      <c r="G33" s="1" t="s">
-        <v>144</v>
-      </c>
+        <v>2015</v>
+      </c>
+      <c r="G33" s="1"/>
       <c r="H33" s="1">
         <v>2</v>
       </c>
-      <c r="I33" s="1">
-        <v>2</v>
+      <c r="I33" s="1" t="s">
+        <v>142</v>
       </c>
       <c r="J33" s="1" t="s">
         <v>9</v>
       </c>
       <c r="K33" s="1" t="s">
-        <v>145</v>
+        <v>59</v>
       </c>
       <c r="L33" s="1" t="s">
         <v>45</v>
       </c>
       <c r="M33" s="1">
-        <v>18</v>
+        <v>21</v>
       </c>
       <c r="N33" s="1">
-        <v>60</v>
+        <v>40</v>
       </c>
       <c r="O33" s="1"/>
       <c r="P33" s="1">
         <f t="shared" si="2"/>
-        <v>18</v>
-      </c>
-      <c r="Q33" s="1" t="s">
-        <v>149</v>
-      </c>
+        <v>21</v>
+      </c>
+      <c r="Q33" s="1"/>
       <c r="R33" s="1"/>
       <c r="S33" s="1"/>
       <c r="T33" s="1"/>
@@ -12509,43 +12597,43 @@
     </row>
     <row r="34" ht="15.5" spans="1:288">
       <c r="A34" s="1" t="s">
-        <v>150</v>
+        <v>146</v>
       </c>
       <c r="B34" s="1">
-        <v>32</v>
+        <v>33</v>
       </c>
       <c r="C34" s="1" t="s">
-        <v>151</v>
+        <v>147</v>
       </c>
       <c r="D34" s="1" t="s">
-        <v>142</v>
+        <v>148</v>
       </c>
       <c r="E34" s="1" t="s">
-        <v>143</v>
+        <v>149</v>
       </c>
       <c r="F34" s="1">
         <v>2014</v>
       </c>
       <c r="G34" s="1" t="s">
-        <v>144</v>
+        <v>150</v>
       </c>
       <c r="H34" s="1">
-        <v>3</v>
+        <v>1</v>
       </c>
       <c r="I34" s="1">
-        <v>3</v>
+        <v>1</v>
       </c>
       <c r="J34" s="1" t="s">
         <v>9</v>
       </c>
       <c r="K34" s="1" t="s">
-        <v>145</v>
+        <v>151</v>
       </c>
       <c r="L34" s="1" t="s">
         <v>45</v>
       </c>
       <c r="M34" s="1">
-        <v>22</v>
+        <v>24</v>
       </c>
       <c r="N34" s="1">
         <v>60</v>
@@ -12553,7 +12641,7 @@
       <c r="O34" s="1"/>
       <c r="P34" s="1">
         <f t="shared" si="2"/>
-        <v>22</v>
+        <v>24</v>
       </c>
       <c r="Q34" s="1" t="s">
         <v>152</v>
@@ -12835,40 +12923,40 @@
         <v>153</v>
       </c>
       <c r="B35" s="1">
-        <v>33</v>
+        <v>34</v>
       </c>
       <c r="C35" s="1" t="s">
         <v>154</v>
       </c>
       <c r="D35" s="1" t="s">
-        <v>142</v>
+        <v>148</v>
       </c>
       <c r="E35" s="1" t="s">
-        <v>143</v>
+        <v>149</v>
       </c>
       <c r="F35" s="1">
         <v>2014</v>
       </c>
       <c r="G35" s="1" t="s">
-        <v>144</v>
+        <v>150</v>
       </c>
       <c r="H35" s="1">
-        <v>4</v>
+        <v>2</v>
       </c>
       <c r="I35" s="1">
-        <v>4</v>
+        <v>2</v>
       </c>
       <c r="J35" s="1" t="s">
         <v>9</v>
       </c>
       <c r="K35" s="1" t="s">
-        <v>145</v>
+        <v>151</v>
       </c>
       <c r="L35" s="1" t="s">
         <v>45</v>
       </c>
       <c r="M35" s="1">
-        <v>20</v>
+        <v>18</v>
       </c>
       <c r="N35" s="1">
         <v>60</v>
@@ -12876,7 +12964,7 @@
       <c r="O35" s="1"/>
       <c r="P35" s="1">
         <f t="shared" si="2"/>
-        <v>20</v>
+        <v>18</v>
       </c>
       <c r="Q35" s="1" t="s">
         <v>155</v>
@@ -13154,40 +13242,44 @@
       <c r="KB35" s="1"/>
     </row>
     <row r="36" ht="15.5" spans="1:288">
-      <c r="A36" s="1"/>
+      <c r="A36" s="1" t="s">
+        <v>156</v>
+      </c>
       <c r="B36" s="1">
-        <v>34</v>
+        <v>35</v>
       </c>
       <c r="C36" s="1" t="s">
-        <v>156</v>
+        <v>157</v>
       </c>
       <c r="D36" s="1" t="s">
-        <v>157</v>
+        <v>148</v>
       </c>
       <c r="E36" s="1" t="s">
-        <v>158</v>
+        <v>149</v>
       </c>
       <c r="F36" s="1">
-        <v>2023</v>
+        <v>2014</v>
       </c>
       <c r="G36" s="1" t="s">
-        <v>159</v>
+        <v>150</v>
       </c>
       <c r="H36" s="1">
-        <v>1</v>
+        <v>3</v>
       </c>
       <c r="I36" s="1">
-        <v>1</v>
+        <v>3</v>
       </c>
       <c r="J36" s="1" t="s">
         <v>9</v>
       </c>
-      <c r="K36" s="1"/>
+      <c r="K36" s="1" t="s">
+        <v>151</v>
+      </c>
       <c r="L36" s="1" t="s">
         <v>45</v>
       </c>
       <c r="M36" s="1">
-        <v>40</v>
+        <v>22</v>
       </c>
       <c r="N36" s="1">
         <v>60</v>
@@ -13195,23 +13287,17 @@
       <c r="O36" s="1"/>
       <c r="P36" s="1">
         <f t="shared" si="2"/>
-        <v>40</v>
-      </c>
-      <c r="Q36" s="1"/>
+        <v>22</v>
+      </c>
+      <c r="Q36" s="1" t="s">
+        <v>158</v>
+      </c>
       <c r="R36" s="1"/>
       <c r="S36" s="1"/>
-      <c r="T36" s="1">
-        <v>1</v>
-      </c>
-      <c r="U36" s="1">
-        <v>0</v>
-      </c>
-      <c r="V36" s="1">
-        <v>1</v>
-      </c>
-      <c r="W36" s="1" t="s">
-        <v>66</v>
-      </c>
+      <c r="T36" s="1"/>
+      <c r="U36" s="1"/>
+      <c r="V36" s="1"/>
+      <c r="W36" s="1"/>
       <c r="X36" s="1"/>
       <c r="Y36" s="1"/>
       <c r="Z36" s="1"/>
@@ -13479,65 +13565,61 @@
       <c r="KB36" s="1"/>
     </row>
     <row r="37" ht="15.5" spans="1:288">
-      <c r="A37" s="1"/>
+      <c r="A37" s="1" t="s">
+        <v>159</v>
+      </c>
       <c r="B37" s="1">
-        <v>35</v>
+        <v>36</v>
       </c>
       <c r="C37" s="1" t="s">
         <v>160</v>
       </c>
       <c r="D37" s="1" t="s">
-        <v>161</v>
+        <v>148</v>
       </c>
       <c r="E37" s="1" t="s">
-        <v>162</v>
+        <v>149</v>
       </c>
       <c r="F37" s="1">
-        <v>2023</v>
+        <v>2014</v>
       </c>
       <c r="G37" s="1" t="s">
-        <v>163</v>
+        <v>150</v>
       </c>
       <c r="H37" s="1">
-        <v>1</v>
+        <v>4</v>
       </c>
       <c r="I37" s="1">
-        <v>1</v>
+        <v>4</v>
       </c>
       <c r="J37" s="1" t="s">
         <v>9</v>
       </c>
       <c r="K37" s="1" t="s">
-        <v>59</v>
+        <v>151</v>
       </c>
       <c r="L37" s="1" t="s">
         <v>45</v>
       </c>
       <c r="M37" s="1">
-        <v>144</v>
+        <v>20</v>
       </c>
       <c r="N37" s="1">
+        <v>60</v>
+      </c>
+      <c r="O37" s="1"/>
+      <c r="P37" s="1">
+        <f t="shared" si="2"/>
         <v>20</v>
       </c>
-      <c r="O37" s="1">
-        <v>2</v>
-      </c>
-      <c r="P37" s="1">
-        <f t="shared" ref="P37:P46" si="3">M37-O37</f>
-        <v>142</v>
-      </c>
-      <c r="Q37" s="1"/>
+      <c r="Q37" s="1" t="s">
+        <v>161</v>
+      </c>
       <c r="R37" s="1"/>
       <c r="S37" s="1"/>
-      <c r="T37" s="1">
-        <v>1</v>
-      </c>
-      <c r="U37" s="1">
-        <v>1</v>
-      </c>
-      <c r="V37" s="1">
-        <v>0</v>
-      </c>
+      <c r="T37" s="1"/>
+      <c r="U37" s="1"/>
+      <c r="V37" s="1"/>
       <c r="W37" s="1"/>
       <c r="X37" s="1"/>
       <c r="Y37" s="1"/>
@@ -13808,22 +13890,22 @@
     <row r="38" ht="15.5" spans="1:288">
       <c r="A38" s="1"/>
       <c r="B38" s="1">
-        <v>36</v>
+        <v>37</v>
       </c>
       <c r="C38" s="1" t="s">
+        <v>162</v>
+      </c>
+      <c r="D38" s="1" t="s">
+        <v>163</v>
+      </c>
+      <c r="E38" s="1" t="s">
         <v>164</v>
       </c>
-      <c r="D38" s="1" t="s">
+      <c r="F38" s="1">
+        <v>2023</v>
+      </c>
+      <c r="G38" s="1" t="s">
         <v>165</v>
-      </c>
-      <c r="E38" s="1" t="s">
-        <v>166</v>
-      </c>
-      <c r="F38" s="1">
-        <v>2021</v>
-      </c>
-      <c r="G38" s="1" t="s">
-        <v>58</v>
       </c>
       <c r="H38" s="1">
         <v>1</v>
@@ -13834,31 +13916,23 @@
       <c r="J38" s="1" t="s">
         <v>9</v>
       </c>
-      <c r="K38" s="1" t="s">
-        <v>59</v>
-      </c>
+      <c r="K38" s="1"/>
       <c r="L38" s="1" t="s">
         <v>45</v>
       </c>
       <c r="M38" s="1">
-        <v>109</v>
+        <v>40</v>
       </c>
       <c r="N38" s="1">
         <v>60</v>
       </c>
-      <c r="O38" s="1">
-        <v>1</v>
-      </c>
+      <c r="O38" s="1"/>
       <c r="P38" s="1">
-        <f t="shared" si="3"/>
-        <v>108</v>
-      </c>
-      <c r="Q38" s="1" t="s">
-        <v>167</v>
-      </c>
-      <c r="R38" s="1" t="s">
-        <v>168</v>
-      </c>
+        <f t="shared" si="2"/>
+        <v>40</v>
+      </c>
+      <c r="Q38" s="1"/>
+      <c r="R38" s="1"/>
       <c r="S38" s="1"/>
       <c r="T38" s="1">
         <v>1</v>
@@ -13867,7 +13941,7 @@
         <v>0</v>
       </c>
       <c r="V38" s="1">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="W38" s="1" t="s">
         <v>66</v>
@@ -14139,26 +14213,24 @@
       <c r="KB38" s="1"/>
     </row>
     <row r="39" ht="15.5" spans="1:288">
-      <c r="A39" s="1" t="s">
-        <v>169</v>
-      </c>
+      <c r="A39" s="1"/>
       <c r="B39" s="1">
-        <v>37</v>
+        <v>38</v>
       </c>
       <c r="C39" s="1" t="s">
-        <v>170</v>
+        <v>166</v>
       </c>
       <c r="D39" s="1" t="s">
-        <v>171</v>
+        <v>167</v>
       </c>
       <c r="E39" s="1" t="s">
-        <v>172</v>
+        <v>168</v>
       </c>
       <c r="F39" s="1">
         <v>2023</v>
       </c>
       <c r="G39" s="1" t="s">
-        <v>173</v>
+        <v>169</v>
       </c>
       <c r="H39" s="1">
         <v>1</v>
@@ -14170,21 +14242,23 @@
         <v>9</v>
       </c>
       <c r="K39" s="1" t="s">
-        <v>84</v>
-      </c>
-      <c r="L39" s="1"/>
+        <v>59</v>
+      </c>
+      <c r="L39" s="1" t="s">
+        <v>45</v>
+      </c>
       <c r="M39" s="1">
-        <v>40</v>
+        <v>144</v>
       </c>
       <c r="N39" s="1">
-        <v>100</v>
+        <v>20</v>
       </c>
       <c r="O39" s="1">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="P39" s="1">
-        <f t="shared" si="3"/>
-        <v>39</v>
+        <f t="shared" ref="P39:P48" si="3">M39-O39</f>
+        <v>142</v>
       </c>
       <c r="Q39" s="1"/>
       <c r="R39" s="1"/>
@@ -14193,14 +14267,12 @@
         <v>1</v>
       </c>
       <c r="U39" s="1">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="V39" s="1">
         <v>0</v>
       </c>
-      <c r="W39" s="1" t="s">
-        <v>66</v>
-      </c>
+      <c r="W39" s="1"/>
       <c r="X39" s="1"/>
       <c r="Y39" s="1"/>
       <c r="Z39" s="1"/>
@@ -14470,22 +14542,22 @@
     <row r="40" ht="15.5" spans="1:288">
       <c r="A40" s="1"/>
       <c r="B40" s="1">
-        <v>38</v>
+        <v>39</v>
       </c>
       <c r="C40" s="1" t="s">
-        <v>174</v>
+        <v>170</v>
       </c>
       <c r="D40" s="1" t="s">
-        <v>175</v>
+        <v>171</v>
       </c>
       <c r="E40" s="1" t="s">
-        <v>176</v>
+        <v>172</v>
       </c>
       <c r="F40" s="1">
-        <v>2022</v>
+        <v>2021</v>
       </c>
       <c r="G40" s="1" t="s">
-        <v>177</v>
+        <v>58</v>
       </c>
       <c r="H40" s="1">
         <v>1</v>
@@ -14496,32 +14568,44 @@
       <c r="J40" s="1" t="s">
         <v>9</v>
       </c>
-      <c r="K40" s="1"/>
+      <c r="K40" s="1" t="s">
+        <v>59</v>
+      </c>
       <c r="L40" s="1" t="s">
         <v>45</v>
       </c>
       <c r="M40" s="1">
-        <v>30</v>
+        <v>109</v>
       </c>
       <c r="N40" s="1">
         <v>60</v>
       </c>
       <c r="O40" s="1">
-        <v>3</v>
+        <v>1</v>
       </c>
       <c r="P40" s="1">
         <f t="shared" si="3"/>
-        <v>27</v>
+        <v>108</v>
       </c>
       <c r="Q40" s="1" t="s">
-        <v>178</v>
-      </c>
-      <c r="R40" s="1"/>
+        <v>173</v>
+      </c>
+      <c r="R40" s="1" t="s">
+        <v>174</v>
+      </c>
       <c r="S40" s="1"/>
-      <c r="T40" s="1"/>
-      <c r="U40" s="1"/>
-      <c r="V40" s="1"/>
-      <c r="W40" s="1"/>
+      <c r="T40" s="1">
+        <v>1</v>
+      </c>
+      <c r="U40" s="1">
+        <v>0</v>
+      </c>
+      <c r="V40" s="1">
+        <v>0</v>
+      </c>
+      <c r="W40" s="1" t="s">
+        <v>66</v>
+      </c>
       <c r="X40" s="1"/>
       <c r="Y40" s="1"/>
       <c r="Z40" s="1"/>
@@ -14789,60 +14873,68 @@
       <c r="KB40" s="1"/>
     </row>
     <row r="41" ht="15.5" spans="1:288">
-      <c r="A41" s="1"/>
+      <c r="A41" s="1" t="s">
+        <v>175</v>
+      </c>
       <c r="B41" s="1">
-        <v>39</v>
+        <v>40</v>
       </c>
       <c r="C41" s="1" t="s">
-        <v>179</v>
+        <v>176</v>
       </c>
       <c r="D41" s="1" t="s">
-        <v>175</v>
+        <v>177</v>
       </c>
       <c r="E41" s="1" t="s">
-        <v>176</v>
+        <v>178</v>
       </c>
       <c r="F41" s="1">
-        <v>2022</v>
+        <v>2023</v>
       </c>
       <c r="G41" s="1" t="s">
-        <v>177</v>
+        <v>111</v>
       </c>
       <c r="H41" s="1">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="I41" s="1">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="J41" s="1" t="s">
         <v>9</v>
       </c>
-      <c r="K41" s="1"/>
-      <c r="L41" s="1" t="s">
-        <v>45</v>
-      </c>
+      <c r="K41" s="1" t="s">
+        <v>84</v>
+      </c>
+      <c r="L41" s="1"/>
       <c r="M41" s="1">
-        <v>48</v>
+        <v>40</v>
       </c>
       <c r="N41" s="1">
-        <v>60</v>
+        <v>100</v>
       </c>
       <c r="O41" s="1">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="P41" s="1">
         <f t="shared" si="3"/>
-        <v>46</v>
-      </c>
-      <c r="Q41" s="1" t="s">
-        <v>178</v>
-      </c>
+        <v>39</v>
+      </c>
+      <c r="Q41" s="1"/>
       <c r="R41" s="1"/>
       <c r="S41" s="1"/>
-      <c r="T41" s="1"/>
-      <c r="U41" s="1"/>
-      <c r="V41" s="1"/>
-      <c r="W41" s="1"/>
+      <c r="T41" s="1">
+        <v>1</v>
+      </c>
+      <c r="U41" s="1">
+        <v>0</v>
+      </c>
+      <c r="V41" s="1">
+        <v>0</v>
+      </c>
+      <c r="W41" s="1" t="s">
+        <v>66</v>
+      </c>
       <c r="X41" s="1"/>
       <c r="Y41" s="1"/>
       <c r="Z41" s="1"/>
@@ -15110,26 +15202,24 @@
       <c r="KB41" s="1"/>
     </row>
     <row r="42" ht="15.5" spans="1:288">
-      <c r="A42" s="1" t="s">
+      <c r="A42" s="1"/>
+      <c r="B42" s="1">
+        <v>41</v>
+      </c>
+      <c r="C42" s="1" t="s">
+        <v>179</v>
+      </c>
+      <c r="D42" s="1" t="s">
         <v>180</v>
       </c>
-      <c r="B42" s="1">
-        <v>40</v>
-      </c>
-      <c r="C42" s="1" t="s">
+      <c r="E42" s="1" t="s">
         <v>181</v>
-      </c>
-      <c r="D42" s="1" t="s">
-        <v>182</v>
-      </c>
-      <c r="E42" s="1" t="s">
-        <v>183</v>
       </c>
       <c r="F42" s="1">
         <v>2022</v>
       </c>
       <c r="G42" s="1" t="s">
-        <v>184</v>
+        <v>182</v>
       </c>
       <c r="H42" s="1">
         <v>1</v>
@@ -15140,34 +15230,32 @@
       <c r="J42" s="1" t="s">
         <v>9</v>
       </c>
-      <c r="K42" s="1" t="s">
-        <v>59</v>
-      </c>
+      <c r="K42" s="1"/>
       <c r="L42" s="1" t="s">
         <v>45</v>
       </c>
       <c r="M42" s="1">
-        <v>328</v>
+        <v>30</v>
       </c>
       <c r="N42" s="1">
-        <v>120</v>
+        <v>60</v>
       </c>
       <c r="O42" s="1">
-        <v>40</v>
+        <v>3</v>
       </c>
       <c r="P42" s="1">
         <f t="shared" si="3"/>
-        <v>288</v>
-      </c>
-      <c r="Q42" s="1"/>
+        <v>27</v>
+      </c>
+      <c r="Q42" s="1" t="s">
+        <v>183</v>
+      </c>
       <c r="R42" s="1"/>
       <c r="S42" s="1"/>
       <c r="T42" s="1"/>
       <c r="U42" s="1"/>
       <c r="V42" s="1"/>
-      <c r="W42" s="1" t="s">
-        <v>53</v>
-      </c>
+      <c r="W42" s="1"/>
       <c r="X42" s="1"/>
       <c r="Y42" s="1"/>
       <c r="Z42" s="1"/>
@@ -15437,50 +15525,52 @@
     <row r="43" ht="15.5" spans="1:288">
       <c r="A43" s="1"/>
       <c r="B43" s="1">
-        <v>41</v>
+        <v>42</v>
       </c>
       <c r="C43" s="1" t="s">
-        <v>185</v>
+        <v>184</v>
       </c>
       <c r="D43" s="1" t="s">
-        <v>186</v>
+        <v>180</v>
       </c>
       <c r="E43" s="1" t="s">
-        <v>91</v>
+        <v>181</v>
       </c>
       <c r="F43" s="1">
-        <v>2020</v>
+        <v>2022</v>
       </c>
       <c r="G43" s="1" t="s">
-        <v>112</v>
+        <v>182</v>
       </c>
       <c r="H43" s="1">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="I43" s="1">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="J43" s="1" t="s">
         <v>9</v>
       </c>
-      <c r="K43" s="1" t="s">
-        <v>59</v>
-      </c>
+      <c r="K43" s="1"/>
       <c r="L43" s="1" t="s">
-        <v>85</v>
+        <v>45</v>
       </c>
       <c r="M43" s="1">
-        <v>23</v>
+        <v>48</v>
       </c>
       <c r="N43" s="1">
-        <v>120</v>
-      </c>
-      <c r="O43" s="1"/>
+        <v>60</v>
+      </c>
+      <c r="O43" s="1">
+        <v>2</v>
+      </c>
       <c r="P43" s="1">
         <f t="shared" si="3"/>
-        <v>23</v>
-      </c>
-      <c r="Q43" s="1"/>
+        <v>46</v>
+      </c>
+      <c r="Q43" s="1" t="s">
+        <v>183</v>
+      </c>
       <c r="R43" s="1"/>
       <c r="S43" s="1"/>
       <c r="T43" s="1"/>
@@ -15754,24 +15844,26 @@
       <c r="KB43" s="1"/>
     </row>
     <row r="44" ht="15.5" spans="1:288">
-      <c r="A44" s="1"/>
+      <c r="A44" s="1" t="s">
+        <v>185</v>
+      </c>
       <c r="B44" s="1">
-        <v>42</v>
+        <v>43</v>
       </c>
       <c r="C44" s="1" t="s">
+        <v>186</v>
+      </c>
+      <c r="D44" s="1" t="s">
         <v>187</v>
       </c>
-      <c r="D44" s="1" t="s">
-        <v>186</v>
-      </c>
       <c r="E44" s="1" t="s">
-        <v>91</v>
+        <v>188</v>
       </c>
       <c r="F44" s="1">
-        <v>2020</v>
+        <v>2022</v>
       </c>
       <c r="G44" s="1" t="s">
-        <v>112</v>
+        <v>189</v>
       </c>
       <c r="H44" s="1">
         <v>1</v>
@@ -15786,20 +15878,20 @@
         <v>59</v>
       </c>
       <c r="L44" s="1" t="s">
-        <v>85</v>
+        <v>45</v>
       </c>
       <c r="M44" s="1">
-        <v>21</v>
+        <v>328</v>
       </c>
       <c r="N44" s="1">
         <v>120</v>
       </c>
       <c r="O44" s="1">
-        <v>3</v>
+        <v>40</v>
       </c>
       <c r="P44" s="1">
         <f t="shared" si="3"/>
-        <v>18</v>
+        <v>288</v>
       </c>
       <c r="Q44" s="1"/>
       <c r="R44" s="1"/>
@@ -15807,7 +15899,9 @@
       <c r="T44" s="1"/>
       <c r="U44" s="1"/>
       <c r="V44" s="1"/>
-      <c r="W44" s="1"/>
+      <c r="W44" s="1" t="s">
+        <v>53</v>
+      </c>
       <c r="X44" s="1"/>
       <c r="Y44" s="1"/>
       <c r="Z44" s="1"/>
@@ -16077,13 +16171,13 @@
     <row r="45" ht="15.5" spans="1:288">
       <c r="A45" s="1"/>
       <c r="B45" s="1">
-        <v>43</v>
+        <v>44</v>
       </c>
       <c r="C45" s="1" t="s">
-        <v>188</v>
+        <v>190</v>
       </c>
       <c r="D45" s="1" t="s">
-        <v>186</v>
+        <v>191</v>
       </c>
       <c r="E45" s="1" t="s">
         <v>91</v>
@@ -16092,7 +16186,7 @@
         <v>2020</v>
       </c>
       <c r="G45" s="1" t="s">
-        <v>112</v>
+        <v>117</v>
       </c>
       <c r="H45" s="1">
         <v>1</v>
@@ -16110,7 +16204,7 @@
         <v>85</v>
       </c>
       <c r="M45" s="1">
-        <v>18</v>
+        <v>23</v>
       </c>
       <c r="N45" s="1">
         <v>120</v>
@@ -16118,7 +16212,7 @@
       <c r="O45" s="1"/>
       <c r="P45" s="1">
         <f t="shared" si="3"/>
-        <v>18</v>
+        <v>23</v>
       </c>
       <c r="Q45" s="1"/>
       <c r="R45" s="1"/>
@@ -16396,22 +16490,22 @@
     <row r="46" ht="15.5" spans="1:288">
       <c r="A46" s="1"/>
       <c r="B46" s="1">
-        <v>44</v>
+        <v>45</v>
       </c>
       <c r="C46" s="1" t="s">
-        <v>189</v>
+        <v>192</v>
       </c>
       <c r="D46" s="1" t="s">
-        <v>190</v>
+        <v>191</v>
       </c>
       <c r="E46" s="1" t="s">
-        <v>191</v>
+        <v>91</v>
       </c>
       <c r="F46" s="1">
-        <v>2023</v>
+        <v>2020</v>
       </c>
       <c r="G46" s="1" t="s">
-        <v>192</v>
+        <v>117</v>
       </c>
       <c r="H46" s="1">
         <v>1</v>
@@ -16419,19 +16513,27 @@
       <c r="I46" s="1">
         <v>1</v>
       </c>
-      <c r="J46" s="1"/>
-      <c r="K46" s="1"/>
-      <c r="L46" s="1"/>
+      <c r="J46" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="K46" s="1" t="s">
+        <v>59</v>
+      </c>
+      <c r="L46" s="1" t="s">
+        <v>85</v>
+      </c>
       <c r="M46" s="1">
-        <v>380</v>
-      </c>
-      <c r="N46" s="1"/>
+        <v>21</v>
+      </c>
+      <c r="N46" s="1">
+        <v>120</v>
+      </c>
       <c r="O46" s="1">
-        <v>32</v>
+        <v>3</v>
       </c>
       <c r="P46" s="1">
         <f t="shared" si="3"/>
-        <v>348</v>
+        <v>18</v>
       </c>
       <c r="Q46" s="1"/>
       <c r="R46" s="1"/>
@@ -16709,36 +16811,49 @@
     <row r="47" ht="15.5" spans="1:288">
       <c r="A47" s="1"/>
       <c r="B47" s="1">
-        <v>45</v>
+        <v>46</v>
       </c>
       <c r="C47" s="1" t="s">
         <v>193</v>
       </c>
       <c r="D47" s="1" t="s">
-        <v>190</v>
+        <v>191</v>
       </c>
       <c r="E47" s="1" t="s">
-        <v>191</v>
+        <v>91</v>
       </c>
       <c r="F47" s="1">
-        <v>2023</v>
+        <v>2020</v>
       </c>
       <c r="G47" s="1" t="s">
-        <v>192</v>
+        <v>117</v>
       </c>
       <c r="H47" s="1">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="I47" s="1">
-        <v>2</v>
-      </c>
-      <c r="J47" s="1"/>
-      <c r="K47" s="1"/>
-      <c r="L47" s="1"/>
-      <c r="M47" s="1"/>
-      <c r="N47" s="1"/>
+        <v>1</v>
+      </c>
+      <c r="J47" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="K47" s="1" t="s">
+        <v>59</v>
+      </c>
+      <c r="L47" s="1" t="s">
+        <v>85</v>
+      </c>
+      <c r="M47" s="1">
+        <v>18</v>
+      </c>
+      <c r="N47" s="1">
+        <v>120</v>
+      </c>
       <c r="O47" s="1"/>
-      <c r="P47" s="1"/>
+      <c r="P47" s="1">
+        <f t="shared" si="3"/>
+        <v>18</v>
+      </c>
       <c r="Q47" s="1"/>
       <c r="R47" s="1"/>
       <c r="S47" s="1"/>
@@ -17015,36 +17130,43 @@
     <row r="48" ht="15.5" spans="1:288">
       <c r="A48" s="1"/>
       <c r="B48" s="1">
-        <v>46</v>
+        <v>47</v>
       </c>
       <c r="C48" s="1" t="s">
         <v>194</v>
       </c>
       <c r="D48" s="1" t="s">
-        <v>190</v>
+        <v>195</v>
       </c>
       <c r="E48" s="1" t="s">
-        <v>191</v>
+        <v>196</v>
       </c>
       <c r="F48" s="1">
         <v>2023</v>
       </c>
       <c r="G48" s="1" t="s">
-        <v>192</v>
+        <v>197</v>
       </c>
       <c r="H48" s="1">
-        <v>3</v>
+        <v>1</v>
       </c>
       <c r="I48" s="1">
-        <v>3</v>
+        <v>1</v>
       </c>
       <c r="J48" s="1"/>
       <c r="K48" s="1"/>
       <c r="L48" s="1"/>
-      <c r="M48" s="1"/>
+      <c r="M48" s="1">
+        <v>380</v>
+      </c>
       <c r="N48" s="1"/>
-      <c r="O48" s="1"/>
-      <c r="P48" s="1"/>
+      <c r="O48" s="1">
+        <v>32</v>
+      </c>
+      <c r="P48" s="1">
+        <f t="shared" si="3"/>
+        <v>348</v>
+      </c>
       <c r="Q48" s="1"/>
       <c r="R48" s="1"/>
       <c r="S48" s="1"/>
@@ -17321,28 +17443,28 @@
     <row r="49" ht="15.5" spans="1:288">
       <c r="A49" s="1"/>
       <c r="B49" s="1">
-        <v>47</v>
+        <v>48</v>
       </c>
       <c r="C49" s="1" t="s">
+        <v>198</v>
+      </c>
+      <c r="D49" s="1" t="s">
         <v>195</v>
       </c>
-      <c r="D49" s="1" t="s">
+      <c r="E49" s="1" t="s">
         <v>196</v>
       </c>
-      <c r="E49" s="1" t="s">
+      <c r="F49" s="1">
+        <v>2023</v>
+      </c>
+      <c r="G49" s="1" t="s">
         <v>197</v>
       </c>
-      <c r="F49" s="1">
-        <v>2021</v>
-      </c>
-      <c r="G49" s="1" t="s">
-        <v>198</v>
-      </c>
       <c r="H49" s="1">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="I49" s="1">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="J49" s="1"/>
       <c r="K49" s="1"/>
@@ -17627,28 +17749,28 @@
     <row r="50" ht="15.5" spans="1:288">
       <c r="A50" s="1"/>
       <c r="B50" s="1">
-        <v>48</v>
+        <v>49</v>
       </c>
       <c r="C50" s="1" t="s">
         <v>199</v>
       </c>
       <c r="D50" s="1" t="s">
+        <v>195</v>
+      </c>
+      <c r="E50" s="1" t="s">
         <v>196</v>
       </c>
-      <c r="E50" s="1" t="s">
+      <c r="F50" s="1">
+        <v>2023</v>
+      </c>
+      <c r="G50" s="1" t="s">
         <v>197</v>
       </c>
-      <c r="F50" s="1">
-        <v>2021</v>
-      </c>
-      <c r="G50" s="1" t="s">
-        <v>198</v>
-      </c>
       <c r="H50" s="1">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="I50" s="1">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="J50" s="1"/>
       <c r="K50" s="1"/>
@@ -17933,28 +18055,28 @@
     <row r="51" ht="15.5" spans="1:288">
       <c r="A51" s="1"/>
       <c r="B51" s="1">
-        <v>49</v>
+        <v>50</v>
       </c>
       <c r="C51" s="1" t="s">
         <v>200</v>
       </c>
       <c r="D51" s="1" t="s">
-        <v>196</v>
+        <v>201</v>
       </c>
       <c r="E51" s="1" t="s">
-        <v>197</v>
+        <v>202</v>
       </c>
       <c r="F51" s="1">
         <v>2021</v>
       </c>
       <c r="G51" s="1" t="s">
-        <v>198</v>
+        <v>203</v>
       </c>
       <c r="H51" s="1">
-        <v>3</v>
+        <v>1</v>
       </c>
       <c r="I51" s="1">
-        <v>3</v>
+        <v>1</v>
       </c>
       <c r="J51" s="1"/>
       <c r="K51" s="1"/>
@@ -18239,28 +18361,28 @@
     <row r="52" ht="15.5" spans="1:288">
       <c r="A52" s="1"/>
       <c r="B52" s="1">
-        <v>50</v>
+        <v>51</v>
       </c>
       <c r="C52" s="1" t="s">
+        <v>204</v>
+      </c>
+      <c r="D52" s="1" t="s">
         <v>201</v>
       </c>
-      <c r="D52" s="1" t="s">
+      <c r="E52" s="1" t="s">
         <v>202</v>
       </c>
-      <c r="E52" s="1" t="s">
+      <c r="F52" s="1">
+        <v>2021</v>
+      </c>
+      <c r="G52" s="1" t="s">
         <v>203</v>
       </c>
-      <c r="F52" s="1">
-        <v>2023</v>
-      </c>
-      <c r="G52" s="1" t="s">
-        <v>204</v>
-      </c>
       <c r="H52" s="1">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="I52" s="1">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="J52" s="1"/>
       <c r="K52" s="1"/>
@@ -18545,28 +18667,28 @@
     <row r="53" ht="15.5" spans="1:288">
       <c r="A53" s="1"/>
       <c r="B53" s="1">
-        <v>51</v>
+        <v>52</v>
       </c>
       <c r="C53" s="1" t="s">
         <v>205</v>
       </c>
       <c r="D53" s="1" t="s">
-        <v>206</v>
+        <v>201</v>
       </c>
       <c r="E53" s="1" t="s">
-        <v>207</v>
+        <v>202</v>
       </c>
       <c r="F53" s="1">
-        <v>2024</v>
+        <v>2021</v>
       </c>
       <c r="G53" s="1" t="s">
-        <v>204</v>
+        <v>203</v>
       </c>
       <c r="H53" s="1">
-        <v>1</v>
+        <v>3</v>
       </c>
       <c r="I53" s="1">
-        <v>1</v>
+        <v>3</v>
       </c>
       <c r="J53" s="1"/>
       <c r="K53" s="1"/>
@@ -18851,22 +18973,22 @@
     <row r="54" ht="15.5" spans="1:288">
       <c r="A54" s="1"/>
       <c r="B54" s="1">
-        <v>52</v>
+        <v>53</v>
       </c>
       <c r="C54" s="1" t="s">
+        <v>206</v>
+      </c>
+      <c r="D54" s="1" t="s">
+        <v>207</v>
+      </c>
+      <c r="E54" s="1" t="s">
         <v>208</v>
       </c>
-      <c r="D54" s="1" t="s">
+      <c r="F54" s="1">
+        <v>2023</v>
+      </c>
+      <c r="G54" s="1" t="s">
         <v>209</v>
-      </c>
-      <c r="E54" s="1" t="s">
-        <v>210</v>
-      </c>
-      <c r="F54" s="1">
-        <v>2024</v>
-      </c>
-      <c r="G54" s="1" t="s">
-        <v>211</v>
       </c>
       <c r="H54" s="1">
         <v>1</v>
@@ -19156,14 +19278,30 @@
     </row>
     <row r="55" ht="15.5" spans="1:288">
       <c r="A55" s="1"/>
-      <c r="B55" s="1"/>
-      <c r="C55" s="1"/>
-      <c r="D55" s="1"/>
-      <c r="E55" s="1"/>
-      <c r="F55" s="1"/>
-      <c r="G55" s="1"/>
-      <c r="H55" s="1"/>
-      <c r="I55" s="1"/>
+      <c r="B55" s="1">
+        <v>54</v>
+      </c>
+      <c r="C55" s="1" t="s">
+        <v>210</v>
+      </c>
+      <c r="D55" s="1" t="s">
+        <v>211</v>
+      </c>
+      <c r="E55" s="1" t="s">
+        <v>212</v>
+      </c>
+      <c r="F55" s="1">
+        <v>2024</v>
+      </c>
+      <c r="G55" s="1" t="s">
+        <v>209</v>
+      </c>
+      <c r="H55" s="1">
+        <v>1</v>
+      </c>
+      <c r="I55" s="1">
+        <v>1</v>
+      </c>
       <c r="J55" s="1"/>
       <c r="K55" s="1"/>
       <c r="L55" s="1"/>
@@ -19446,14 +19584,30 @@
     </row>
     <row r="56" ht="15.5" spans="1:288">
       <c r="A56" s="1"/>
-      <c r="B56" s="1"/>
-      <c r="C56" s="1"/>
-      <c r="D56" s="1"/>
-      <c r="E56" s="1"/>
-      <c r="F56" s="1"/>
-      <c r="G56" s="1"/>
-      <c r="H56" s="1"/>
-      <c r="I56" s="1"/>
+      <c r="B56" s="1">
+        <v>55</v>
+      </c>
+      <c r="C56" s="1" t="s">
+        <v>213</v>
+      </c>
+      <c r="D56" s="1" t="s">
+        <v>214</v>
+      </c>
+      <c r="E56" s="1" t="s">
+        <v>215</v>
+      </c>
+      <c r="F56" s="1">
+        <v>2024</v>
+      </c>
+      <c r="G56" s="1" t="s">
+        <v>216</v>
+      </c>
+      <c r="H56" s="1">
+        <v>1</v>
+      </c>
+      <c r="I56" s="1">
+        <v>1</v>
+      </c>
       <c r="J56" s="1"/>
       <c r="K56" s="1"/>
       <c r="L56" s="1"/>
@@ -23504,7 +23658,7 @@
       <c r="KA69" s="1"/>
       <c r="KB69" s="1"/>
     </row>
-    <row r="70" ht="15.5" spans="1:12">
+    <row r="70" ht="15.5" spans="1:288">
       <c r="A70" s="1"/>
       <c r="B70" s="1"/>
       <c r="C70" s="1"/>
@@ -23517,9 +23671,589 @@
       <c r="J70" s="1"/>
       <c r="K70" s="1"/>
       <c r="L70" s="1"/>
+      <c r="M70" s="1"/>
+      <c r="N70" s="1"/>
+      <c r="O70" s="1"/>
+      <c r="P70" s="1"/>
+      <c r="Q70" s="1"/>
+      <c r="R70" s="1"/>
+      <c r="S70" s="1"/>
+      <c r="T70" s="1"/>
+      <c r="U70" s="1"/>
+      <c r="V70" s="1"/>
+      <c r="W70" s="1"/>
+      <c r="X70" s="1"/>
+      <c r="Y70" s="1"/>
+      <c r="Z70" s="1"/>
+      <c r="AA70" s="1"/>
+      <c r="AB70" s="1"/>
+      <c r="AC70" s="1"/>
+      <c r="AD70" s="1"/>
+      <c r="AE70" s="1"/>
+      <c r="AF70" s="1"/>
+      <c r="AG70" s="1"/>
+      <c r="AH70" s="1"/>
+      <c r="AI70" s="1"/>
+      <c r="AJ70" s="1"/>
+      <c r="AK70" s="1"/>
+      <c r="AL70" s="1"/>
+      <c r="AM70" s="1"/>
+      <c r="AN70" s="1"/>
+      <c r="AO70" s="1"/>
+      <c r="AP70" s="1"/>
+      <c r="AQ70" s="1"/>
+      <c r="AR70" s="1"/>
+      <c r="AS70" s="1"/>
+      <c r="AT70" s="1"/>
+      <c r="AU70" s="1"/>
+      <c r="AV70" s="1"/>
+      <c r="AW70" s="1"/>
+      <c r="AX70" s="1"/>
+      <c r="AY70" s="1"/>
+      <c r="AZ70" s="1"/>
+      <c r="BA70" s="1"/>
+      <c r="BB70" s="1"/>
+      <c r="BC70" s="1"/>
+      <c r="BD70" s="1"/>
+      <c r="BE70" s="1"/>
+      <c r="BF70" s="1"/>
+      <c r="BG70" s="1"/>
+      <c r="BH70" s="1"/>
+      <c r="BI70" s="1"/>
+      <c r="BJ70" s="1"/>
+      <c r="BK70" s="1"/>
+      <c r="BL70" s="1"/>
+      <c r="BM70" s="1"/>
+      <c r="BN70" s="1"/>
+      <c r="BO70" s="1"/>
+      <c r="BP70" s="1"/>
+      <c r="BQ70" s="1"/>
+      <c r="BR70" s="1"/>
+      <c r="BS70" s="1"/>
+      <c r="BT70" s="1"/>
+      <c r="BU70" s="1"/>
+      <c r="BV70" s="1"/>
+      <c r="BW70" s="1"/>
+      <c r="BX70" s="1"/>
+      <c r="BY70" s="1"/>
+      <c r="BZ70" s="1"/>
+      <c r="CA70" s="1"/>
+      <c r="CB70" s="1"/>
+      <c r="CC70" s="1"/>
+      <c r="CD70" s="1"/>
+      <c r="CE70" s="1"/>
+      <c r="CF70" s="1"/>
+      <c r="CG70" s="1"/>
+      <c r="CH70" s="1"/>
+      <c r="CI70" s="1"/>
+      <c r="CJ70" s="1"/>
+      <c r="CK70" s="1"/>
+      <c r="CL70" s="1"/>
+      <c r="CM70" s="1"/>
+      <c r="CN70" s="1"/>
+      <c r="CO70" s="1"/>
+      <c r="CP70" s="1"/>
+      <c r="CQ70" s="1"/>
+      <c r="CR70" s="1"/>
+      <c r="CS70" s="1"/>
+      <c r="CT70" s="1"/>
+      <c r="CU70" s="1"/>
+      <c r="CV70" s="1"/>
+      <c r="CW70" s="1"/>
+      <c r="CX70" s="1"/>
+      <c r="CY70" s="1"/>
+      <c r="CZ70" s="1"/>
+      <c r="DA70" s="1"/>
+      <c r="DB70" s="1"/>
+      <c r="DC70" s="1"/>
+      <c r="DD70" s="1"/>
+      <c r="DE70" s="1"/>
+      <c r="DF70" s="1"/>
+      <c r="DG70" s="1"/>
+      <c r="DH70" s="1"/>
+      <c r="DI70" s="1"/>
+      <c r="DJ70" s="1"/>
+      <c r="DK70" s="1"/>
+      <c r="DL70" s="1"/>
+      <c r="DM70" s="1"/>
+      <c r="DN70" s="1"/>
+      <c r="DO70" s="1"/>
+      <c r="DP70" s="1"/>
+      <c r="DQ70" s="1"/>
+      <c r="DR70" s="1"/>
+      <c r="DS70" s="1"/>
+      <c r="DT70" s="1"/>
+      <c r="DU70" s="1"/>
+      <c r="DV70" s="1"/>
+      <c r="DW70" s="1"/>
+      <c r="DX70" s="1"/>
+      <c r="DY70" s="1"/>
+      <c r="DZ70" s="1"/>
+      <c r="EA70" s="1"/>
+      <c r="EB70" s="1"/>
+      <c r="EC70" s="1"/>
+      <c r="ED70" s="1"/>
+      <c r="EE70" s="1"/>
+      <c r="EF70" s="1"/>
+      <c r="EG70" s="1"/>
+      <c r="EH70" s="1"/>
+      <c r="EI70" s="1"/>
+      <c r="EJ70" s="1"/>
+      <c r="EK70" s="1"/>
+      <c r="EL70" s="1"/>
+      <c r="EM70" s="1"/>
+      <c r="EN70" s="1"/>
+      <c r="EO70" s="1"/>
+      <c r="EP70" s="1"/>
+      <c r="EQ70" s="1"/>
+      <c r="ER70" s="1"/>
+      <c r="ES70" s="1"/>
+      <c r="ET70" s="1"/>
+      <c r="EU70" s="1"/>
+      <c r="EV70" s="1"/>
+      <c r="EW70" s="1"/>
+      <c r="EX70" s="1"/>
+      <c r="EY70" s="1"/>
+      <c r="EZ70" s="1"/>
+      <c r="FA70" s="1"/>
+      <c r="FB70" s="1"/>
+      <c r="FC70" s="1"/>
+      <c r="FD70" s="1"/>
+      <c r="FE70" s="1"/>
+      <c r="FF70" s="1"/>
+      <c r="FG70" s="1"/>
+      <c r="FH70" s="1"/>
+      <c r="FI70" s="1"/>
+      <c r="FJ70" s="1"/>
+      <c r="FK70" s="1"/>
+      <c r="FL70" s="1"/>
+      <c r="FM70" s="1"/>
+      <c r="FN70" s="1"/>
+      <c r="FO70" s="1"/>
+      <c r="FP70" s="1"/>
+      <c r="FQ70" s="1"/>
+      <c r="FR70" s="1"/>
+      <c r="FS70" s="1"/>
+      <c r="FT70" s="1"/>
+      <c r="FU70" s="1"/>
+      <c r="FV70" s="1"/>
+      <c r="FW70" s="1"/>
+      <c r="FX70" s="1"/>
+      <c r="FY70" s="1"/>
+      <c r="FZ70" s="1"/>
+      <c r="GA70" s="1"/>
+      <c r="GB70" s="1"/>
+      <c r="GC70" s="1"/>
+      <c r="GD70" s="1"/>
+      <c r="GE70" s="1"/>
+      <c r="GF70" s="1"/>
+      <c r="GG70" s="1"/>
+      <c r="GH70" s="1"/>
+      <c r="GI70" s="1"/>
+      <c r="GJ70" s="1"/>
+      <c r="GK70" s="1"/>
+      <c r="GL70" s="1"/>
+      <c r="GM70" s="1"/>
+      <c r="GN70" s="1"/>
+      <c r="GO70" s="1"/>
+      <c r="GP70" s="1"/>
+      <c r="GQ70" s="1"/>
+      <c r="GR70" s="1"/>
+      <c r="GS70" s="1"/>
+      <c r="GT70" s="1"/>
+      <c r="GU70" s="1"/>
+      <c r="GV70" s="1"/>
+      <c r="GW70" s="1"/>
+      <c r="GX70" s="1"/>
+      <c r="GY70" s="1"/>
+      <c r="GZ70" s="1"/>
+      <c r="HA70" s="1"/>
+      <c r="HB70" s="1"/>
+      <c r="HC70" s="1"/>
+      <c r="HD70" s="1"/>
+      <c r="HE70" s="1"/>
+      <c r="HF70" s="1"/>
+      <c r="HG70" s="1"/>
+      <c r="HH70" s="1"/>
+      <c r="HI70" s="1"/>
+      <c r="HJ70" s="1"/>
+      <c r="HK70" s="1"/>
+      <c r="HL70" s="1"/>
+      <c r="HM70" s="1"/>
+      <c r="HN70" s="1"/>
+      <c r="HO70" s="1"/>
+      <c r="HP70" s="1"/>
+      <c r="HQ70" s="1"/>
+      <c r="HR70" s="1"/>
+      <c r="HS70" s="1"/>
+      <c r="HT70" s="1"/>
+      <c r="HU70" s="1"/>
+      <c r="HV70" s="1"/>
+      <c r="HW70" s="1"/>
+      <c r="HX70" s="1"/>
+      <c r="HY70" s="1"/>
+      <c r="HZ70" s="1"/>
+      <c r="IA70" s="1"/>
+      <c r="IB70" s="1"/>
+      <c r="IC70" s="1"/>
+      <c r="ID70" s="1"/>
+      <c r="IE70" s="1"/>
+      <c r="IF70" s="1"/>
+      <c r="IG70" s="1"/>
+      <c r="IH70" s="1"/>
+      <c r="II70" s="1"/>
+      <c r="IJ70" s="1"/>
+      <c r="IK70" s="1"/>
+      <c r="IL70" s="1"/>
+      <c r="IM70" s="1"/>
+      <c r="IN70" s="1"/>
+      <c r="IO70" s="1"/>
+      <c r="IP70" s="1"/>
+      <c r="IQ70" s="1"/>
+      <c r="IR70" s="1"/>
+      <c r="IS70" s="1"/>
+      <c r="IT70" s="1"/>
+      <c r="IU70" s="1"/>
+      <c r="IV70" s="1"/>
+      <c r="IW70" s="1"/>
+      <c r="IX70" s="1"/>
+      <c r="IY70" s="1"/>
+      <c r="IZ70" s="1"/>
+      <c r="JA70" s="1"/>
+      <c r="JB70" s="1"/>
+      <c r="JC70" s="1"/>
+      <c r="JD70" s="1"/>
+      <c r="JE70" s="1"/>
+      <c r="JF70" s="1"/>
+      <c r="JG70" s="1"/>
+      <c r="JH70" s="1"/>
+      <c r="JI70" s="1"/>
+      <c r="JJ70" s="1"/>
+      <c r="JK70" s="1"/>
+      <c r="JL70" s="1"/>
+      <c r="JM70" s="1"/>
+      <c r="JN70" s="1"/>
+      <c r="JO70" s="1"/>
+      <c r="JP70" s="1"/>
+      <c r="JQ70" s="1"/>
+      <c r="JR70" s="1"/>
+      <c r="JS70" s="1"/>
+      <c r="JT70" s="1"/>
+      <c r="JU70" s="1"/>
+      <c r="JV70" s="1"/>
+      <c r="JW70" s="1"/>
+      <c r="JX70" s="1"/>
+      <c r="JY70" s="1"/>
+      <c r="JZ70" s="1"/>
+      <c r="KA70" s="1"/>
+      <c r="KB70" s="1"/>
+    </row>
+    <row r="71" ht="15.5" spans="1:288">
+      <c r="A71" s="1"/>
+      <c r="B71" s="1"/>
+      <c r="C71" s="1"/>
+      <c r="D71" s="1"/>
+      <c r="E71" s="1"/>
+      <c r="F71" s="1"/>
+      <c r="G71" s="1"/>
+      <c r="H71" s="1"/>
+      <c r="I71" s="1"/>
+      <c r="J71" s="1"/>
+      <c r="K71" s="1"/>
+      <c r="L71" s="1"/>
+      <c r="M71" s="1"/>
+      <c r="N71" s="1"/>
+      <c r="O71" s="1"/>
+      <c r="P71" s="1"/>
+      <c r="Q71" s="1"/>
+      <c r="R71" s="1"/>
+      <c r="S71" s="1"/>
+      <c r="T71" s="1"/>
+      <c r="U71" s="1"/>
+      <c r="V71" s="1"/>
+      <c r="W71" s="1"/>
+      <c r="X71" s="1"/>
+      <c r="Y71" s="1"/>
+      <c r="Z71" s="1"/>
+      <c r="AA71" s="1"/>
+      <c r="AB71" s="1"/>
+      <c r="AC71" s="1"/>
+      <c r="AD71" s="1"/>
+      <c r="AE71" s="1"/>
+      <c r="AF71" s="1"/>
+      <c r="AG71" s="1"/>
+      <c r="AH71" s="1"/>
+      <c r="AI71" s="1"/>
+      <c r="AJ71" s="1"/>
+      <c r="AK71" s="1"/>
+      <c r="AL71" s="1"/>
+      <c r="AM71" s="1"/>
+      <c r="AN71" s="1"/>
+      <c r="AO71" s="1"/>
+      <c r="AP71" s="1"/>
+      <c r="AQ71" s="1"/>
+      <c r="AR71" s="1"/>
+      <c r="AS71" s="1"/>
+      <c r="AT71" s="1"/>
+      <c r="AU71" s="1"/>
+      <c r="AV71" s="1"/>
+      <c r="AW71" s="1"/>
+      <c r="AX71" s="1"/>
+      <c r="AY71" s="1"/>
+      <c r="AZ71" s="1"/>
+      <c r="BA71" s="1"/>
+      <c r="BB71" s="1"/>
+      <c r="BC71" s="1"/>
+      <c r="BD71" s="1"/>
+      <c r="BE71" s="1"/>
+      <c r="BF71" s="1"/>
+      <c r="BG71" s="1"/>
+      <c r="BH71" s="1"/>
+      <c r="BI71" s="1"/>
+      <c r="BJ71" s="1"/>
+      <c r="BK71" s="1"/>
+      <c r="BL71" s="1"/>
+      <c r="BM71" s="1"/>
+      <c r="BN71" s="1"/>
+      <c r="BO71" s="1"/>
+      <c r="BP71" s="1"/>
+      <c r="BQ71" s="1"/>
+      <c r="BR71" s="1"/>
+      <c r="BS71" s="1"/>
+      <c r="BT71" s="1"/>
+      <c r="BU71" s="1"/>
+      <c r="BV71" s="1"/>
+      <c r="BW71" s="1"/>
+      <c r="BX71" s="1"/>
+      <c r="BY71" s="1"/>
+      <c r="BZ71" s="1"/>
+      <c r="CA71" s="1"/>
+      <c r="CB71" s="1"/>
+      <c r="CC71" s="1"/>
+      <c r="CD71" s="1"/>
+      <c r="CE71" s="1"/>
+      <c r="CF71" s="1"/>
+      <c r="CG71" s="1"/>
+      <c r="CH71" s="1"/>
+      <c r="CI71" s="1"/>
+      <c r="CJ71" s="1"/>
+      <c r="CK71" s="1"/>
+      <c r="CL71" s="1"/>
+      <c r="CM71" s="1"/>
+      <c r="CN71" s="1"/>
+      <c r="CO71" s="1"/>
+      <c r="CP71" s="1"/>
+      <c r="CQ71" s="1"/>
+      <c r="CR71" s="1"/>
+      <c r="CS71" s="1"/>
+      <c r="CT71" s="1"/>
+      <c r="CU71" s="1"/>
+      <c r="CV71" s="1"/>
+      <c r="CW71" s="1"/>
+      <c r="CX71" s="1"/>
+      <c r="CY71" s="1"/>
+      <c r="CZ71" s="1"/>
+      <c r="DA71" s="1"/>
+      <c r="DB71" s="1"/>
+      <c r="DC71" s="1"/>
+      <c r="DD71" s="1"/>
+      <c r="DE71" s="1"/>
+      <c r="DF71" s="1"/>
+      <c r="DG71" s="1"/>
+      <c r="DH71" s="1"/>
+      <c r="DI71" s="1"/>
+      <c r="DJ71" s="1"/>
+      <c r="DK71" s="1"/>
+      <c r="DL71" s="1"/>
+      <c r="DM71" s="1"/>
+      <c r="DN71" s="1"/>
+      <c r="DO71" s="1"/>
+      <c r="DP71" s="1"/>
+      <c r="DQ71" s="1"/>
+      <c r="DR71" s="1"/>
+      <c r="DS71" s="1"/>
+      <c r="DT71" s="1"/>
+      <c r="DU71" s="1"/>
+      <c r="DV71" s="1"/>
+      <c r="DW71" s="1"/>
+      <c r="DX71" s="1"/>
+      <c r="DY71" s="1"/>
+      <c r="DZ71" s="1"/>
+      <c r="EA71" s="1"/>
+      <c r="EB71" s="1"/>
+      <c r="EC71" s="1"/>
+      <c r="ED71" s="1"/>
+      <c r="EE71" s="1"/>
+      <c r="EF71" s="1"/>
+      <c r="EG71" s="1"/>
+      <c r="EH71" s="1"/>
+      <c r="EI71" s="1"/>
+      <c r="EJ71" s="1"/>
+      <c r="EK71" s="1"/>
+      <c r="EL71" s="1"/>
+      <c r="EM71" s="1"/>
+      <c r="EN71" s="1"/>
+      <c r="EO71" s="1"/>
+      <c r="EP71" s="1"/>
+      <c r="EQ71" s="1"/>
+      <c r="ER71" s="1"/>
+      <c r="ES71" s="1"/>
+      <c r="ET71" s="1"/>
+      <c r="EU71" s="1"/>
+      <c r="EV71" s="1"/>
+      <c r="EW71" s="1"/>
+      <c r="EX71" s="1"/>
+      <c r="EY71" s="1"/>
+      <c r="EZ71" s="1"/>
+      <c r="FA71" s="1"/>
+      <c r="FB71" s="1"/>
+      <c r="FC71" s="1"/>
+      <c r="FD71" s="1"/>
+      <c r="FE71" s="1"/>
+      <c r="FF71" s="1"/>
+      <c r="FG71" s="1"/>
+      <c r="FH71" s="1"/>
+      <c r="FI71" s="1"/>
+      <c r="FJ71" s="1"/>
+      <c r="FK71" s="1"/>
+      <c r="FL71" s="1"/>
+      <c r="FM71" s="1"/>
+      <c r="FN71" s="1"/>
+      <c r="FO71" s="1"/>
+      <c r="FP71" s="1"/>
+      <c r="FQ71" s="1"/>
+      <c r="FR71" s="1"/>
+      <c r="FS71" s="1"/>
+      <c r="FT71" s="1"/>
+      <c r="FU71" s="1"/>
+      <c r="FV71" s="1"/>
+      <c r="FW71" s="1"/>
+      <c r="FX71" s="1"/>
+      <c r="FY71" s="1"/>
+      <c r="FZ71" s="1"/>
+      <c r="GA71" s="1"/>
+      <c r="GB71" s="1"/>
+      <c r="GC71" s="1"/>
+      <c r="GD71" s="1"/>
+      <c r="GE71" s="1"/>
+      <c r="GF71" s="1"/>
+      <c r="GG71" s="1"/>
+      <c r="GH71" s="1"/>
+      <c r="GI71" s="1"/>
+      <c r="GJ71" s="1"/>
+      <c r="GK71" s="1"/>
+      <c r="GL71" s="1"/>
+      <c r="GM71" s="1"/>
+      <c r="GN71" s="1"/>
+      <c r="GO71" s="1"/>
+      <c r="GP71" s="1"/>
+      <c r="GQ71" s="1"/>
+      <c r="GR71" s="1"/>
+      <c r="GS71" s="1"/>
+      <c r="GT71" s="1"/>
+      <c r="GU71" s="1"/>
+      <c r="GV71" s="1"/>
+      <c r="GW71" s="1"/>
+      <c r="GX71" s="1"/>
+      <c r="GY71" s="1"/>
+      <c r="GZ71" s="1"/>
+      <c r="HA71" s="1"/>
+      <c r="HB71" s="1"/>
+      <c r="HC71" s="1"/>
+      <c r="HD71" s="1"/>
+      <c r="HE71" s="1"/>
+      <c r="HF71" s="1"/>
+      <c r="HG71" s="1"/>
+      <c r="HH71" s="1"/>
+      <c r="HI71" s="1"/>
+      <c r="HJ71" s="1"/>
+      <c r="HK71" s="1"/>
+      <c r="HL71" s="1"/>
+      <c r="HM71" s="1"/>
+      <c r="HN71" s="1"/>
+      <c r="HO71" s="1"/>
+      <c r="HP71" s="1"/>
+      <c r="HQ71" s="1"/>
+      <c r="HR71" s="1"/>
+      <c r="HS71" s="1"/>
+      <c r="HT71" s="1"/>
+      <c r="HU71" s="1"/>
+      <c r="HV71" s="1"/>
+      <c r="HW71" s="1"/>
+      <c r="HX71" s="1"/>
+      <c r="HY71" s="1"/>
+      <c r="HZ71" s="1"/>
+      <c r="IA71" s="1"/>
+      <c r="IB71" s="1"/>
+      <c r="IC71" s="1"/>
+      <c r="ID71" s="1"/>
+      <c r="IE71" s="1"/>
+      <c r="IF71" s="1"/>
+      <c r="IG71" s="1"/>
+      <c r="IH71" s="1"/>
+      <c r="II71" s="1"/>
+      <c r="IJ71" s="1"/>
+      <c r="IK71" s="1"/>
+      <c r="IL71" s="1"/>
+      <c r="IM71" s="1"/>
+      <c r="IN71" s="1"/>
+      <c r="IO71" s="1"/>
+      <c r="IP71" s="1"/>
+      <c r="IQ71" s="1"/>
+      <c r="IR71" s="1"/>
+      <c r="IS71" s="1"/>
+      <c r="IT71" s="1"/>
+      <c r="IU71" s="1"/>
+      <c r="IV71" s="1"/>
+      <c r="IW71" s="1"/>
+      <c r="IX71" s="1"/>
+      <c r="IY71" s="1"/>
+      <c r="IZ71" s="1"/>
+      <c r="JA71" s="1"/>
+      <c r="JB71" s="1"/>
+      <c r="JC71" s="1"/>
+      <c r="JD71" s="1"/>
+      <c r="JE71" s="1"/>
+      <c r="JF71" s="1"/>
+      <c r="JG71" s="1"/>
+      <c r="JH71" s="1"/>
+      <c r="JI71" s="1"/>
+      <c r="JJ71" s="1"/>
+      <c r="JK71" s="1"/>
+      <c r="JL71" s="1"/>
+      <c r="JM71" s="1"/>
+      <c r="JN71" s="1"/>
+      <c r="JO71" s="1"/>
+      <c r="JP71" s="1"/>
+      <c r="JQ71" s="1"/>
+      <c r="JR71" s="1"/>
+      <c r="JS71" s="1"/>
+      <c r="JT71" s="1"/>
+      <c r="JU71" s="1"/>
+      <c r="JV71" s="1"/>
+      <c r="JW71" s="1"/>
+      <c r="JX71" s="1"/>
+      <c r="JY71" s="1"/>
+      <c r="JZ71" s="1"/>
+      <c r="KA71" s="1"/>
+      <c r="KB71" s="1"/>
+    </row>
+    <row r="72" ht="15.5" spans="1:12">
+      <c r="A72" s="1"/>
+      <c r="B72" s="1"/>
+      <c r="C72" s="1"/>
+      <c r="D72" s="1"/>
+      <c r="E72" s="1"/>
+      <c r="F72" s="1"/>
+      <c r="G72" s="1"/>
+      <c r="H72" s="1"/>
+      <c r="I72" s="1"/>
+      <c r="J72" s="1"/>
+      <c r="K72" s="1"/>
+      <c r="L72" s="1"/>
     </row>
   </sheetData>
-  <autoFilter xmlns:etc="http://www.wps.cn/officeDocument/2017/etCustomData" ref="A1:S54" etc:filterBottomFollowUsedRange="0">
+  <autoFilter xmlns:etc="http://www.wps.cn/officeDocument/2017/etCustomData" ref="A1:S56" etc:filterBottomFollowUsedRange="0">
     <extLst>
       <etc:autoFilterAnalysis etc:version="v1" etc:showPane="0">
         <etc:analysisCharts>
@@ -23534,7 +24268,7 @@
     </extLst>
   </autoFilter>
   <hyperlinks>
-    <hyperlink ref="G54" r:id="rId1" display="Cognitive, Affective, &amp; Behavioral Neuroscience" tooltip="https://link.springer.com/journal/13415"/>
+    <hyperlink ref="G56" r:id="rId1" display="Cognitive, Affective, &amp; Behavioral Neuroscience" tooltip="https://link.springer.com/journal/13415"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait"/>
@@ -23767,7 +24501,7 @@
         <v>2020</v>
       </c>
       <c r="D11" s="3" t="s">
-        <v>110</v>
+        <v>115</v>
       </c>
       <c r="E11" s="3">
         <v>2022</v>
@@ -23787,7 +24521,7 @@
         <v>2020</v>
       </c>
       <c r="D12" s="3" t="s">
-        <v>118</v>
+        <v>123</v>
       </c>
       <c r="E12" s="3">
         <v>2021</v>
@@ -23807,7 +24541,7 @@
         <v>2019</v>
       </c>
       <c r="D13" s="3" t="s">
-        <v>123</v>
+        <v>128</v>
       </c>
       <c r="E13" s="3">
         <v>2023</v>
@@ -23827,7 +24561,7 @@
         <v>2019</v>
       </c>
       <c r="D14" s="3" t="s">
-        <v>129</v>
+        <v>134</v>
       </c>
       <c r="E14" s="3">
         <v>2023</v>
@@ -23847,7 +24581,7 @@
         <v>2018</v>
       </c>
       <c r="D15" s="3" t="s">
-        <v>134</v>
+        <v>140</v>
       </c>
       <c r="E15" s="3">
         <v>2014</v>
@@ -23867,7 +24601,7 @@
         <v>2018</v>
       </c>
       <c r="D16" s="3" t="s">
-        <v>138</v>
+        <v>144</v>
       </c>
       <c r="E16" s="3">
         <v>2015</v>
@@ -23887,7 +24621,7 @@
         <v>2021</v>
       </c>
       <c r="D17" s="3" t="s">
-        <v>142</v>
+        <v>148</v>
       </c>
       <c r="E17" s="3">
         <v>2014</v>
@@ -23907,7 +24641,7 @@
         <v>2021</v>
       </c>
       <c r="D18" s="3" t="s">
-        <v>157</v>
+        <v>163</v>
       </c>
       <c r="E18" s="3">
         <v>2023</v>
@@ -23927,7 +24661,7 @@
         <v>2021</v>
       </c>
       <c r="D19" s="3" t="s">
-        <v>161</v>
+        <v>167</v>
       </c>
       <c r="E19" s="3">
         <v>2023</v>
@@ -23947,7 +24681,7 @@
         <v>2021</v>
       </c>
       <c r="D20" s="3" t="s">
-        <v>165</v>
+        <v>171</v>
       </c>
       <c r="E20" s="3">
         <v>2021</v>
@@ -23961,19 +24695,19 @@
     </row>
     <row r="21" ht="15.5" spans="1:8">
       <c r="A21" s="1" t="s">
-        <v>110</v>
+        <v>115</v>
       </c>
       <c r="B21" s="1">
         <v>2022</v>
       </c>
       <c r="D21" s="3" t="s">
-        <v>171</v>
+        <v>177</v>
       </c>
       <c r="E21" s="3">
         <v>2023</v>
       </c>
       <c r="G21" s="1" t="s">
-        <v>110</v>
+        <v>115</v>
       </c>
       <c r="H21" s="1">
         <v>2022</v>
@@ -23981,19 +24715,19 @@
     </row>
     <row r="22" ht="15.5" spans="1:8">
       <c r="A22" s="1" t="s">
-        <v>110</v>
+        <v>115</v>
       </c>
       <c r="B22" s="1">
         <v>2022</v>
       </c>
       <c r="D22" s="3" t="s">
-        <v>175</v>
+        <v>180</v>
       </c>
       <c r="E22" s="3">
         <v>2022</v>
       </c>
       <c r="G22" s="1" t="s">
-        <v>110</v>
+        <v>115</v>
       </c>
       <c r="H22" s="1">
         <v>2022</v>
@@ -24001,19 +24735,19 @@
     </row>
     <row r="23" ht="15.5" spans="1:8">
       <c r="A23" s="1" t="s">
-        <v>110</v>
+        <v>115</v>
       </c>
       <c r="B23" s="1">
         <v>2022</v>
       </c>
       <c r="D23" s="3" t="s">
-        <v>182</v>
+        <v>187</v>
       </c>
       <c r="E23" s="3">
         <v>2022</v>
       </c>
       <c r="G23" s="1" t="s">
-        <v>110</v>
+        <v>115</v>
       </c>
       <c r="H23" s="1">
         <v>2022</v>
@@ -24021,19 +24755,19 @@
     </row>
     <row r="24" ht="15.5" hidden="1" spans="1:8">
       <c r="A24" s="1" t="s">
-        <v>118</v>
+        <v>123</v>
       </c>
       <c r="B24" s="1">
         <v>2021</v>
       </c>
       <c r="D24" s="3" t="s">
-        <v>186</v>
+        <v>191</v>
       </c>
       <c r="E24" s="3">
         <v>2020</v>
       </c>
       <c r="G24" s="1" t="s">
-        <v>118</v>
+        <v>123</v>
       </c>
       <c r="H24" s="1">
         <v>2021</v>
@@ -24041,19 +24775,19 @@
     </row>
     <row r="25" ht="15.5" hidden="1" spans="1:8">
       <c r="A25" s="1" t="s">
-        <v>123</v>
+        <v>128</v>
       </c>
       <c r="B25" s="1">
         <v>2023</v>
       </c>
       <c r="D25" s="3" t="s">
-        <v>190</v>
+        <v>195</v>
       </c>
       <c r="E25" s="3">
         <v>2023</v>
       </c>
       <c r="G25" s="1" t="s">
-        <v>123</v>
+        <v>128</v>
       </c>
       <c r="H25" s="1">
         <v>2023</v>
@@ -24061,19 +24795,19 @@
     </row>
     <row r="26" ht="15.5" hidden="1" spans="1:8">
       <c r="A26" s="1" t="s">
-        <v>129</v>
+        <v>134</v>
       </c>
       <c r="B26" s="1">
         <v>2023</v>
       </c>
       <c r="D26" s="3" t="s">
-        <v>196</v>
+        <v>201</v>
       </c>
       <c r="E26" s="3" t="s">
-        <v>212</v>
+        <v>217</v>
       </c>
       <c r="G26" s="1" t="s">
-        <v>129</v>
+        <v>134</v>
       </c>
       <c r="H26" s="1">
         <v>2023</v>
@@ -24081,13 +24815,13 @@
     </row>
     <row r="27" ht="15.5" hidden="1" spans="1:8">
       <c r="A27" s="1" t="s">
-        <v>134</v>
+        <v>140</v>
       </c>
       <c r="B27" s="1">
         <v>2014</v>
       </c>
       <c r="G27" s="1" t="s">
-        <v>134</v>
+        <v>140</v>
       </c>
       <c r="H27" s="1">
         <v>2014</v>
@@ -24095,13 +24829,13 @@
     </row>
     <row r="28" ht="15.5" spans="1:8">
       <c r="A28" s="1" t="s">
-        <v>138</v>
+        <v>144</v>
       </c>
       <c r="B28" s="1">
         <v>2015</v>
       </c>
       <c r="G28" s="1" t="s">
-        <v>138</v>
+        <v>144</v>
       </c>
       <c r="H28" s="1">
         <v>2015</v>
@@ -24109,13 +24843,13 @@
     </row>
     <row r="29" ht="15.5" spans="1:8">
       <c r="A29" s="1" t="s">
-        <v>138</v>
+        <v>144</v>
       </c>
       <c r="B29" s="1">
         <v>2015</v>
       </c>
       <c r="G29" s="1" t="s">
-        <v>138</v>
+        <v>144</v>
       </c>
       <c r="H29" s="1">
         <v>2015</v>
@@ -24123,13 +24857,13 @@
     </row>
     <row r="30" ht="15.5" spans="1:8">
       <c r="A30" s="1" t="s">
-        <v>142</v>
+        <v>148</v>
       </c>
       <c r="B30" s="1">
         <v>2014</v>
       </c>
       <c r="G30" s="1" t="s">
-        <v>142</v>
+        <v>148</v>
       </c>
       <c r="H30" s="1">
         <v>2014</v>
@@ -24137,13 +24871,13 @@
     </row>
     <row r="31" ht="15.5" spans="1:8">
       <c r="A31" s="1" t="s">
-        <v>142</v>
+        <v>148</v>
       </c>
       <c r="B31" s="1">
         <v>2014</v>
       </c>
       <c r="G31" s="1" t="s">
-        <v>142</v>
+        <v>148</v>
       </c>
       <c r="H31" s="1">
         <v>2014</v>
@@ -24151,13 +24885,13 @@
     </row>
     <row r="32" ht="15.5" spans="1:8">
       <c r="A32" s="1" t="s">
-        <v>142</v>
+        <v>148</v>
       </c>
       <c r="B32" s="1">
         <v>2014</v>
       </c>
       <c r="G32" s="1" t="s">
-        <v>142</v>
+        <v>148</v>
       </c>
       <c r="H32" s="1">
         <v>2014</v>
@@ -24165,13 +24899,13 @@
     </row>
     <row r="33" ht="15.5" spans="1:8">
       <c r="A33" s="1" t="s">
-        <v>142</v>
+        <v>148</v>
       </c>
       <c r="B33" s="1">
         <v>2014</v>
       </c>
       <c r="G33" s="1" t="s">
-        <v>142</v>
+        <v>148</v>
       </c>
       <c r="H33" s="1">
         <v>2014</v>
@@ -24179,13 +24913,13 @@
     </row>
     <row r="34" ht="15.5" hidden="1" spans="1:8">
       <c r="A34" s="1" t="s">
-        <v>157</v>
+        <v>163</v>
       </c>
       <c r="B34" s="1">
         <v>2023</v>
       </c>
       <c r="G34" s="1" t="s">
-        <v>157</v>
+        <v>163</v>
       </c>
       <c r="H34" s="1">
         <v>2023</v>
@@ -24193,13 +24927,13 @@
     </row>
     <row r="35" ht="15.5" hidden="1" spans="1:8">
       <c r="A35" s="1" t="s">
-        <v>161</v>
+        <v>167</v>
       </c>
       <c r="B35" s="1">
         <v>2023</v>
       </c>
       <c r="G35" s="1" t="s">
-        <v>161</v>
+        <v>167</v>
       </c>
       <c r="H35" s="1">
         <v>2023</v>
@@ -24207,13 +24941,13 @@
     </row>
     <row r="36" ht="15.5" hidden="1" spans="1:8">
       <c r="A36" s="1" t="s">
-        <v>165</v>
+        <v>171</v>
       </c>
       <c r="B36" s="1">
         <v>2021</v>
       </c>
       <c r="G36" s="1" t="s">
-        <v>165</v>
+        <v>171</v>
       </c>
       <c r="H36" s="1">
         <v>2021</v>
@@ -24221,13 +24955,13 @@
     </row>
     <row r="37" ht="15.5" hidden="1" spans="1:8">
       <c r="A37" s="1" t="s">
-        <v>171</v>
+        <v>177</v>
       </c>
       <c r="B37" s="1">
         <v>2023</v>
       </c>
       <c r="G37" s="1" t="s">
-        <v>171</v>
+        <v>177</v>
       </c>
       <c r="H37" s="1">
         <v>2023</v>
@@ -24235,13 +24969,13 @@
     </row>
     <row r="38" ht="15.5" spans="1:8">
       <c r="A38" s="1" t="s">
-        <v>175</v>
+        <v>180</v>
       </c>
       <c r="B38" s="1">
         <v>2022</v>
       </c>
       <c r="G38" s="1" t="s">
-        <v>175</v>
+        <v>180</v>
       </c>
       <c r="H38" s="1">
         <v>2022</v>
@@ -24249,13 +24983,13 @@
     </row>
     <row r="39" ht="15.5" spans="1:8">
       <c r="A39" s="1" t="s">
-        <v>175</v>
+        <v>180</v>
       </c>
       <c r="B39" s="1">
         <v>2022</v>
       </c>
       <c r="G39" s="1" t="s">
-        <v>175</v>
+        <v>180</v>
       </c>
       <c r="H39" s="1">
         <v>2022</v>
@@ -24263,13 +24997,13 @@
     </row>
     <row r="40" ht="15.5" hidden="1" spans="1:8">
       <c r="A40" s="1" t="s">
-        <v>182</v>
+        <v>187</v>
       </c>
       <c r="B40" s="1">
         <v>2022</v>
       </c>
       <c r="G40" s="1" t="s">
-        <v>182</v>
+        <v>187</v>
       </c>
       <c r="H40" s="1">
         <v>2022</v>
@@ -24277,13 +25011,13 @@
     </row>
     <row r="41" ht="15.5" spans="1:8">
       <c r="A41" s="1" t="s">
-        <v>186</v>
+        <v>191</v>
       </c>
       <c r="B41" s="1">
         <v>2020</v>
       </c>
       <c r="G41" s="1" t="s">
-        <v>186</v>
+        <v>191</v>
       </c>
       <c r="H41" s="1">
         <v>2020</v>
@@ -24291,13 +25025,13 @@
     </row>
     <row r="42" ht="15.5" spans="1:8">
       <c r="A42" s="1" t="s">
-        <v>186</v>
+        <v>191</v>
       </c>
       <c r="B42" s="1">
         <v>2020</v>
       </c>
       <c r="G42" s="1" t="s">
-        <v>186</v>
+        <v>191</v>
       </c>
       <c r="H42" s="1">
         <v>2020</v>
@@ -24305,13 +25039,13 @@
     </row>
     <row r="43" ht="15.5" spans="1:8">
       <c r="A43" s="1" t="s">
-        <v>186</v>
+        <v>191</v>
       </c>
       <c r="B43" s="1">
         <v>2020</v>
       </c>
       <c r="G43" s="1" t="s">
-        <v>186</v>
+        <v>191</v>
       </c>
       <c r="H43" s="1">
         <v>2020</v>
@@ -24319,13 +25053,13 @@
     </row>
     <row r="44" ht="15.5" spans="1:8">
       <c r="A44" s="1" t="s">
-        <v>190</v>
+        <v>195</v>
       </c>
       <c r="B44" s="1">
         <v>2023</v>
       </c>
       <c r="G44" s="1" t="s">
-        <v>190</v>
+        <v>195</v>
       </c>
       <c r="H44" s="1">
         <v>2023</v>
@@ -24333,13 +25067,13 @@
     </row>
     <row r="45" ht="15.5" spans="1:8">
       <c r="A45" s="1" t="s">
-        <v>190</v>
+        <v>195</v>
       </c>
       <c r="B45" s="1">
         <v>2023</v>
       </c>
       <c r="G45" s="1" t="s">
-        <v>190</v>
+        <v>195</v>
       </c>
       <c r="H45" s="1">
         <v>2023</v>
@@ -24347,13 +25081,13 @@
     </row>
     <row r="46" ht="15.5" spans="1:8">
       <c r="A46" s="1" t="s">
-        <v>190</v>
+        <v>195</v>
       </c>
       <c r="B46" s="1">
         <v>2023</v>
       </c>
       <c r="G46" s="1" t="s">
-        <v>190</v>
+        <v>195</v>
       </c>
       <c r="H46" s="1">
         <v>2023</v>
@@ -24361,13 +25095,13 @@
     </row>
     <row r="47" ht="15.5" spans="1:8">
       <c r="A47" s="1" t="s">
-        <v>196</v>
+        <v>201</v>
       </c>
       <c r="B47" s="1">
         <v>2021</v>
       </c>
       <c r="G47" s="1" t="s">
-        <v>196</v>
+        <v>201</v>
       </c>
       <c r="H47" s="1">
         <v>2021</v>
@@ -24375,13 +25109,13 @@
     </row>
     <row r="48" ht="15.5" spans="1:8">
       <c r="A48" s="1" t="s">
-        <v>196</v>
+        <v>201</v>
       </c>
       <c r="B48" s="1">
         <v>2021</v>
       </c>
       <c r="G48" s="1" t="s">
-        <v>196</v>
+        <v>201</v>
       </c>
       <c r="H48" s="1">
         <v>2021</v>
@@ -24389,13 +25123,13 @@
     </row>
     <row r="49" ht="15.5" spans="1:8">
       <c r="A49" s="1" t="s">
-        <v>196</v>
+        <v>201</v>
       </c>
       <c r="B49" s="1">
         <v>2021</v>
       </c>
       <c r="G49" s="1" t="s">
-        <v>196</v>
+        <v>201</v>
       </c>
       <c r="H49" s="1">
         <v>2021</v>
@@ -24403,13 +25137,13 @@
     </row>
     <row r="50" ht="15.5" hidden="1" spans="1:8">
       <c r="A50" s="1" t="s">
-        <v>202</v>
+        <v>207</v>
       </c>
       <c r="B50" s="1">
         <v>2023</v>
       </c>
       <c r="G50" s="1" t="s">
-        <v>202</v>
+        <v>207</v>
       </c>
       <c r="H50" s="1">
         <v>2023</v>
@@ -24417,13 +25151,13 @@
     </row>
     <row r="51" ht="15.5" hidden="1" spans="1:8">
       <c r="A51" s="1" t="s">
-        <v>206</v>
+        <v>211</v>
       </c>
       <c r="B51" s="1">
         <v>2024</v>
       </c>
       <c r="G51" s="1" t="s">
-        <v>206</v>
+        <v>211</v>
       </c>
       <c r="H51" s="1">
         <v>2024</v>
@@ -24431,13 +25165,13 @@
     </row>
     <row r="52" ht="15.5" hidden="1" spans="1:8">
       <c r="A52" s="1" t="s">
-        <v>209</v>
+        <v>214</v>
       </c>
       <c r="B52" s="1">
         <v>2024</v>
       </c>
       <c r="G52" s="1" t="s">
-        <v>209</v>
+        <v>214</v>
       </c>
       <c r="H52" s="1">
         <v>2024</v>

</xml_diff>

<commit_message>
Update Clean_Data and Process_Data
</commit_message>
<xml_diff>
--- a/Label.xlsx
+++ b/Label.xlsx
@@ -32,7 +32,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="581" uniqueCount="219">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="587" uniqueCount="220">
   <si>
     <t>Note</t>
   </si>
@@ -110,6 +110,9 @@
   </si>
   <si>
     <t>Female</t>
+  </si>
+  <si>
+    <t>No Gender Data</t>
   </si>
   <si>
     <t>Pair Number</t>
@@ -366,9 +369,6 @@
     <t>Facial Gender: (Male, Female)</t>
   </si>
   <si>
-    <t>No Gender Data</t>
-  </si>
-  <si>
     <t>P95E2</t>
   </si>
   <si>
@@ -412,6 +412,9 @@
       </rPr>
       <t>, Blocked)</t>
     </r>
+  </si>
+  <si>
+    <t>Pn4E2</t>
   </si>
   <si>
     <t>Pn13E1</t>
@@ -1886,11 +1889,11 @@
   <dimension ref="A1:KB72"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane xSplit="3" ySplit="1" topLeftCell="D2" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="3" ySplit="1" topLeftCell="U8" activePane="bottomRight" state="frozen"/>
       <selection/>
       <selection pane="topRight"/>
       <selection pane="bottomLeft"/>
-      <selection pane="bottomRight" activeCell="U29" sqref="U29"/>
+      <selection pane="bottomRight" activeCell="AE20" sqref="AE20"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9" defaultRowHeight="14"/>
@@ -1918,9 +1921,10 @@
     <col min="22" max="22" width="8.66666666666667" customWidth="1"/>
     <col min="23" max="23" width="23.8333333333333" style="4" customWidth="1"/>
     <col min="24" max="24" width="14.5" customWidth="1"/>
+    <col min="27" max="27" width="15.1666666666667" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" ht="15.5" spans="1:26">
+    <row r="1" ht="15.5" spans="1:27">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -1998,29 +2002,32 @@
       </c>
       <c r="Z1" t="s">
         <v>25</v>
+      </c>
+      <c r="AA1" t="s">
+        <v>26</v>
       </c>
     </row>
     <row r="2" ht="15.5" spans="1:288">
       <c r="A2" s="1" t="s">
-        <v>26</v>
+        <v>27</v>
       </c>
       <c r="B2" s="1">
         <v>1</v>
       </c>
       <c r="C2" s="1" t="s">
-        <v>27</v>
+        <v>28</v>
       </c>
       <c r="D2" s="1" t="s">
-        <v>28</v>
+        <v>29</v>
       </c>
       <c r="E2" s="1" t="s">
-        <v>29</v>
+        <v>30</v>
       </c>
       <c r="F2" s="1">
         <v>2019</v>
       </c>
       <c r="G2" s="1" t="s">
-        <v>30</v>
+        <v>31</v>
       </c>
       <c r="H2" s="1">
         <v>1</v>
@@ -2032,10 +2039,10 @@
         <v>9</v>
       </c>
       <c r="K2" s="1" t="s">
-        <v>31</v>
+        <v>32</v>
       </c>
       <c r="L2" s="1" t="s">
-        <v>32</v>
+        <v>33</v>
       </c>
       <c r="M2" s="1">
         <v>28</v>
@@ -2045,7 +2052,7 @@
       </c>
       <c r="O2" s="1"/>
       <c r="P2" s="1">
-        <f t="shared" ref="P2:P7" si="0">M2-O2</f>
+        <f t="shared" ref="P2:P9" si="0">M2-O2</f>
         <v>28</v>
       </c>
       <c r="Q2" s="1"/>
@@ -2062,7 +2069,7 @@
       </c>
       <c r="W2" s="1"/>
       <c r="X2" s="1" t="s">
-        <v>33</v>
+        <v>34</v>
       </c>
       <c r="Y2" s="1">
         <v>12</v>
@@ -2335,25 +2342,25 @@
     </row>
     <row r="3" ht="15.5" spans="1:288">
       <c r="A3" s="1" t="s">
-        <v>26</v>
+        <v>27</v>
       </c>
       <c r="B3" s="1">
         <v>2</v>
       </c>
       <c r="C3" s="1" t="s">
-        <v>34</v>
+        <v>35</v>
       </c>
       <c r="D3" s="1" t="s">
-        <v>28</v>
+        <v>29</v>
       </c>
       <c r="E3" s="1" t="s">
-        <v>29</v>
+        <v>30</v>
       </c>
       <c r="F3" s="1">
         <v>2019</v>
       </c>
       <c r="G3" s="1" t="s">
-        <v>30</v>
+        <v>31</v>
       </c>
       <c r="H3" s="1">
         <v>2</v>
@@ -2365,10 +2372,10 @@
         <v>9</v>
       </c>
       <c r="K3" s="1" t="s">
-        <v>31</v>
+        <v>32</v>
       </c>
       <c r="L3" s="1" t="s">
-        <v>32</v>
+        <v>33</v>
       </c>
       <c r="M3" s="1">
         <v>28</v>
@@ -2395,7 +2402,7 @@
       </c>
       <c r="W3" s="1"/>
       <c r="X3" s="1" t="s">
-        <v>33</v>
+        <v>34</v>
       </c>
       <c r="Y3" s="1">
         <v>6</v>
@@ -2668,25 +2675,25 @@
     </row>
     <row r="4" ht="15.5" spans="1:288">
       <c r="A4" s="1" t="s">
-        <v>26</v>
+        <v>27</v>
       </c>
       <c r="B4" s="1">
         <v>3</v>
       </c>
       <c r="C4" s="1" t="s">
-        <v>35</v>
+        <v>36</v>
       </c>
       <c r="D4" s="1" t="s">
-        <v>28</v>
+        <v>29</v>
       </c>
       <c r="E4" s="1" t="s">
-        <v>29</v>
+        <v>30</v>
       </c>
       <c r="F4" s="1">
         <v>2019</v>
       </c>
       <c r="G4" s="1" t="s">
-        <v>30</v>
+        <v>31</v>
       </c>
       <c r="H4" s="1">
         <v>3</v>
@@ -2698,10 +2705,10 @@
         <v>9</v>
       </c>
       <c r="K4" s="1" t="s">
-        <v>31</v>
+        <v>32</v>
       </c>
       <c r="L4" s="1" t="s">
-        <v>32</v>
+        <v>33</v>
       </c>
       <c r="M4" s="1">
         <v>28</v>
@@ -2728,7 +2735,7 @@
       </c>
       <c r="W4" s="1"/>
       <c r="X4" s="1" t="s">
-        <v>33</v>
+        <v>34</v>
       </c>
       <c r="Y4" s="1">
         <v>8</v>
@@ -3001,25 +3008,25 @@
     </row>
     <row r="5" ht="15.5" spans="1:288">
       <c r="A5" s="1" t="s">
-        <v>26</v>
+        <v>27</v>
       </c>
       <c r="B5" s="1">
         <v>4</v>
       </c>
       <c r="C5" s="1" t="s">
-        <v>36</v>
+        <v>37</v>
       </c>
       <c r="D5" s="1" t="s">
-        <v>28</v>
+        <v>29</v>
       </c>
       <c r="E5" s="1" t="s">
-        <v>29</v>
+        <v>30</v>
       </c>
       <c r="F5" s="1">
         <v>2019</v>
       </c>
       <c r="G5" s="1" t="s">
-        <v>30</v>
+        <v>31</v>
       </c>
       <c r="H5" s="1">
         <v>4</v>
@@ -3028,13 +3035,13 @@
         <v>4</v>
       </c>
       <c r="J5" s="1" t="s">
-        <v>37</v>
+        <v>38</v>
       </c>
       <c r="K5" s="1" t="s">
-        <v>38</v>
+        <v>39</v>
       </c>
       <c r="L5" s="1" t="s">
-        <v>39</v>
+        <v>40</v>
       </c>
       <c r="M5" s="1">
         <v>40</v>
@@ -3061,7 +3068,7 @@
       </c>
       <c r="W5" s="1"/>
       <c r="X5" s="1" t="s">
-        <v>33</v>
+        <v>34</v>
       </c>
       <c r="Y5" s="1">
         <v>14</v>
@@ -3334,25 +3341,25 @@
     </row>
     <row r="6" ht="15.5" spans="1:288">
       <c r="A6" s="1" t="s">
-        <v>26</v>
+        <v>27</v>
       </c>
       <c r="B6" s="1">
         <v>5</v>
       </c>
       <c r="C6" s="1" t="s">
-        <v>40</v>
+        <v>41</v>
       </c>
       <c r="D6" s="1" t="s">
-        <v>41</v>
+        <v>42</v>
       </c>
       <c r="E6" s="1" t="s">
-        <v>42</v>
+        <v>43</v>
       </c>
       <c r="F6" s="1">
         <v>2020</v>
       </c>
       <c r="G6" s="1" t="s">
-        <v>43</v>
+        <v>44</v>
       </c>
       <c r="H6" s="1">
         <v>1</v>
@@ -3364,10 +3371,10 @@
         <v>9</v>
       </c>
       <c r="K6" s="1" t="s">
-        <v>44</v>
+        <v>45</v>
       </c>
       <c r="L6" s="1" t="s">
-        <v>45</v>
+        <v>46</v>
       </c>
       <c r="M6" s="1">
         <v>92</v>
@@ -3381,10 +3388,10 @@
         <v>92</v>
       </c>
       <c r="Q6" s="1" t="s">
-        <v>46</v>
+        <v>47</v>
       </c>
       <c r="R6" s="1" t="s">
-        <v>47</v>
+        <v>48</v>
       </c>
       <c r="S6" s="1"/>
       <c r="T6" s="7">
@@ -3398,7 +3405,7 @@
       </c>
       <c r="W6" s="1"/>
       <c r="X6" s="1" t="s">
-        <v>33</v>
+        <v>34</v>
       </c>
       <c r="Y6" s="1">
         <v>19</v>
@@ -3406,7 +3413,9 @@
       <c r="Z6" s="1">
         <v>79</v>
       </c>
-      <c r="AA6" s="1"/>
+      <c r="AA6" s="1" t="s">
+        <v>26</v>
+      </c>
       <c r="AB6" s="1"/>
       <c r="AC6" s="1"/>
       <c r="AD6" s="1"/>
@@ -3675,19 +3684,19 @@
         <v>6</v>
       </c>
       <c r="C7" s="1" t="s">
-        <v>48</v>
+        <v>49</v>
       </c>
       <c r="D7" s="1" t="s">
-        <v>49</v>
+        <v>50</v>
       </c>
       <c r="E7" s="1" t="s">
-        <v>50</v>
+        <v>51</v>
       </c>
       <c r="F7" s="1">
         <v>2020</v>
       </c>
       <c r="G7" s="1" t="s">
-        <v>51</v>
+        <v>52</v>
       </c>
       <c r="H7" s="1">
         <v>1</v>
@@ -3700,7 +3709,7 @@
       </c>
       <c r="K7" s="1"/>
       <c r="L7" s="1" t="s">
-        <v>52</v>
+        <v>53</v>
       </c>
       <c r="M7" s="1">
         <v>46</v>
@@ -3726,10 +3735,10 @@
         <v>0</v>
       </c>
       <c r="W7" s="1" t="s">
-        <v>53</v>
+        <v>54</v>
       </c>
       <c r="X7" s="1" t="s">
-        <v>54</v>
+        <v>55</v>
       </c>
       <c r="Y7" s="1">
         <v>19</v>
@@ -4006,19 +4015,19 @@
         <v>7</v>
       </c>
       <c r="C8" s="1" t="s">
-        <v>55</v>
+        <v>56</v>
       </c>
       <c r="D8" s="1" t="s">
-        <v>56</v>
+        <v>57</v>
       </c>
       <c r="E8" s="1" t="s">
-        <v>57</v>
+        <v>58</v>
       </c>
       <c r="F8" s="1">
         <v>2020</v>
       </c>
       <c r="G8" s="1" t="s">
-        <v>58</v>
+        <v>59</v>
       </c>
       <c r="H8" s="1">
         <v>1</v>
@@ -4030,10 +4039,10 @@
         <v>9</v>
       </c>
       <c r="K8" s="1" t="s">
-        <v>59</v>
+        <v>60</v>
       </c>
       <c r="L8" s="1" t="s">
-        <v>45</v>
+        <v>46</v>
       </c>
       <c r="M8" s="1">
         <v>31</v>
@@ -4043,7 +4052,7 @@
       </c>
       <c r="O8" s="1"/>
       <c r="P8" s="1">
-        <f t="shared" ref="P8:P48" si="1">M8-O8</f>
+        <f t="shared" si="0"/>
         <v>31</v>
       </c>
       <c r="R8" s="1"/>
@@ -4059,7 +4068,7 @@
       </c>
       <c r="W8" s="1"/>
       <c r="X8" s="1" t="s">
-        <v>60</v>
+        <v>61</v>
       </c>
       <c r="Y8" s="1">
         <v>14</v>
@@ -4336,19 +4345,19 @@
         <v>8</v>
       </c>
       <c r="C9" s="1" t="s">
-        <v>61</v>
+        <v>62</v>
       </c>
       <c r="D9" s="1" t="s">
-        <v>62</v>
+        <v>63</v>
       </c>
       <c r="E9" s="1" t="s">
-        <v>63</v>
+        <v>64</v>
       </c>
       <c r="F9" s="1">
         <v>2021</v>
       </c>
       <c r="G9" s="1" t="s">
-        <v>64</v>
+        <v>65</v>
       </c>
       <c r="H9" s="1">
         <v>1</v>
@@ -4361,7 +4370,7 @@
       </c>
       <c r="K9" s="1"/>
       <c r="L9" s="1" t="s">
-        <v>52</v>
+        <v>53</v>
       </c>
       <c r="M9" s="1">
         <v>40</v>
@@ -4373,11 +4382,11 @@
         <v>7</v>
       </c>
       <c r="P9" s="1">
-        <f t="shared" si="1"/>
+        <f t="shared" si="0"/>
         <v>33</v>
       </c>
       <c r="Q9" s="9" t="s">
-        <v>65</v>
+        <v>66</v>
       </c>
       <c r="R9" s="1"/>
       <c r="S9" s="1"/>
@@ -4391,7 +4400,7 @@
         <v>0</v>
       </c>
       <c r="W9" s="1" t="s">
-        <v>66</v>
+        <v>67</v>
       </c>
       <c r="X9" s="1"/>
       <c r="Y9" s="1">
@@ -4669,19 +4678,19 @@
         <v>9</v>
       </c>
       <c r="C10" s="1" t="s">
-        <v>67</v>
+        <v>68</v>
       </c>
       <c r="D10" s="1" t="s">
-        <v>68</v>
+        <v>69</v>
       </c>
       <c r="E10" s="1" t="s">
-        <v>29</v>
+        <v>30</v>
       </c>
       <c r="F10" s="1">
         <v>2020</v>
       </c>
       <c r="G10" s="1" t="s">
-        <v>69</v>
+        <v>70</v>
       </c>
       <c r="H10" s="1">
         <v>2</v>
@@ -4694,7 +4703,7 @@
       </c>
       <c r="K10" s="1"/>
       <c r="L10" s="1" t="s">
-        <v>45</v>
+        <v>46</v>
       </c>
       <c r="M10" s="1">
         <v>56</v>
@@ -4706,7 +4715,7 @@
         <v>1</v>
       </c>
       <c r="P10" s="1">
-        <f t="shared" si="1"/>
+        <f t="shared" ref="P10:P48" si="1">M10-O10</f>
         <v>55</v>
       </c>
       <c r="Q10" s="1"/>
@@ -4723,7 +4732,7 @@
       </c>
       <c r="W10" s="1"/>
       <c r="X10" s="1" t="s">
-        <v>60</v>
+        <v>61</v>
       </c>
       <c r="Y10" s="1">
         <v>28</v>
@@ -4996,25 +5005,25 @@
     </row>
     <row r="11" ht="15.5" spans="1:288">
       <c r="A11" s="1" t="s">
-        <v>70</v>
+        <v>71</v>
       </c>
       <c r="B11" s="1">
         <v>10</v>
       </c>
       <c r="C11" s="1" t="s">
-        <v>71</v>
+        <v>72</v>
       </c>
       <c r="D11" s="1" t="s">
-        <v>72</v>
+        <v>73</v>
       </c>
       <c r="E11" s="1" t="s">
-        <v>73</v>
+        <v>74</v>
       </c>
       <c r="F11" s="1">
         <v>2020</v>
       </c>
       <c r="G11" s="1" t="s">
-        <v>74</v>
+        <v>75</v>
       </c>
       <c r="H11" s="1">
         <v>1</v>
@@ -5027,7 +5036,7 @@
       </c>
       <c r="K11" s="1"/>
       <c r="L11" s="1" t="s">
-        <v>75</v>
+        <v>76</v>
       </c>
       <c r="M11" s="1">
         <v>26</v>
@@ -5041,7 +5050,7 @@
         <v>26</v>
       </c>
       <c r="Q11" s="1" t="s">
-        <v>76</v>
+        <v>77</v>
       </c>
       <c r="R11" s="1"/>
       <c r="S11" s="1"/>
@@ -5055,10 +5064,10 @@
         <v>0</v>
       </c>
       <c r="W11" s="1" t="s">
-        <v>66</v>
+        <v>67</v>
       </c>
       <c r="X11" s="1" t="s">
-        <v>54</v>
+        <v>55</v>
       </c>
       <c r="Y11" s="1">
         <v>10</v>
@@ -5335,19 +5344,19 @@
         <v>11</v>
       </c>
       <c r="C12" s="1" t="s">
-        <v>77</v>
+        <v>78</v>
       </c>
       <c r="D12" s="1" t="s">
-        <v>72</v>
+        <v>73</v>
       </c>
       <c r="E12" s="1" t="s">
-        <v>73</v>
+        <v>74</v>
       </c>
       <c r="F12" s="1">
         <v>2020</v>
       </c>
       <c r="G12" s="1" t="s">
-        <v>74</v>
+        <v>75</v>
       </c>
       <c r="H12" s="1">
         <v>2</v>
@@ -5360,7 +5369,7 @@
       </c>
       <c r="K12" s="1"/>
       <c r="L12" s="1" t="s">
-        <v>78</v>
+        <v>79</v>
       </c>
       <c r="M12" s="1">
         <v>26</v>
@@ -5374,7 +5383,7 @@
         <v>26</v>
       </c>
       <c r="Q12" s="1" t="s">
-        <v>79</v>
+        <v>80</v>
       </c>
       <c r="R12" s="1"/>
       <c r="S12" s="1"/>
@@ -5388,10 +5397,10 @@
         <v>0</v>
       </c>
       <c r="W12" s="1" t="s">
-        <v>66</v>
+        <v>67</v>
       </c>
       <c r="X12" s="1" t="s">
-        <v>54</v>
+        <v>55</v>
       </c>
       <c r="Y12" s="1">
         <v>7</v>
@@ -5668,19 +5677,19 @@
         <v>12</v>
       </c>
       <c r="C13" s="1" t="s">
-        <v>80</v>
+        <v>81</v>
       </c>
       <c r="D13" s="1" t="s">
-        <v>81</v>
+        <v>82</v>
       </c>
       <c r="E13" s="1" t="s">
-        <v>82</v>
+        <v>83</v>
       </c>
       <c r="F13" s="1">
         <v>2019</v>
       </c>
       <c r="G13" s="1" t="s">
-        <v>83</v>
+        <v>84</v>
       </c>
       <c r="H13" s="1">
         <v>1</v>
@@ -5692,10 +5701,10 @@
         <v>9</v>
       </c>
       <c r="K13" s="1" t="s">
-        <v>84</v>
+        <v>85</v>
       </c>
       <c r="L13" s="1" t="s">
-        <v>85</v>
+        <v>86</v>
       </c>
       <c r="M13" s="1">
         <v>103</v>
@@ -5715,16 +5724,16 @@
         <v>1</v>
       </c>
       <c r="U13" t="s">
-        <v>86</v>
+        <v>87</v>
       </c>
       <c r="V13" s="8">
         <v>0</v>
       </c>
       <c r="W13" s="1" t="s">
-        <v>66</v>
+        <v>67</v>
       </c>
       <c r="X13" s="1" t="s">
-        <v>87</v>
+        <v>88</v>
       </c>
       <c r="Y13" s="1">
         <v>13</v>
@@ -5997,25 +6006,25 @@
     </row>
     <row r="14" ht="15.5" spans="1:288">
       <c r="A14" s="1" t="s">
-        <v>88</v>
+        <v>89</v>
       </c>
       <c r="B14" s="1">
         <v>13</v>
       </c>
       <c r="C14" s="1" t="s">
-        <v>89</v>
+        <v>90</v>
       </c>
       <c r="D14" s="1" t="s">
-        <v>90</v>
+        <v>91</v>
       </c>
       <c r="E14" s="1" t="s">
-        <v>91</v>
+        <v>92</v>
       </c>
       <c r="F14" s="1">
         <v>2018</v>
       </c>
       <c r="G14" s="1" t="s">
-        <v>92</v>
+        <v>93</v>
       </c>
       <c r="H14" s="1">
         <v>1</v>
@@ -6027,10 +6036,10 @@
         <v>9</v>
       </c>
       <c r="K14" s="1" t="s">
-        <v>59</v>
+        <v>60</v>
       </c>
       <c r="L14" s="1" t="s">
-        <v>45</v>
+        <v>46</v>
       </c>
       <c r="M14" s="1">
         <v>19</v>
@@ -6046,11 +6055,11 @@
         <v>18</v>
       </c>
       <c r="Q14" s="1" t="s">
-        <v>93</v>
+        <v>94</v>
       </c>
       <c r="R14" s="1"/>
       <c r="S14" s="1" t="s">
-        <v>94</v>
+        <v>26</v>
       </c>
       <c r="T14" s="7">
         <v>1</v>
@@ -6062,10 +6071,10 @@
         <v>1</v>
       </c>
       <c r="W14" s="1" t="s">
-        <v>66</v>
+        <v>67</v>
       </c>
       <c r="X14" s="1" t="s">
-        <v>60</v>
+        <v>61</v>
       </c>
       <c r="Y14" s="1">
         <v>9</v>
@@ -6073,7 +6082,9 @@
       <c r="Z14" s="1">
         <v>9</v>
       </c>
-      <c r="AA14" s="1"/>
+      <c r="AA14" s="1" t="s">
+        <v>26</v>
+      </c>
       <c r="AB14" s="1"/>
       <c r="AC14" s="1"/>
       <c r="AD14" s="1"/>
@@ -6338,7 +6349,7 @@
     </row>
     <row r="15" ht="15.5" spans="1:288">
       <c r="A15" s="1" t="s">
-        <v>88</v>
+        <v>89</v>
       </c>
       <c r="B15" s="1">
         <v>14</v>
@@ -6347,16 +6358,16 @@
         <v>95</v>
       </c>
       <c r="D15" s="1" t="s">
-        <v>90</v>
+        <v>91</v>
       </c>
       <c r="E15" s="1" t="s">
-        <v>91</v>
+        <v>92</v>
       </c>
       <c r="F15" s="1">
         <v>2018</v>
       </c>
       <c r="G15" s="1" t="s">
-        <v>92</v>
+        <v>93</v>
       </c>
       <c r="H15" s="1">
         <v>2</v>
@@ -6368,10 +6379,10 @@
         <v>9</v>
       </c>
       <c r="K15" s="1" t="s">
-        <v>59</v>
+        <v>60</v>
       </c>
       <c r="L15" s="1" t="s">
-        <v>45</v>
+        <v>46</v>
       </c>
       <c r="M15" s="1">
         <v>20</v>
@@ -6387,11 +6398,11 @@
         <v>18</v>
       </c>
       <c r="Q15" s="1" t="s">
-        <v>93</v>
+        <v>94</v>
       </c>
       <c r="R15" s="1"/>
       <c r="S15" s="1" t="s">
-        <v>94</v>
+        <v>26</v>
       </c>
       <c r="T15" s="7">
         <v>1</v>
@@ -6403,10 +6414,10 @@
         <v>1</v>
       </c>
       <c r="W15" s="1" t="s">
-        <v>66</v>
+        <v>67</v>
       </c>
       <c r="X15" s="1" t="s">
-        <v>60</v>
+        <v>61</v>
       </c>
       <c r="Y15" s="1">
         <v>9</v>
@@ -6414,7 +6425,9 @@
       <c r="Z15" s="1">
         <v>9</v>
       </c>
-      <c r="AA15" s="1"/>
+      <c r="AA15" s="1" t="s">
+        <v>26</v>
+      </c>
       <c r="AB15" s="1"/>
       <c r="AC15" s="1"/>
       <c r="AD15" s="1"/>
@@ -6695,7 +6708,7 @@
         <v>2021</v>
       </c>
       <c r="G16" s="1" t="s">
-        <v>43</v>
+        <v>44</v>
       </c>
       <c r="H16" s="1">
         <v>1</v>
@@ -6707,10 +6720,10 @@
         <v>9</v>
       </c>
       <c r="K16" s="1" t="s">
-        <v>59</v>
+        <v>60</v>
       </c>
       <c r="L16" s="1" t="s">
-        <v>45</v>
+        <v>46</v>
       </c>
       <c r="M16" s="1">
         <v>30</v>
@@ -6747,7 +6760,9 @@
       <c r="Z16" s="1">
         <v>21</v>
       </c>
-      <c r="AA16" s="1"/>
+      <c r="AA16" s="1" t="s">
+        <v>26</v>
+      </c>
       <c r="AB16" s="1"/>
       <c r="AC16" s="1"/>
       <c r="AD16" s="1"/>
@@ -7016,7 +7031,7 @@
         <v>16</v>
       </c>
       <c r="C17" s="1" t="s">
-        <v>96</v>
+        <v>100</v>
       </c>
       <c r="D17" s="1" t="s">
         <v>97</v>
@@ -7028,7 +7043,7 @@
         <v>2021</v>
       </c>
       <c r="G17" s="1" t="s">
-        <v>43</v>
+        <v>44</v>
       </c>
       <c r="H17" s="1">
         <v>2</v>
@@ -7040,10 +7055,10 @@
         <v>9</v>
       </c>
       <c r="K17" s="1" t="s">
-        <v>59</v>
+        <v>60</v>
       </c>
       <c r="L17" s="1" t="s">
-        <v>45</v>
+        <v>46</v>
       </c>
       <c r="M17" s="1">
         <v>30</v>
@@ -7078,7 +7093,9 @@
       <c r="Z17" s="1">
         <v>17</v>
       </c>
-      <c r="AA17" s="1"/>
+      <c r="AA17" s="1" t="s">
+        <v>26</v>
+      </c>
       <c r="AB17" s="1"/>
       <c r="AC17" s="1"/>
       <c r="AD17" s="1"/>
@@ -7347,13 +7364,13 @@
         <v>17</v>
       </c>
       <c r="C18" s="1" t="s">
-        <v>100</v>
+        <v>101</v>
       </c>
       <c r="D18" s="1" t="s">
-        <v>101</v>
+        <v>102</v>
       </c>
       <c r="E18" s="1" t="s">
-        <v>102</v>
+        <v>103</v>
       </c>
       <c r="F18" s="1">
         <v>2021</v>
@@ -7369,10 +7386,10 @@
         <v>9</v>
       </c>
       <c r="K18" s="1" t="s">
-        <v>59</v>
+        <v>60</v>
       </c>
       <c r="L18" s="1" t="s">
-        <v>45</v>
+        <v>46</v>
       </c>
       <c r="M18" s="1">
         <v>13</v>
@@ -7398,10 +7415,10 @@
         <v>0</v>
       </c>
       <c r="W18" s="1" t="s">
-        <v>66</v>
+        <v>67</v>
       </c>
       <c r="X18" s="1" t="s">
-        <v>103</v>
+        <v>104</v>
       </c>
       <c r="Y18" s="1">
         <v>3</v>
@@ -7678,13 +7695,13 @@
         <v>18</v>
       </c>
       <c r="C19" s="1" t="s">
-        <v>104</v>
+        <v>105</v>
       </c>
       <c r="D19" s="1" t="s">
-        <v>101</v>
+        <v>102</v>
       </c>
       <c r="E19" s="1" t="s">
-        <v>102</v>
+        <v>103</v>
       </c>
       <c r="F19" s="1">
         <v>2021</v>
@@ -7697,13 +7714,13 @@
         <v>2</v>
       </c>
       <c r="J19" s="6" t="s">
-        <v>105</v>
+        <v>106</v>
       </c>
       <c r="K19" s="1" t="s">
-        <v>106</v>
+        <v>107</v>
       </c>
       <c r="L19" s="1" t="s">
-        <v>45</v>
+        <v>46</v>
       </c>
       <c r="M19" s="1">
         <v>27</v>
@@ -7729,10 +7746,10 @@
         <v>0</v>
       </c>
       <c r="W19" s="1" t="s">
-        <v>66</v>
+        <v>67</v>
       </c>
       <c r="X19" s="1" t="s">
-        <v>103</v>
+        <v>104</v>
       </c>
       <c r="Y19" s="1">
         <v>9</v>
@@ -8009,13 +8026,13 @@
         <v>19</v>
       </c>
       <c r="C20" s="1" t="s">
-        <v>107</v>
+        <v>108</v>
       </c>
       <c r="D20" s="1" t="s">
-        <v>101</v>
+        <v>102</v>
       </c>
       <c r="E20" s="1" t="s">
-        <v>102</v>
+        <v>103</v>
       </c>
       <c r="F20" s="1">
         <v>2021</v>
@@ -8031,10 +8048,10 @@
         <v>9</v>
       </c>
       <c r="K20" s="1" t="s">
-        <v>105</v>
+        <v>106</v>
       </c>
       <c r="L20" s="1" t="s">
-        <v>45</v>
+        <v>46</v>
       </c>
       <c r="M20" s="1">
         <v>27</v>
@@ -8060,10 +8077,10 @@
         <v>0</v>
       </c>
       <c r="W20" s="1" t="s">
-        <v>66</v>
+        <v>67</v>
       </c>
       <c r="X20" s="1" t="s">
-        <v>103</v>
+        <v>104</v>
       </c>
       <c r="Y20" s="1">
         <v>12</v>
@@ -8340,13 +8357,13 @@
         <v>20</v>
       </c>
       <c r="C21" s="1" t="s">
-        <v>108</v>
+        <v>109</v>
       </c>
       <c r="D21" s="1" t="s">
-        <v>101</v>
+        <v>102</v>
       </c>
       <c r="E21" s="1" t="s">
-        <v>102</v>
+        <v>103</v>
       </c>
       <c r="F21" s="1">
         <v>2021</v>
@@ -8362,10 +8379,10 @@
         <v>9</v>
       </c>
       <c r="K21" s="1" t="s">
-        <v>59</v>
+        <v>60</v>
       </c>
       <c r="L21" s="1" t="s">
-        <v>45</v>
+        <v>46</v>
       </c>
       <c r="M21" s="1">
         <v>26</v>
@@ -8391,10 +8408,10 @@
         <v>0</v>
       </c>
       <c r="W21" s="1" t="s">
-        <v>66</v>
+        <v>67</v>
       </c>
       <c r="X21" s="1" t="s">
-        <v>103</v>
+        <v>104</v>
       </c>
       <c r="Y21" s="1">
         <v>9</v>
@@ -8671,19 +8688,19 @@
         <v>21</v>
       </c>
       <c r="C22" s="1" t="s">
-        <v>109</v>
+        <v>110</v>
       </c>
       <c r="D22" s="1" t="s">
-        <v>110</v>
+        <v>111</v>
       </c>
       <c r="E22" s="1" t="s">
-        <v>111</v>
+        <v>112</v>
       </c>
       <c r="F22" s="1">
         <v>2020</v>
       </c>
       <c r="G22" s="1" t="s">
-        <v>112</v>
+        <v>113</v>
       </c>
       <c r="H22" s="1">
         <v>1</v>
@@ -8696,7 +8713,7 @@
       </c>
       <c r="K22" s="1"/>
       <c r="L22" s="1" t="s">
-        <v>45</v>
+        <v>46</v>
       </c>
       <c r="M22" s="1">
         <v>38</v>
@@ -8724,10 +8741,10 @@
         <v>0</v>
       </c>
       <c r="W22" s="1" t="s">
-        <v>66</v>
+        <v>67</v>
       </c>
       <c r="X22" s="1" t="s">
-        <v>87</v>
+        <v>88</v>
       </c>
       <c r="Y22" s="1">
         <v>9</v>
@@ -9004,19 +9021,19 @@
         <v>22</v>
       </c>
       <c r="C23" s="1" t="s">
-        <v>113</v>
+        <v>114</v>
       </c>
       <c r="D23" s="1" t="s">
-        <v>110</v>
+        <v>111</v>
       </c>
       <c r="E23" s="1" t="s">
-        <v>111</v>
+        <v>112</v>
       </c>
       <c r="F23" s="1">
         <v>2020</v>
       </c>
       <c r="G23" s="1" t="s">
-        <v>112</v>
+        <v>113</v>
       </c>
       <c r="H23" s="1">
         <v>2</v>
@@ -9029,7 +9046,7 @@
       </c>
       <c r="K23" s="1"/>
       <c r="L23" s="1" t="s">
-        <v>45</v>
+        <v>46</v>
       </c>
       <c r="M23" s="1">
         <v>33</v>
@@ -9057,10 +9074,10 @@
         <v>0</v>
       </c>
       <c r="W23" s="1" t="s">
-        <v>66</v>
+        <v>67</v>
       </c>
       <c r="X23" s="1" t="s">
-        <v>87</v>
+        <v>88</v>
       </c>
       <c r="Y23" s="1">
         <v>7</v>
@@ -9337,19 +9354,19 @@
         <v>23</v>
       </c>
       <c r="C24" s="1" t="s">
-        <v>114</v>
+        <v>115</v>
       </c>
       <c r="D24" s="1" t="s">
-        <v>110</v>
+        <v>111</v>
       </c>
       <c r="E24" s="1" t="s">
-        <v>111</v>
+        <v>112</v>
       </c>
       <c r="F24" s="1">
         <v>2020</v>
       </c>
       <c r="G24" s="1" t="s">
-        <v>112</v>
+        <v>113</v>
       </c>
       <c r="H24" s="1">
         <v>3</v>
@@ -9362,7 +9379,7 @@
       </c>
       <c r="K24" s="1"/>
       <c r="L24" s="1" t="s">
-        <v>45</v>
+        <v>46</v>
       </c>
       <c r="M24" s="1">
         <v>36</v>
@@ -9390,10 +9407,10 @@
         <v>0</v>
       </c>
       <c r="W24" s="1" t="s">
-        <v>66</v>
+        <v>67</v>
       </c>
       <c r="X24" s="1" t="s">
-        <v>87</v>
+        <v>88</v>
       </c>
       <c r="Y24" s="1">
         <v>7</v>
@@ -9670,19 +9687,19 @@
         <v>24</v>
       </c>
       <c r="C25" s="1" t="s">
-        <v>115</v>
+        <v>116</v>
       </c>
       <c r="D25" s="1" t="s">
-        <v>116</v>
+        <v>117</v>
       </c>
       <c r="E25" s="1" t="s">
-        <v>117</v>
+        <v>118</v>
       </c>
       <c r="F25" s="1">
         <v>2022</v>
       </c>
       <c r="G25" s="1" t="s">
-        <v>118</v>
+        <v>119</v>
       </c>
       <c r="H25" s="1">
         <v>1</v>
@@ -9694,7 +9711,7 @@
         <v>9</v>
       </c>
       <c r="K25" s="1" t="s">
-        <v>59</v>
+        <v>60</v>
       </c>
       <c r="L25" s="1"/>
       <c r="M25" s="1">
@@ -9997,19 +10014,19 @@
         <v>25</v>
       </c>
       <c r="C26" s="1" t="s">
-        <v>119</v>
+        <v>120</v>
       </c>
       <c r="D26" s="1" t="s">
-        <v>116</v>
+        <v>117</v>
       </c>
       <c r="E26" s="1" t="s">
-        <v>117</v>
+        <v>118</v>
       </c>
       <c r="F26" s="1">
         <v>2022</v>
       </c>
       <c r="G26" s="1" t="s">
-        <v>118</v>
+        <v>119</v>
       </c>
       <c r="H26" s="1">
         <v>2</v>
@@ -10021,7 +10038,7 @@
         <v>9</v>
       </c>
       <c r="K26" s="1" t="s">
-        <v>59</v>
+        <v>60</v>
       </c>
       <c r="L26" s="1"/>
       <c r="M26" s="1">
@@ -10036,7 +10053,7 @@
         <v>24</v>
       </c>
       <c r="Q26" s="1" t="s">
-        <v>120</v>
+        <v>121</v>
       </c>
       <c r="R26" s="1"/>
       <c r="S26" s="1"/>
@@ -10326,19 +10343,19 @@
         <v>26</v>
       </c>
       <c r="C27" s="1" t="s">
-        <v>121</v>
+        <v>122</v>
       </c>
       <c r="D27" s="1" t="s">
-        <v>116</v>
+        <v>117</v>
       </c>
       <c r="E27" s="1" t="s">
-        <v>117</v>
+        <v>118</v>
       </c>
       <c r="F27" s="1">
         <v>2022</v>
       </c>
       <c r="G27" s="1" t="s">
-        <v>118</v>
+        <v>119</v>
       </c>
       <c r="H27" s="1">
         <v>3</v>
@@ -10350,7 +10367,7 @@
         <v>9</v>
       </c>
       <c r="K27" s="1" t="s">
-        <v>59</v>
+        <v>60</v>
       </c>
       <c r="L27" s="1"/>
       <c r="M27" s="1">
@@ -10365,7 +10382,7 @@
         <v>25</v>
       </c>
       <c r="Q27" s="1" t="s">
-        <v>122</v>
+        <v>123</v>
       </c>
       <c r="R27" s="1"/>
       <c r="S27" s="1"/>
@@ -10655,19 +10672,19 @@
         <v>27</v>
       </c>
       <c r="C28" s="1" t="s">
-        <v>123</v>
+        <v>124</v>
       </c>
       <c r="D28" s="1" t="s">
-        <v>124</v>
+        <v>125</v>
       </c>
       <c r="E28" s="1" t="s">
-        <v>125</v>
+        <v>126</v>
       </c>
       <c r="F28" s="1">
         <v>2021</v>
       </c>
       <c r="G28" s="1" t="s">
-        <v>126</v>
+        <v>127</v>
       </c>
       <c r="H28" s="1">
         <v>1</v>
@@ -10679,10 +10696,10 @@
         <v>9</v>
       </c>
       <c r="K28" s="1" t="s">
-        <v>59</v>
+        <v>60</v>
       </c>
       <c r="L28" s="1" t="s">
-        <v>45</v>
+        <v>46</v>
       </c>
       <c r="M28" s="1">
         <v>105</v>
@@ -10696,7 +10713,7 @@
         <v>105</v>
       </c>
       <c r="Q28" s="10" t="s">
-        <v>127</v>
+        <v>128</v>
       </c>
       <c r="R28" s="1"/>
       <c r="S28" s="1"/>
@@ -10710,10 +10727,10 @@
         <v>0</v>
       </c>
       <c r="W28" s="1" t="s">
-        <v>66</v>
+        <v>67</v>
       </c>
       <c r="X28" s="1" t="s">
-        <v>54</v>
+        <v>55</v>
       </c>
       <c r="Y28" s="1">
         <v>51</v>
@@ -10986,25 +11003,25 @@
     </row>
     <row r="29" ht="15.5" spans="1:288">
       <c r="A29" s="1" t="s">
-        <v>88</v>
+        <v>89</v>
       </c>
       <c r="B29" s="1">
         <v>28</v>
       </c>
       <c r="C29" s="1" t="s">
-        <v>128</v>
+        <v>129</v>
       </c>
       <c r="D29" s="1" t="s">
-        <v>129</v>
+        <v>130</v>
       </c>
       <c r="E29" s="1" t="s">
-        <v>130</v>
+        <v>131</v>
       </c>
       <c r="F29" s="1">
         <v>2023</v>
       </c>
       <c r="G29" s="1" t="s">
-        <v>131</v>
+        <v>132</v>
       </c>
       <c r="H29" s="1">
         <v>1</v>
@@ -11017,7 +11034,7 @@
       </c>
       <c r="K29" s="1"/>
       <c r="L29" s="1" t="s">
-        <v>45</v>
+        <v>46</v>
       </c>
       <c r="M29" s="1">
         <v>302</v>
@@ -11045,7 +11062,7 @@
         <v>0</v>
       </c>
       <c r="W29" s="11" t="s">
-        <v>132</v>
+        <v>133</v>
       </c>
       <c r="X29" s="1"/>
       <c r="Y29" s="1">
@@ -11321,19 +11338,19 @@
     </row>
     <row r="30" ht="15.5" spans="1:288">
       <c r="A30" s="1" t="s">
-        <v>133</v>
+        <v>134</v>
       </c>
       <c r="B30" s="1">
         <v>29</v>
       </c>
       <c r="C30" s="1" t="s">
-        <v>134</v>
+        <v>135</v>
       </c>
       <c r="D30" s="1" t="s">
-        <v>135</v>
+        <v>136</v>
       </c>
       <c r="E30" s="1" t="s">
-        <v>50</v>
+        <v>51</v>
       </c>
       <c r="F30" s="1">
         <v>2023</v>
@@ -11343,14 +11360,14 @@
         <v>1</v>
       </c>
       <c r="I30" s="1" t="s">
-        <v>136</v>
+        <v>137</v>
       </c>
       <c r="J30" s="1" t="s">
         <v>9</v>
       </c>
       <c r="K30" s="1"/>
       <c r="L30" s="1" t="s">
-        <v>45</v>
+        <v>46</v>
       </c>
       <c r="M30" s="1">
         <v>23</v>
@@ -11366,11 +11383,11 @@
         <v>20</v>
       </c>
       <c r="Q30" s="1" t="s">
-        <v>137</v>
+        <v>138</v>
       </c>
       <c r="R30" s="1"/>
       <c r="S30" s="1" t="s">
-        <v>138</v>
+        <v>139</v>
       </c>
       <c r="T30" s="7">
         <v>1</v>
@@ -11650,19 +11667,19 @@
     </row>
     <row r="31" ht="15.5" spans="1:288">
       <c r="A31" s="1" t="s">
-        <v>139</v>
+        <v>140</v>
       </c>
       <c r="B31" s="1">
         <v>30</v>
       </c>
       <c r="C31" s="1" t="s">
-        <v>140</v>
+        <v>141</v>
       </c>
       <c r="D31" s="1" t="s">
-        <v>141</v>
+        <v>142</v>
       </c>
       <c r="E31" s="1" t="s">
-        <v>142</v>
+        <v>143</v>
       </c>
       <c r="F31" s="1">
         <v>2014</v>
@@ -11672,16 +11689,16 @@
         <v>1</v>
       </c>
       <c r="I31" s="1" t="s">
-        <v>143</v>
+        <v>144</v>
       </c>
       <c r="J31" s="1" t="s">
         <v>9</v>
       </c>
       <c r="K31" s="1" t="s">
-        <v>59</v>
+        <v>60</v>
       </c>
       <c r="L31" s="1" t="s">
-        <v>45</v>
+        <v>46</v>
       </c>
       <c r="M31" s="1">
         <v>24</v>
@@ -11969,19 +11986,19 @@
     </row>
     <row r="32" ht="15.5" spans="1:288">
       <c r="A32" s="1" t="s">
-        <v>139</v>
+        <v>140</v>
       </c>
       <c r="B32" s="1">
         <v>31</v>
       </c>
       <c r="C32" s="1" t="s">
-        <v>144</v>
+        <v>145</v>
       </c>
       <c r="D32" s="1" t="s">
-        <v>145</v>
+        <v>146</v>
       </c>
       <c r="E32" s="1" t="s">
-        <v>142</v>
+        <v>143</v>
       </c>
       <c r="F32" s="1">
         <v>2015</v>
@@ -11991,16 +12008,16 @@
         <v>1</v>
       </c>
       <c r="I32" s="1" t="s">
-        <v>143</v>
+        <v>144</v>
       </c>
       <c r="J32" s="1" t="s">
         <v>9</v>
       </c>
       <c r="K32" s="1" t="s">
-        <v>59</v>
+        <v>60</v>
       </c>
       <c r="L32" s="1" t="s">
-        <v>45</v>
+        <v>46</v>
       </c>
       <c r="M32" s="1">
         <v>20</v>
@@ -12288,19 +12305,19 @@
     </row>
     <row r="33" ht="15.5" spans="1:288">
       <c r="A33" s="1" t="s">
-        <v>139</v>
+        <v>140</v>
       </c>
       <c r="B33" s="1">
         <v>32</v>
       </c>
       <c r="C33" s="1" t="s">
+        <v>147</v>
+      </c>
+      <c r="D33" s="1" t="s">
         <v>146</v>
       </c>
-      <c r="D33" s="1" t="s">
-        <v>145</v>
-      </c>
       <c r="E33" s="1" t="s">
-        <v>142</v>
+        <v>143</v>
       </c>
       <c r="F33" s="1">
         <v>2015</v>
@@ -12310,16 +12327,16 @@
         <v>2</v>
       </c>
       <c r="I33" s="1" t="s">
-        <v>143</v>
+        <v>144</v>
       </c>
       <c r="J33" s="1" t="s">
         <v>9</v>
       </c>
       <c r="K33" s="1" t="s">
-        <v>59</v>
+        <v>60</v>
       </c>
       <c r="L33" s="1" t="s">
-        <v>45</v>
+        <v>46</v>
       </c>
       <c r="M33" s="1">
         <v>21</v>
@@ -12607,25 +12624,25 @@
     </row>
     <row r="34" ht="15.5" spans="1:288">
       <c r="A34" s="1" t="s">
-        <v>147</v>
+        <v>148</v>
       </c>
       <c r="B34" s="1">
         <v>33</v>
       </c>
       <c r="C34" s="1" t="s">
-        <v>148</v>
+        <v>149</v>
       </c>
       <c r="D34" s="1" t="s">
-        <v>149</v>
+        <v>150</v>
       </c>
       <c r="E34" s="1" t="s">
-        <v>150</v>
+        <v>151</v>
       </c>
       <c r="F34" s="1">
         <v>2014</v>
       </c>
       <c r="G34" s="1" t="s">
-        <v>151</v>
+        <v>152</v>
       </c>
       <c r="H34" s="1">
         <v>1</v>
@@ -12637,10 +12654,10 @@
         <v>9</v>
       </c>
       <c r="K34" s="1" t="s">
-        <v>152</v>
+        <v>153</v>
       </c>
       <c r="L34" s="1" t="s">
-        <v>45</v>
+        <v>46</v>
       </c>
       <c r="M34" s="1">
         <v>24</v>
@@ -12654,7 +12671,7 @@
         <v>24</v>
       </c>
       <c r="Q34" s="1" t="s">
-        <v>153</v>
+        <v>154</v>
       </c>
       <c r="R34" s="1"/>
       <c r="S34" s="1"/>
@@ -12930,25 +12947,25 @@
     </row>
     <row r="35" ht="15.5" spans="1:288">
       <c r="A35" s="1" t="s">
-        <v>154</v>
+        <v>155</v>
       </c>
       <c r="B35" s="1">
         <v>34</v>
       </c>
       <c r="C35" s="1" t="s">
-        <v>155</v>
+        <v>156</v>
       </c>
       <c r="D35" s="1" t="s">
-        <v>149</v>
+        <v>150</v>
       </c>
       <c r="E35" s="1" t="s">
-        <v>150</v>
+        <v>151</v>
       </c>
       <c r="F35" s="1">
         <v>2014</v>
       </c>
       <c r="G35" s="1" t="s">
-        <v>151</v>
+        <v>152</v>
       </c>
       <c r="H35" s="1">
         <v>2</v>
@@ -12960,10 +12977,10 @@
         <v>9</v>
       </c>
       <c r="K35" s="1" t="s">
-        <v>152</v>
+        <v>153</v>
       </c>
       <c r="L35" s="1" t="s">
-        <v>45</v>
+        <v>46</v>
       </c>
       <c r="M35" s="1">
         <v>18</v>
@@ -12977,7 +12994,7 @@
         <v>18</v>
       </c>
       <c r="Q35" s="1" t="s">
-        <v>156</v>
+        <v>157</v>
       </c>
       <c r="R35" s="1"/>
       <c r="S35" s="1"/>
@@ -13253,25 +13270,25 @@
     </row>
     <row r="36" ht="15.5" spans="1:288">
       <c r="A36" s="1" t="s">
-        <v>157</v>
+        <v>158</v>
       </c>
       <c r="B36" s="1">
         <v>35</v>
       </c>
       <c r="C36" s="1" t="s">
-        <v>158</v>
+        <v>159</v>
       </c>
       <c r="D36" s="1" t="s">
-        <v>149</v>
+        <v>150</v>
       </c>
       <c r="E36" s="1" t="s">
-        <v>150</v>
+        <v>151</v>
       </c>
       <c r="F36" s="1">
         <v>2014</v>
       </c>
       <c r="G36" s="1" t="s">
-        <v>151</v>
+        <v>152</v>
       </c>
       <c r="H36" s="1">
         <v>3</v>
@@ -13283,10 +13300,10 @@
         <v>9</v>
       </c>
       <c r="K36" s="1" t="s">
-        <v>152</v>
+        <v>153</v>
       </c>
       <c r="L36" s="1" t="s">
-        <v>45</v>
+        <v>46</v>
       </c>
       <c r="M36" s="1">
         <v>22</v>
@@ -13300,7 +13317,7 @@
         <v>22</v>
       </c>
       <c r="Q36" s="1" t="s">
-        <v>159</v>
+        <v>160</v>
       </c>
       <c r="R36" s="1"/>
       <c r="S36" s="1"/>
@@ -13576,25 +13593,25 @@
     </row>
     <row r="37" ht="15.5" spans="1:288">
       <c r="A37" s="1" t="s">
-        <v>160</v>
+        <v>161</v>
       </c>
       <c r="B37" s="1">
         <v>36</v>
       </c>
       <c r="C37" s="1" t="s">
-        <v>161</v>
+        <v>162</v>
       </c>
       <c r="D37" s="1" t="s">
-        <v>149</v>
+        <v>150</v>
       </c>
       <c r="E37" s="1" t="s">
-        <v>150</v>
+        <v>151</v>
       </c>
       <c r="F37" s="1">
         <v>2014</v>
       </c>
       <c r="G37" s="1" t="s">
-        <v>151</v>
+        <v>152</v>
       </c>
       <c r="H37" s="1">
         <v>4</v>
@@ -13606,10 +13623,10 @@
         <v>9</v>
       </c>
       <c r="K37" s="1" t="s">
-        <v>152</v>
+        <v>153</v>
       </c>
       <c r="L37" s="1" t="s">
-        <v>45</v>
+        <v>46</v>
       </c>
       <c r="M37" s="1">
         <v>20</v>
@@ -13623,7 +13640,7 @@
         <v>20</v>
       </c>
       <c r="Q37" s="1" t="s">
-        <v>162</v>
+        <v>163</v>
       </c>
       <c r="R37" s="1"/>
       <c r="S37" s="1"/>
@@ -13903,19 +13920,19 @@
         <v>37</v>
       </c>
       <c r="C38" s="1" t="s">
-        <v>163</v>
+        <v>164</v>
       </c>
       <c r="D38" s="1" t="s">
-        <v>164</v>
+        <v>165</v>
       </c>
       <c r="E38" s="1" t="s">
-        <v>165</v>
+        <v>166</v>
       </c>
       <c r="F38" s="1">
         <v>2023</v>
       </c>
       <c r="G38" s="1" t="s">
-        <v>166</v>
+        <v>167</v>
       </c>
       <c r="H38" s="1">
         <v>1</v>
@@ -13928,7 +13945,7 @@
       </c>
       <c r="K38" s="1"/>
       <c r="L38" s="1" t="s">
-        <v>45</v>
+        <v>46</v>
       </c>
       <c r="M38" s="1">
         <v>40</v>
@@ -13954,7 +13971,7 @@
         <v>1</v>
       </c>
       <c r="W38" s="1" t="s">
-        <v>66</v>
+        <v>67</v>
       </c>
       <c r="X38" s="1"/>
       <c r="Y38" s="1"/>
@@ -14228,19 +14245,19 @@
         <v>38</v>
       </c>
       <c r="C39" s="1" t="s">
-        <v>167</v>
+        <v>168</v>
       </c>
       <c r="D39" s="1" t="s">
-        <v>168</v>
+        <v>169</v>
       </c>
       <c r="E39" s="1" t="s">
-        <v>169</v>
+        <v>170</v>
       </c>
       <c r="F39" s="1">
         <v>2023</v>
       </c>
       <c r="G39" s="1" t="s">
-        <v>170</v>
+        <v>171</v>
       </c>
       <c r="H39" s="1">
         <v>1</v>
@@ -14252,10 +14269,10 @@
         <v>9</v>
       </c>
       <c r="K39" s="1" t="s">
-        <v>59</v>
+        <v>60</v>
       </c>
       <c r="L39" s="1" t="s">
-        <v>45</v>
+        <v>46</v>
       </c>
       <c r="M39" s="1">
         <v>144</v>
@@ -14555,19 +14572,19 @@
         <v>39</v>
       </c>
       <c r="C40" s="1" t="s">
-        <v>171</v>
+        <v>172</v>
       </c>
       <c r="D40" s="1" t="s">
-        <v>172</v>
+        <v>173</v>
       </c>
       <c r="E40" s="1" t="s">
-        <v>173</v>
+        <v>174</v>
       </c>
       <c r="F40" s="1">
         <v>2021</v>
       </c>
       <c r="G40" s="1" t="s">
-        <v>58</v>
+        <v>59</v>
       </c>
       <c r="H40" s="1">
         <v>1</v>
@@ -14579,10 +14596,10 @@
         <v>9</v>
       </c>
       <c r="K40" s="1" t="s">
-        <v>59</v>
+        <v>60</v>
       </c>
       <c r="L40" s="1" t="s">
-        <v>45</v>
+        <v>46</v>
       </c>
       <c r="M40" s="1">
         <v>109</v>
@@ -14598,10 +14615,10 @@
         <v>108</v>
       </c>
       <c r="Q40" s="1" t="s">
-        <v>174</v>
+        <v>175</v>
       </c>
       <c r="R40" s="1" t="s">
-        <v>175</v>
+        <v>176</v>
       </c>
       <c r="S40" s="1"/>
       <c r="T40" s="1">
@@ -14614,7 +14631,7 @@
         <v>0</v>
       </c>
       <c r="W40" s="1" t="s">
-        <v>66</v>
+        <v>67</v>
       </c>
       <c r="X40" s="1"/>
       <c r="Y40" s="1"/>
@@ -14884,25 +14901,25 @@
     </row>
     <row r="41" ht="15.5" spans="1:288">
       <c r="A41" s="1" t="s">
-        <v>176</v>
+        <v>177</v>
       </c>
       <c r="B41" s="1">
         <v>40</v>
       </c>
       <c r="C41" s="1" t="s">
-        <v>177</v>
+        <v>178</v>
       </c>
       <c r="D41" s="1" t="s">
-        <v>178</v>
+        <v>179</v>
       </c>
       <c r="E41" s="1" t="s">
-        <v>179</v>
+        <v>180</v>
       </c>
       <c r="F41" s="1">
         <v>2023</v>
       </c>
       <c r="G41" s="1" t="s">
-        <v>112</v>
+        <v>113</v>
       </c>
       <c r="H41" s="1">
         <v>1</v>
@@ -14914,7 +14931,7 @@
         <v>9</v>
       </c>
       <c r="K41" s="1" t="s">
-        <v>84</v>
+        <v>85</v>
       </c>
       <c r="L41" s="1"/>
       <c r="M41" s="1">
@@ -14943,7 +14960,7 @@
         <v>0</v>
       </c>
       <c r="W41" s="1" t="s">
-        <v>66</v>
+        <v>67</v>
       </c>
       <c r="X41" s="1"/>
       <c r="Y41" s="1"/>
@@ -15217,19 +15234,19 @@
         <v>41</v>
       </c>
       <c r="C42" s="1" t="s">
-        <v>180</v>
+        <v>181</v>
       </c>
       <c r="D42" s="1" t="s">
-        <v>181</v>
+        <v>182</v>
       </c>
       <c r="E42" s="1" t="s">
-        <v>182</v>
+        <v>183</v>
       </c>
       <c r="F42" s="1">
         <v>2022</v>
       </c>
       <c r="G42" s="1" t="s">
-        <v>183</v>
+        <v>184</v>
       </c>
       <c r="H42" s="1">
         <v>1</v>
@@ -15242,7 +15259,7 @@
       </c>
       <c r="K42" s="1"/>
       <c r="L42" s="1" t="s">
-        <v>45</v>
+        <v>46</v>
       </c>
       <c r="M42" s="1">
         <v>30</v>
@@ -15258,7 +15275,7 @@
         <v>27</v>
       </c>
       <c r="Q42" s="1" t="s">
-        <v>184</v>
+        <v>185</v>
       </c>
       <c r="R42" s="1"/>
       <c r="S42" s="1"/>
@@ -15538,19 +15555,19 @@
         <v>42</v>
       </c>
       <c r="C43" s="1" t="s">
-        <v>185</v>
+        <v>186</v>
       </c>
       <c r="D43" s="1" t="s">
-        <v>181</v>
+        <v>182</v>
       </c>
       <c r="E43" s="1" t="s">
-        <v>182</v>
+        <v>183</v>
       </c>
       <c r="F43" s="1">
         <v>2022</v>
       </c>
       <c r="G43" s="1" t="s">
-        <v>183</v>
+        <v>184</v>
       </c>
       <c r="H43" s="1">
         <v>2</v>
@@ -15563,7 +15580,7 @@
       </c>
       <c r="K43" s="1"/>
       <c r="L43" s="1" t="s">
-        <v>45</v>
+        <v>46</v>
       </c>
       <c r="M43" s="1">
         <v>48</v>
@@ -15579,7 +15596,7 @@
         <v>46</v>
       </c>
       <c r="Q43" s="1" t="s">
-        <v>184</v>
+        <v>185</v>
       </c>
       <c r="R43" s="1"/>
       <c r="S43" s="1"/>
@@ -15855,25 +15872,25 @@
     </row>
     <row r="44" ht="15.5" spans="1:288">
       <c r="A44" s="1" t="s">
-        <v>186</v>
+        <v>187</v>
       </c>
       <c r="B44" s="1">
         <v>43</v>
       </c>
       <c r="C44" s="1" t="s">
-        <v>187</v>
+        <v>188</v>
       </c>
       <c r="D44" s="1" t="s">
-        <v>188</v>
+        <v>189</v>
       </c>
       <c r="E44" s="1" t="s">
-        <v>189</v>
+        <v>190</v>
       </c>
       <c r="F44" s="1">
         <v>2022</v>
       </c>
       <c r="G44" s="1" t="s">
-        <v>190</v>
+        <v>191</v>
       </c>
       <c r="H44" s="1">
         <v>1</v>
@@ -15885,10 +15902,10 @@
         <v>9</v>
       </c>
       <c r="K44" s="1" t="s">
-        <v>59</v>
+        <v>60</v>
       </c>
       <c r="L44" s="1" t="s">
-        <v>45</v>
+        <v>46</v>
       </c>
       <c r="M44" s="1">
         <v>328</v>
@@ -15910,7 +15927,7 @@
       <c r="U44" s="1"/>
       <c r="V44" s="1"/>
       <c r="W44" s="1" t="s">
-        <v>53</v>
+        <v>54</v>
       </c>
       <c r="X44" s="1"/>
       <c r="Y44" s="1"/>
@@ -16184,19 +16201,19 @@
         <v>44</v>
       </c>
       <c r="C45" s="1" t="s">
-        <v>191</v>
+        <v>192</v>
       </c>
       <c r="D45" s="1" t="s">
-        <v>192</v>
+        <v>193</v>
       </c>
       <c r="E45" s="1" t="s">
-        <v>91</v>
+        <v>92</v>
       </c>
       <c r="F45" s="1">
         <v>2020</v>
       </c>
       <c r="G45" s="1" t="s">
-        <v>118</v>
+        <v>119</v>
       </c>
       <c r="H45" s="1">
         <v>1</v>
@@ -16208,10 +16225,10 @@
         <v>9</v>
       </c>
       <c r="K45" s="1" t="s">
-        <v>59</v>
+        <v>60</v>
       </c>
       <c r="L45" s="1" t="s">
-        <v>85</v>
+        <v>86</v>
       </c>
       <c r="M45" s="1">
         <v>23</v>
@@ -16503,19 +16520,19 @@
         <v>45</v>
       </c>
       <c r="C46" s="1" t="s">
+        <v>194</v>
+      </c>
+      <c r="D46" s="1" t="s">
         <v>193</v>
       </c>
-      <c r="D46" s="1" t="s">
-        <v>192</v>
-      </c>
       <c r="E46" s="1" t="s">
-        <v>91</v>
+        <v>92</v>
       </c>
       <c r="F46" s="1">
         <v>2020</v>
       </c>
       <c r="G46" s="1" t="s">
-        <v>118</v>
+        <v>119</v>
       </c>
       <c r="H46" s="1">
         <v>1</v>
@@ -16527,10 +16544,10 @@
         <v>9</v>
       </c>
       <c r="K46" s="1" t="s">
-        <v>59</v>
+        <v>60</v>
       </c>
       <c r="L46" s="1" t="s">
-        <v>85</v>
+        <v>86</v>
       </c>
       <c r="M46" s="1">
         <v>21</v>
@@ -16824,19 +16841,19 @@
         <v>46</v>
       </c>
       <c r="C47" s="1" t="s">
-        <v>194</v>
+        <v>195</v>
       </c>
       <c r="D47" s="1" t="s">
-        <v>192</v>
+        <v>193</v>
       </c>
       <c r="E47" s="1" t="s">
-        <v>91</v>
+        <v>92</v>
       </c>
       <c r="F47" s="1">
         <v>2020</v>
       </c>
       <c r="G47" s="1" t="s">
-        <v>118</v>
+        <v>119</v>
       </c>
       <c r="H47" s="1">
         <v>1</v>
@@ -16848,10 +16865,10 @@
         <v>9</v>
       </c>
       <c r="K47" s="1" t="s">
-        <v>59</v>
+        <v>60</v>
       </c>
       <c r="L47" s="1" t="s">
-        <v>85</v>
+        <v>86</v>
       </c>
       <c r="M47" s="1">
         <v>18</v>
@@ -17143,19 +17160,19 @@
         <v>47</v>
       </c>
       <c r="C48" s="1" t="s">
-        <v>195</v>
+        <v>196</v>
       </c>
       <c r="D48" s="1" t="s">
-        <v>196</v>
+        <v>197</v>
       </c>
       <c r="E48" s="1" t="s">
-        <v>197</v>
+        <v>198</v>
       </c>
       <c r="F48" s="1">
         <v>2023</v>
       </c>
       <c r="G48" s="1" t="s">
-        <v>198</v>
+        <v>199</v>
       </c>
       <c r="H48" s="1">
         <v>1</v>
@@ -17456,19 +17473,19 @@
         <v>48</v>
       </c>
       <c r="C49" s="1" t="s">
-        <v>199</v>
+        <v>200</v>
       </c>
       <c r="D49" s="1" t="s">
-        <v>196</v>
+        <v>197</v>
       </c>
       <c r="E49" s="1" t="s">
-        <v>197</v>
+        <v>198</v>
       </c>
       <c r="F49" s="1">
         <v>2023</v>
       </c>
       <c r="G49" s="1" t="s">
-        <v>198</v>
+        <v>199</v>
       </c>
       <c r="H49" s="1">
         <v>2</v>
@@ -17762,19 +17779,19 @@
         <v>49</v>
       </c>
       <c r="C50" s="1" t="s">
-        <v>200</v>
+        <v>201</v>
       </c>
       <c r="D50" s="1" t="s">
-        <v>196</v>
+        <v>197</v>
       </c>
       <c r="E50" s="1" t="s">
-        <v>197</v>
+        <v>198</v>
       </c>
       <c r="F50" s="1">
         <v>2023</v>
       </c>
       <c r="G50" s="1" t="s">
-        <v>198</v>
+        <v>199</v>
       </c>
       <c r="H50" s="1">
         <v>3</v>
@@ -18068,19 +18085,19 @@
         <v>50</v>
       </c>
       <c r="C51" s="1" t="s">
-        <v>201</v>
+        <v>202</v>
       </c>
       <c r="D51" s="1" t="s">
-        <v>202</v>
+        <v>203</v>
       </c>
       <c r="E51" s="1" t="s">
-        <v>203</v>
+        <v>204</v>
       </c>
       <c r="F51" s="1">
         <v>2021</v>
       </c>
       <c r="G51" s="1" t="s">
-        <v>204</v>
+        <v>205</v>
       </c>
       <c r="H51" s="1">
         <v>1</v>
@@ -18374,19 +18391,19 @@
         <v>51</v>
       </c>
       <c r="C52" s="1" t="s">
-        <v>205</v>
+        <v>206</v>
       </c>
       <c r="D52" s="1" t="s">
-        <v>202</v>
+        <v>203</v>
       </c>
       <c r="E52" s="1" t="s">
-        <v>203</v>
+        <v>204</v>
       </c>
       <c r="F52" s="1">
         <v>2021</v>
       </c>
       <c r="G52" s="1" t="s">
-        <v>204</v>
+        <v>205</v>
       </c>
       <c r="H52" s="1">
         <v>2</v>
@@ -18680,19 +18697,19 @@
         <v>52</v>
       </c>
       <c r="C53" s="1" t="s">
-        <v>206</v>
+        <v>207</v>
       </c>
       <c r="D53" s="1" t="s">
-        <v>202</v>
+        <v>203</v>
       </c>
       <c r="E53" s="1" t="s">
-        <v>203</v>
+        <v>204</v>
       </c>
       <c r="F53" s="1">
         <v>2021</v>
       </c>
       <c r="G53" s="1" t="s">
-        <v>204</v>
+        <v>205</v>
       </c>
       <c r="H53" s="1">
         <v>3</v>
@@ -18986,19 +19003,19 @@
         <v>53</v>
       </c>
       <c r="C54" s="1" t="s">
-        <v>207</v>
+        <v>208</v>
       </c>
       <c r="D54" s="1" t="s">
-        <v>208</v>
+        <v>209</v>
       </c>
       <c r="E54" s="1" t="s">
-        <v>209</v>
+        <v>210</v>
       </c>
       <c r="F54" s="1">
         <v>2023</v>
       </c>
       <c r="G54" s="1" t="s">
-        <v>210</v>
+        <v>211</v>
       </c>
       <c r="H54" s="1">
         <v>1</v>
@@ -19292,19 +19309,19 @@
         <v>54</v>
       </c>
       <c r="C55" s="1" t="s">
-        <v>211</v>
+        <v>212</v>
       </c>
       <c r="D55" s="1" t="s">
-        <v>212</v>
+        <v>213</v>
       </c>
       <c r="E55" s="1" t="s">
-        <v>213</v>
+        <v>214</v>
       </c>
       <c r="F55" s="1">
         <v>2024</v>
       </c>
       <c r="G55" s="1" t="s">
-        <v>210</v>
+        <v>211</v>
       </c>
       <c r="H55" s="1">
         <v>1</v>
@@ -19598,19 +19615,19 @@
         <v>55</v>
       </c>
       <c r="C56" s="1" t="s">
-        <v>214</v>
+        <v>215</v>
       </c>
       <c r="D56" s="1" t="s">
-        <v>215</v>
+        <v>216</v>
       </c>
       <c r="E56" s="1" t="s">
-        <v>216</v>
+        <v>217</v>
       </c>
       <c r="F56" s="1">
         <v>2024</v>
       </c>
       <c r="G56" s="1" t="s">
-        <v>217</v>
+        <v>218</v>
       </c>
       <c r="H56" s="1">
         <v>1</v>
@@ -24325,19 +24342,19 @@
     </row>
     <row r="2" ht="15.5" spans="1:8">
       <c r="A2" s="1" t="s">
-        <v>28</v>
+        <v>29</v>
       </c>
       <c r="B2" s="1">
         <v>2019</v>
       </c>
       <c r="D2" s="3" t="s">
-        <v>28</v>
+        <v>29</v>
       </c>
       <c r="E2" s="3">
         <v>2019</v>
       </c>
       <c r="G2" s="1" t="s">
-        <v>28</v>
+        <v>29</v>
       </c>
       <c r="H2" s="1">
         <v>2019</v>
@@ -24345,19 +24362,19 @@
     </row>
     <row r="3" ht="15.5" spans="1:8">
       <c r="A3" s="1" t="s">
-        <v>28</v>
+        <v>29</v>
       </c>
       <c r="B3" s="1">
         <v>2019</v>
       </c>
       <c r="D3" s="3" t="s">
-        <v>41</v>
+        <v>42</v>
       </c>
       <c r="E3" s="3">
         <v>2020</v>
       </c>
       <c r="G3" s="1" t="s">
-        <v>28</v>
+        <v>29</v>
       </c>
       <c r="H3" s="1">
         <v>2019</v>
@@ -24365,19 +24382,19 @@
     </row>
     <row r="4" ht="15.5" spans="1:8">
       <c r="A4" s="1" t="s">
-        <v>28</v>
+        <v>29</v>
       </c>
       <c r="B4" s="1">
         <v>2019</v>
       </c>
       <c r="D4" s="3" t="s">
-        <v>49</v>
+        <v>50</v>
       </c>
       <c r="E4" s="3">
         <v>2020</v>
       </c>
       <c r="G4" s="1" t="s">
-        <v>28</v>
+        <v>29</v>
       </c>
       <c r="H4" s="1">
         <v>2019</v>
@@ -24385,19 +24402,19 @@
     </row>
     <row r="5" ht="15.5" spans="1:8">
       <c r="A5" s="1" t="s">
-        <v>28</v>
+        <v>29</v>
       </c>
       <c r="B5" s="1">
         <v>2019</v>
       </c>
       <c r="D5" s="3" t="s">
-        <v>68</v>
+        <v>69</v>
       </c>
       <c r="E5" s="3">
         <v>2020</v>
       </c>
       <c r="G5" s="1" t="s">
-        <v>28</v>
+        <v>29</v>
       </c>
       <c r="H5" s="1">
         <v>2019</v>
@@ -24405,19 +24422,19 @@
     </row>
     <row r="6" ht="15.5" hidden="1" spans="1:8">
       <c r="A6" s="1" t="s">
-        <v>41</v>
+        <v>42</v>
       </c>
       <c r="B6" s="1">
         <v>2020</v>
       </c>
       <c r="D6" s="3" t="s">
-        <v>72</v>
+        <v>73</v>
       </c>
       <c r="E6" s="3">
         <v>2020</v>
       </c>
       <c r="G6" s="1" t="s">
-        <v>41</v>
+        <v>42</v>
       </c>
       <c r="H6" s="1">
         <v>2020</v>
@@ -24425,19 +24442,19 @@
     </row>
     <row r="7" ht="15.5" hidden="1" spans="1:8">
       <c r="A7" s="1" t="s">
-        <v>49</v>
+        <v>50</v>
       </c>
       <c r="B7" s="1">
         <v>2020</v>
       </c>
       <c r="D7" s="3" t="s">
-        <v>81</v>
+        <v>82</v>
       </c>
       <c r="E7" s="3">
         <v>2019</v>
       </c>
       <c r="G7" s="1" t="s">
-        <v>49</v>
+        <v>50</v>
       </c>
       <c r="H7" s="1">
         <v>2020</v>
@@ -24445,19 +24462,19 @@
     </row>
     <row r="8" ht="15.5" hidden="1" spans="1:8">
       <c r="A8" s="1" t="s">
-        <v>56</v>
+        <v>57</v>
       </c>
       <c r="B8" s="1">
         <v>2020</v>
       </c>
       <c r="D8" s="3" t="s">
-        <v>90</v>
+        <v>91</v>
       </c>
       <c r="E8" s="3">
         <v>2018</v>
       </c>
       <c r="G8" s="1" t="s">
-        <v>56</v>
+        <v>57</v>
       </c>
       <c r="H8" s="1">
         <v>2020</v>
@@ -24465,7 +24482,7 @@
     </row>
     <row r="9" ht="15.5" hidden="1" spans="1:8">
       <c r="A9" s="1" t="s">
-        <v>62</v>
+        <v>63</v>
       </c>
       <c r="B9" s="1">
         <v>2021</v>
@@ -24477,7 +24494,7 @@
         <v>2021</v>
       </c>
       <c r="G9" s="1" t="s">
-        <v>62</v>
+        <v>63</v>
       </c>
       <c r="H9" s="1">
         <v>2021</v>
@@ -24485,19 +24502,19 @@
     </row>
     <row r="10" ht="15.5" hidden="1" spans="1:8">
       <c r="A10" s="1" t="s">
-        <v>68</v>
+        <v>69</v>
       </c>
       <c r="B10" s="1">
         <v>2020</v>
       </c>
       <c r="D10" s="3" t="s">
-        <v>101</v>
+        <v>102</v>
       </c>
       <c r="E10" s="3">
         <v>2021</v>
       </c>
       <c r="G10" s="1" t="s">
-        <v>68</v>
+        <v>69</v>
       </c>
       <c r="H10" s="1">
         <v>2020</v>
@@ -24505,19 +24522,19 @@
     </row>
     <row r="11" ht="15.5" spans="1:8">
       <c r="A11" s="1" t="s">
-        <v>72</v>
+        <v>73</v>
       </c>
       <c r="B11" s="1">
         <v>2020</v>
       </c>
       <c r="D11" s="3" t="s">
-        <v>116</v>
+        <v>117</v>
       </c>
       <c r="E11" s="3">
         <v>2022</v>
       </c>
       <c r="G11" s="1" t="s">
-        <v>72</v>
+        <v>73</v>
       </c>
       <c r="H11" s="1">
         <v>2020</v>
@@ -24525,19 +24542,19 @@
     </row>
     <row r="12" ht="15.5" spans="1:8">
       <c r="A12" s="1" t="s">
-        <v>72</v>
+        <v>73</v>
       </c>
       <c r="B12" s="1">
         <v>2020</v>
       </c>
       <c r="D12" s="3" t="s">
-        <v>124</v>
+        <v>125</v>
       </c>
       <c r="E12" s="3">
         <v>2021</v>
       </c>
       <c r="G12" s="1" t="s">
-        <v>72</v>
+        <v>73</v>
       </c>
       <c r="H12" s="1">
         <v>2020</v>
@@ -24545,19 +24562,19 @@
     </row>
     <row r="13" ht="15.5" spans="1:8">
       <c r="A13" s="1" t="s">
-        <v>81</v>
+        <v>82</v>
       </c>
       <c r="B13" s="1">
         <v>2019</v>
       </c>
       <c r="D13" s="3" t="s">
-        <v>129</v>
+        <v>130</v>
       </c>
       <c r="E13" s="3">
         <v>2023</v>
       </c>
       <c r="G13" s="1" t="s">
-        <v>81</v>
+        <v>82</v>
       </c>
       <c r="H13" s="1">
         <v>2019</v>
@@ -24565,19 +24582,19 @@
     </row>
     <row r="14" ht="15.5" spans="1:8">
       <c r="A14" s="1" t="s">
-        <v>81</v>
+        <v>82</v>
       </c>
       <c r="B14" s="1">
         <v>2019</v>
       </c>
       <c r="D14" s="3" t="s">
-        <v>135</v>
+        <v>136</v>
       </c>
       <c r="E14" s="3">
         <v>2023</v>
       </c>
       <c r="G14" s="1" t="s">
-        <v>81</v>
+        <v>82</v>
       </c>
       <c r="H14" s="1">
         <v>2019</v>
@@ -24585,19 +24602,19 @@
     </row>
     <row r="15" ht="15.5" spans="1:8">
       <c r="A15" s="1" t="s">
-        <v>90</v>
+        <v>91</v>
       </c>
       <c r="B15" s="1">
         <v>2018</v>
       </c>
       <c r="D15" s="3" t="s">
-        <v>141</v>
+        <v>142</v>
       </c>
       <c r="E15" s="3">
         <v>2014</v>
       </c>
       <c r="G15" s="1" t="s">
-        <v>90</v>
+        <v>91</v>
       </c>
       <c r="H15" s="1">
         <v>2018</v>
@@ -24605,19 +24622,19 @@
     </row>
     <row r="16" ht="15.5" spans="1:8">
       <c r="A16" s="1" t="s">
-        <v>90</v>
+        <v>91</v>
       </c>
       <c r="B16" s="1">
         <v>2018</v>
       </c>
       <c r="D16" s="3" t="s">
-        <v>145</v>
+        <v>146</v>
       </c>
       <c r="E16" s="3">
         <v>2015</v>
       </c>
       <c r="G16" s="1" t="s">
-        <v>90</v>
+        <v>91</v>
       </c>
       <c r="H16" s="1">
         <v>2018</v>
@@ -24631,7 +24648,7 @@
         <v>2021</v>
       </c>
       <c r="D17" s="3" t="s">
-        <v>149</v>
+        <v>150</v>
       </c>
       <c r="E17" s="3">
         <v>2014</v>
@@ -24645,19 +24662,19 @@
     </row>
     <row r="18" ht="15.5" spans="1:8">
       <c r="A18" s="1" t="s">
-        <v>101</v>
+        <v>102</v>
       </c>
       <c r="B18" s="1">
         <v>2021</v>
       </c>
       <c r="D18" s="3" t="s">
-        <v>164</v>
+        <v>165</v>
       </c>
       <c r="E18" s="3">
         <v>2023</v>
       </c>
       <c r="G18" s="1" t="s">
-        <v>101</v>
+        <v>102</v>
       </c>
       <c r="H18" s="1">
         <v>2021</v>
@@ -24665,19 +24682,19 @@
     </row>
     <row r="19" ht="15.5" spans="1:8">
       <c r="A19" s="1" t="s">
-        <v>101</v>
+        <v>102</v>
       </c>
       <c r="B19" s="1">
         <v>2021</v>
       </c>
       <c r="D19" s="3" t="s">
-        <v>168</v>
+        <v>169</v>
       </c>
       <c r="E19" s="3">
         <v>2023</v>
       </c>
       <c r="G19" s="1" t="s">
-        <v>101</v>
+        <v>102</v>
       </c>
       <c r="H19" s="1">
         <v>2021</v>
@@ -24685,19 +24702,19 @@
     </row>
     <row r="20" ht="15.5" spans="1:8">
       <c r="A20" s="1" t="s">
-        <v>101</v>
+        <v>102</v>
       </c>
       <c r="B20" s="1">
         <v>2021</v>
       </c>
       <c r="D20" s="3" t="s">
-        <v>172</v>
+        <v>173</v>
       </c>
       <c r="E20" s="3">
         <v>2021</v>
       </c>
       <c r="G20" s="1" t="s">
-        <v>101</v>
+        <v>102</v>
       </c>
       <c r="H20" s="1">
         <v>2021</v>
@@ -24705,19 +24722,19 @@
     </row>
     <row r="21" ht="15.5" spans="1:8">
       <c r="A21" s="1" t="s">
-        <v>116</v>
+        <v>117</v>
       </c>
       <c r="B21" s="1">
         <v>2022</v>
       </c>
       <c r="D21" s="3" t="s">
-        <v>178</v>
+        <v>179</v>
       </c>
       <c r="E21" s="3">
         <v>2023</v>
       </c>
       <c r="G21" s="1" t="s">
-        <v>116</v>
+        <v>117</v>
       </c>
       <c r="H21" s="1">
         <v>2022</v>
@@ -24725,19 +24742,19 @@
     </row>
     <row r="22" ht="15.5" spans="1:8">
       <c r="A22" s="1" t="s">
-        <v>116</v>
+        <v>117</v>
       </c>
       <c r="B22" s="1">
         <v>2022</v>
       </c>
       <c r="D22" s="3" t="s">
-        <v>181</v>
+        <v>182</v>
       </c>
       <c r="E22" s="3">
         <v>2022</v>
       </c>
       <c r="G22" s="1" t="s">
-        <v>116</v>
+        <v>117</v>
       </c>
       <c r="H22" s="1">
         <v>2022</v>
@@ -24745,19 +24762,19 @@
     </row>
     <row r="23" ht="15.5" spans="1:8">
       <c r="A23" s="1" t="s">
-        <v>116</v>
+        <v>117</v>
       </c>
       <c r="B23" s="1">
         <v>2022</v>
       </c>
       <c r="D23" s="3" t="s">
-        <v>188</v>
+        <v>189</v>
       </c>
       <c r="E23" s="3">
         <v>2022</v>
       </c>
       <c r="G23" s="1" t="s">
-        <v>116</v>
+        <v>117</v>
       </c>
       <c r="H23" s="1">
         <v>2022</v>
@@ -24765,19 +24782,19 @@
     </row>
     <row r="24" ht="15.5" hidden="1" spans="1:8">
       <c r="A24" s="1" t="s">
-        <v>124</v>
+        <v>125</v>
       </c>
       <c r="B24" s="1">
         <v>2021</v>
       </c>
       <c r="D24" s="3" t="s">
-        <v>192</v>
+        <v>193</v>
       </c>
       <c r="E24" s="3">
         <v>2020</v>
       </c>
       <c r="G24" s="1" t="s">
-        <v>124</v>
+        <v>125</v>
       </c>
       <c r="H24" s="1">
         <v>2021</v>
@@ -24785,19 +24802,19 @@
     </row>
     <row r="25" ht="15.5" hidden="1" spans="1:8">
       <c r="A25" s="1" t="s">
-        <v>129</v>
+        <v>130</v>
       </c>
       <c r="B25" s="1">
         <v>2023</v>
       </c>
       <c r="D25" s="3" t="s">
-        <v>196</v>
+        <v>197</v>
       </c>
       <c r="E25" s="3">
         <v>2023</v>
       </c>
       <c r="G25" s="1" t="s">
-        <v>129</v>
+        <v>130</v>
       </c>
       <c r="H25" s="1">
         <v>2023</v>
@@ -24805,19 +24822,19 @@
     </row>
     <row r="26" ht="15.5" hidden="1" spans="1:8">
       <c r="A26" s="1" t="s">
-        <v>135</v>
+        <v>136</v>
       </c>
       <c r="B26" s="1">
         <v>2023</v>
       </c>
       <c r="D26" s="3" t="s">
-        <v>202</v>
+        <v>203</v>
       </c>
       <c r="E26" s="3" t="s">
-        <v>218</v>
+        <v>219</v>
       </c>
       <c r="G26" s="1" t="s">
-        <v>135</v>
+        <v>136</v>
       </c>
       <c r="H26" s="1">
         <v>2023</v>
@@ -24825,13 +24842,13 @@
     </row>
     <row r="27" ht="15.5" hidden="1" spans="1:8">
       <c r="A27" s="1" t="s">
-        <v>141</v>
+        <v>142</v>
       </c>
       <c r="B27" s="1">
         <v>2014</v>
       </c>
       <c r="G27" s="1" t="s">
-        <v>141</v>
+        <v>142</v>
       </c>
       <c r="H27" s="1">
         <v>2014</v>
@@ -24839,13 +24856,13 @@
     </row>
     <row r="28" ht="15.5" spans="1:8">
       <c r="A28" s="1" t="s">
-        <v>145</v>
+        <v>146</v>
       </c>
       <c r="B28" s="1">
         <v>2015</v>
       </c>
       <c r="G28" s="1" t="s">
-        <v>145</v>
+        <v>146</v>
       </c>
       <c r="H28" s="1">
         <v>2015</v>
@@ -24853,13 +24870,13 @@
     </row>
     <row r="29" ht="15.5" spans="1:8">
       <c r="A29" s="1" t="s">
-        <v>145</v>
+        <v>146</v>
       </c>
       <c r="B29" s="1">
         <v>2015</v>
       </c>
       <c r="G29" s="1" t="s">
-        <v>145</v>
+        <v>146</v>
       </c>
       <c r="H29" s="1">
         <v>2015</v>
@@ -24867,13 +24884,13 @@
     </row>
     <row r="30" ht="15.5" spans="1:8">
       <c r="A30" s="1" t="s">
-        <v>149</v>
+        <v>150</v>
       </c>
       <c r="B30" s="1">
         <v>2014</v>
       </c>
       <c r="G30" s="1" t="s">
-        <v>149</v>
+        <v>150</v>
       </c>
       <c r="H30" s="1">
         <v>2014</v>
@@ -24881,13 +24898,13 @@
     </row>
     <row r="31" ht="15.5" spans="1:8">
       <c r="A31" s="1" t="s">
-        <v>149</v>
+        <v>150</v>
       </c>
       <c r="B31" s="1">
         <v>2014</v>
       </c>
       <c r="G31" s="1" t="s">
-        <v>149</v>
+        <v>150</v>
       </c>
       <c r="H31" s="1">
         <v>2014</v>
@@ -24895,13 +24912,13 @@
     </row>
     <row r="32" ht="15.5" spans="1:8">
       <c r="A32" s="1" t="s">
-        <v>149</v>
+        <v>150</v>
       </c>
       <c r="B32" s="1">
         <v>2014</v>
       </c>
       <c r="G32" s="1" t="s">
-        <v>149</v>
+        <v>150</v>
       </c>
       <c r="H32" s="1">
         <v>2014</v>
@@ -24909,13 +24926,13 @@
     </row>
     <row r="33" ht="15.5" spans="1:8">
       <c r="A33" s="1" t="s">
-        <v>149</v>
+        <v>150</v>
       </c>
       <c r="B33" s="1">
         <v>2014</v>
       </c>
       <c r="G33" s="1" t="s">
-        <v>149</v>
+        <v>150</v>
       </c>
       <c r="H33" s="1">
         <v>2014</v>
@@ -24923,13 +24940,13 @@
     </row>
     <row r="34" ht="15.5" hidden="1" spans="1:8">
       <c r="A34" s="1" t="s">
-        <v>164</v>
+        <v>165</v>
       </c>
       <c r="B34" s="1">
         <v>2023</v>
       </c>
       <c r="G34" s="1" t="s">
-        <v>164</v>
+        <v>165</v>
       </c>
       <c r="H34" s="1">
         <v>2023</v>
@@ -24937,13 +24954,13 @@
     </row>
     <row r="35" ht="15.5" hidden="1" spans="1:8">
       <c r="A35" s="1" t="s">
-        <v>168</v>
+        <v>169</v>
       </c>
       <c r="B35" s="1">
         <v>2023</v>
       </c>
       <c r="G35" s="1" t="s">
-        <v>168</v>
+        <v>169</v>
       </c>
       <c r="H35" s="1">
         <v>2023</v>
@@ -24951,13 +24968,13 @@
     </row>
     <row r="36" ht="15.5" hidden="1" spans="1:8">
       <c r="A36" s="1" t="s">
-        <v>172</v>
+        <v>173</v>
       </c>
       <c r="B36" s="1">
         <v>2021</v>
       </c>
       <c r="G36" s="1" t="s">
-        <v>172</v>
+        <v>173</v>
       </c>
       <c r="H36" s="1">
         <v>2021</v>
@@ -24965,13 +24982,13 @@
     </row>
     <row r="37" ht="15.5" hidden="1" spans="1:8">
       <c r="A37" s="1" t="s">
-        <v>178</v>
+        <v>179</v>
       </c>
       <c r="B37" s="1">
         <v>2023</v>
       </c>
       <c r="G37" s="1" t="s">
-        <v>178</v>
+        <v>179</v>
       </c>
       <c r="H37" s="1">
         <v>2023</v>
@@ -24979,13 +24996,13 @@
     </row>
     <row r="38" ht="15.5" spans="1:8">
       <c r="A38" s="1" t="s">
-        <v>181</v>
+        <v>182</v>
       </c>
       <c r="B38" s="1">
         <v>2022</v>
       </c>
       <c r="G38" s="1" t="s">
-        <v>181</v>
+        <v>182</v>
       </c>
       <c r="H38" s="1">
         <v>2022</v>
@@ -24993,13 +25010,13 @@
     </row>
     <row r="39" ht="15.5" spans="1:8">
       <c r="A39" s="1" t="s">
-        <v>181</v>
+        <v>182</v>
       </c>
       <c r="B39" s="1">
         <v>2022</v>
       </c>
       <c r="G39" s="1" t="s">
-        <v>181</v>
+        <v>182</v>
       </c>
       <c r="H39" s="1">
         <v>2022</v>
@@ -25007,13 +25024,13 @@
     </row>
     <row r="40" ht="15.5" hidden="1" spans="1:8">
       <c r="A40" s="1" t="s">
-        <v>188</v>
+        <v>189</v>
       </c>
       <c r="B40" s="1">
         <v>2022</v>
       </c>
       <c r="G40" s="1" t="s">
-        <v>188</v>
+        <v>189</v>
       </c>
       <c r="H40" s="1">
         <v>2022</v>
@@ -25021,13 +25038,13 @@
     </row>
     <row r="41" ht="15.5" spans="1:8">
       <c r="A41" s="1" t="s">
-        <v>192</v>
+        <v>193</v>
       </c>
       <c r="B41" s="1">
         <v>2020</v>
       </c>
       <c r="G41" s="1" t="s">
-        <v>192</v>
+        <v>193</v>
       </c>
       <c r="H41" s="1">
         <v>2020</v>
@@ -25035,13 +25052,13 @@
     </row>
     <row r="42" ht="15.5" spans="1:8">
       <c r="A42" s="1" t="s">
-        <v>192</v>
+        <v>193</v>
       </c>
       <c r="B42" s="1">
         <v>2020</v>
       </c>
       <c r="G42" s="1" t="s">
-        <v>192</v>
+        <v>193</v>
       </c>
       <c r="H42" s="1">
         <v>2020</v>
@@ -25049,13 +25066,13 @@
     </row>
     <row r="43" ht="15.5" spans="1:8">
       <c r="A43" s="1" t="s">
-        <v>192</v>
+        <v>193</v>
       </c>
       <c r="B43" s="1">
         <v>2020</v>
       </c>
       <c r="G43" s="1" t="s">
-        <v>192</v>
+        <v>193</v>
       </c>
       <c r="H43" s="1">
         <v>2020</v>
@@ -25063,13 +25080,13 @@
     </row>
     <row r="44" ht="15.5" spans="1:8">
       <c r="A44" s="1" t="s">
-        <v>196</v>
+        <v>197</v>
       </c>
       <c r="B44" s="1">
         <v>2023</v>
       </c>
       <c r="G44" s="1" t="s">
-        <v>196</v>
+        <v>197</v>
       </c>
       <c r="H44" s="1">
         <v>2023</v>
@@ -25077,13 +25094,13 @@
     </row>
     <row r="45" ht="15.5" spans="1:8">
       <c r="A45" s="1" t="s">
-        <v>196</v>
+        <v>197</v>
       </c>
       <c r="B45" s="1">
         <v>2023</v>
       </c>
       <c r="G45" s="1" t="s">
-        <v>196</v>
+        <v>197</v>
       </c>
       <c r="H45" s="1">
         <v>2023</v>
@@ -25091,13 +25108,13 @@
     </row>
     <row r="46" ht="15.5" spans="1:8">
       <c r="A46" s="1" t="s">
-        <v>196</v>
+        <v>197</v>
       </c>
       <c r="B46" s="1">
         <v>2023</v>
       </c>
       <c r="G46" s="1" t="s">
-        <v>196</v>
+        <v>197</v>
       </c>
       <c r="H46" s="1">
         <v>2023</v>
@@ -25105,13 +25122,13 @@
     </row>
     <row r="47" ht="15.5" spans="1:8">
       <c r="A47" s="1" t="s">
-        <v>202</v>
+        <v>203</v>
       </c>
       <c r="B47" s="1">
         <v>2021</v>
       </c>
       <c r="G47" s="1" t="s">
-        <v>202</v>
+        <v>203</v>
       </c>
       <c r="H47" s="1">
         <v>2021</v>
@@ -25119,13 +25136,13 @@
     </row>
     <row r="48" ht="15.5" spans="1:8">
       <c r="A48" s="1" t="s">
-        <v>202</v>
+        <v>203</v>
       </c>
       <c r="B48" s="1">
         <v>2021</v>
       </c>
       <c r="G48" s="1" t="s">
-        <v>202</v>
+        <v>203</v>
       </c>
       <c r="H48" s="1">
         <v>2021</v>
@@ -25133,13 +25150,13 @@
     </row>
     <row r="49" ht="15.5" spans="1:8">
       <c r="A49" s="1" t="s">
-        <v>202</v>
+        <v>203</v>
       </c>
       <c r="B49" s="1">
         <v>2021</v>
       </c>
       <c r="G49" s="1" t="s">
-        <v>202</v>
+        <v>203</v>
       </c>
       <c r="H49" s="1">
         <v>2021</v>
@@ -25147,13 +25164,13 @@
     </row>
     <row r="50" ht="15.5" hidden="1" spans="1:8">
       <c r="A50" s="1" t="s">
-        <v>208</v>
+        <v>209</v>
       </c>
       <c r="B50" s="1">
         <v>2023</v>
       </c>
       <c r="G50" s="1" t="s">
-        <v>208</v>
+        <v>209</v>
       </c>
       <c r="H50" s="1">
         <v>2023</v>
@@ -25161,13 +25178,13 @@
     </row>
     <row r="51" ht="15.5" hidden="1" spans="1:8">
       <c r="A51" s="1" t="s">
-        <v>212</v>
+        <v>213</v>
       </c>
       <c r="B51" s="1">
         <v>2024</v>
       </c>
       <c r="G51" s="1" t="s">
-        <v>212</v>
+        <v>213</v>
       </c>
       <c r="H51" s="1">
         <v>2024</v>
@@ -25175,13 +25192,13 @@
     </row>
     <row r="52" ht="15.5" hidden="1" spans="1:8">
       <c r="A52" s="1" t="s">
-        <v>215</v>
+        <v>216</v>
       </c>
       <c r="B52" s="1">
         <v>2024</v>
       </c>
       <c r="G52" s="1" t="s">
-        <v>215</v>
+        <v>216</v>
       </c>
       <c r="H52" s="1">
         <v>2024</v>

</xml_diff>

<commit_message>
Add new paper & Update Clean_Data and Process_Data
</commit_message>
<xml_diff>
--- a/Label.xlsx
+++ b/Label.xlsx
@@ -2258,12 +2258,12 @@
   <sheetPr/>
   <dimension ref="A1:KF72"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
-      <pane xSplit="3" ySplit="1" topLeftCell="D10" activePane="bottomRight" state="frozen"/>
+    <sheetView tabSelected="1" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
+      <pane xSplit="3" ySplit="1" topLeftCell="D18" activePane="bottomRight" state="frozen"/>
       <selection/>
       <selection pane="topRight"/>
       <selection pane="bottomLeft"/>
-      <selection pane="bottomRight" activeCell="O30" sqref="O30"/>
+      <selection pane="bottomRight" activeCell="F27" sqref="F27"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9" defaultRowHeight="14"/>

</xml_diff>

<commit_message>
Update Reports and Label
</commit_message>
<xml_diff>
--- a/Label.xlsx
+++ b/Label.xlsx
@@ -4,14 +4,15 @@
   <fileVersion appName="xl" lastEdited="3" lowestEdited="5" rupBuild="9302"/>
   <workbookPr/>
   <bookViews>
-    <workbookView windowWidth="24750" windowHeight="10480"/>
+    <workbookView windowWidth="19950" windowHeight="10480" activeTab="2"/>
   </bookViews>
   <sheets>
     <sheet name="Label" sheetId="1" r:id="rId1"/>
     <sheet name="Sheet1" sheetId="2" r:id="rId2"/>
+    <sheet name="Sheet2" sheetId="3" r:id="rId3"/>
   </sheets>
   <definedNames>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">Label!$A$1:$V$56</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">Label!$A$1:$V$52</definedName>
     <definedName name="_xlnm._FilterDatabase" localSheetId="1" hidden="1">Sheet1!$A$1:$A$68</definedName>
   </definedNames>
   <calcPr calcId="191029"/>
@@ -32,7 +33,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="703" uniqueCount="252">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="742" uniqueCount="248">
   <si>
     <t>Note</t>
   </si>
@@ -1024,12 +1025,6 @@
     <t>NeuroImage</t>
   </si>
   <si>
-    <t>Pt10E2</t>
-  </si>
-  <si>
-    <t>Pt10E3</t>
-  </si>
-  <si>
     <t>Pt13E1</t>
   </si>
   <si>
@@ -1040,12 +1035,6 @@
   </si>
   <si>
     <t>International Journal of Environmental Research and Public Health</t>
-  </si>
-  <si>
-    <t>Pt13Ea</t>
-  </si>
-  <si>
-    <t>Pt13Eb</t>
   </si>
   <si>
     <t>Pt18E1</t>
@@ -2256,14 +2245,14 @@
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:etc="http://www.wps.cn/officeDocument/2017/etCustomData">
   <sheetPr/>
-  <dimension ref="A1:KF72"/>
+  <dimension ref="A1:KF68"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
-      <pane xSplit="3" ySplit="1" topLeftCell="D18" activePane="bottomRight" state="frozen"/>
+    <sheetView workbookViewId="0">
+      <pane xSplit="3" ySplit="1" topLeftCell="D23" activePane="bottomRight" state="frozen"/>
       <selection/>
       <selection pane="topRight"/>
       <selection pane="bottomLeft"/>
-      <selection pane="bottomRight" activeCell="F27" sqref="F27"/>
+      <selection pane="bottomRight" activeCell="F1" sqref="F1:F52"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9" defaultRowHeight="14"/>
@@ -2279,11 +2268,13 @@
     <col min="9" max="10" width="9" customWidth="1"/>
     <col min="11" max="11" width="20.0833333333333" customWidth="1"/>
     <col min="12" max="12" width="21.5833333333333" customWidth="1"/>
-    <col min="13" max="13" width="11.625" customWidth="1"/>
-    <col min="14" max="16" width="13.0916666666667" customWidth="1"/>
-    <col min="17" max="17" width="13.5416666666667" customWidth="1"/>
+    <col min="13" max="13" width="11.75" customWidth="1"/>
+    <col min="14" max="14" width="13.0833333333333" customWidth="1"/>
+    <col min="15" max="15" width="14.25" customWidth="1"/>
+    <col min="16" max="16" width="12.9166666666667" customWidth="1"/>
+    <col min="17" max="17" width="13.25" customWidth="1"/>
     <col min="18" max="18" width="12.75" customWidth="1"/>
-    <col min="19" max="19" width="9" customWidth="1"/>
+    <col min="19" max="19" width="7.58333333333333" customWidth="1"/>
     <col min="20" max="20" width="41.6666666666667" customWidth="1"/>
     <col min="21" max="21" width="29" customWidth="1"/>
     <col min="23" max="23" width="13.25" customWidth="1"/>
@@ -5213,7 +5204,7 @@
         <v>5</v>
       </c>
       <c r="S10" s="1">
-        <f t="shared" ref="S10:S24" si="1">M10-R10</f>
+        <f>M10-R10</f>
         <v>51</v>
       </c>
       <c r="T10" s="1"/>
@@ -5558,7 +5549,7 @@
         <v>2</v>
       </c>
       <c r="S11" s="1">
-        <f t="shared" si="1"/>
+        <f>M11-R11</f>
         <v>24</v>
       </c>
       <c r="T11" s="1" t="s">
@@ -5903,7 +5894,7 @@
         <v>1</v>
       </c>
       <c r="S12" s="1">
-        <f t="shared" si="1"/>
+        <f>M12-R12</f>
         <v>25</v>
       </c>
       <c r="T12" s="1" t="s">
@@ -6252,7 +6243,7 @@
         <v>0</v>
       </c>
       <c r="S13" s="1">
-        <f t="shared" si="1"/>
+        <f>M13-R13</f>
         <v>103</v>
       </c>
       <c r="T13" s="1"/>
@@ -6601,7 +6592,7 @@
         <v>1</v>
       </c>
       <c r="S14" s="1">
-        <f t="shared" si="1"/>
+        <f t="shared" ref="S14:S24" si="1">M14-R14</f>
         <v>18</v>
       </c>
       <c r="T14" s="1" t="s">
@@ -18499,42 +18490,73 @@
         <v>226</v>
       </c>
       <c r="D49" s="1" t="s">
-        <v>223</v>
+        <v>227</v>
       </c>
       <c r="E49" s="1" t="s">
-        <v>224</v>
+        <v>228</v>
       </c>
       <c r="F49" s="1">
-        <v>2023</v>
+        <v>2021</v>
       </c>
       <c r="G49" s="1" t="s">
-        <v>225</v>
+        <v>229</v>
       </c>
       <c r="H49" s="1">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="I49" s="1">
-        <v>2</v>
-      </c>
-      <c r="J49" s="1"/>
-      <c r="K49" s="1"/>
-      <c r="L49" s="1"/>
-      <c r="M49" s="1"/>
-      <c r="N49" s="1"/>
-      <c r="O49" s="1"/>
-      <c r="P49" s="1"/>
-      <c r="Q49" s="1"/>
-      <c r="R49" s="1"/>
-      <c r="S49" s="1"/>
+        <v>1</v>
+      </c>
+      <c r="J49" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="K49" s="1" t="s">
+        <v>69</v>
+      </c>
+      <c r="L49" s="1" t="s">
+        <v>54</v>
+      </c>
+      <c r="M49" s="1">
+        <v>84</v>
+      </c>
+      <c r="N49" s="1" t="s">
+        <v>38</v>
+      </c>
+      <c r="O49" s="1">
+        <v>3</v>
+      </c>
+      <c r="P49" s="1">
+        <v>320</v>
+      </c>
+      <c r="Q49" s="1">
+        <v>4</v>
+      </c>
+      <c r="R49" s="1">
+        <v>0</v>
+      </c>
+      <c r="S49" s="1">
+        <v>84</v>
+      </c>
       <c r="T49" s="1"/>
       <c r="U49" s="1"/>
       <c r="V49" s="1"/>
-      <c r="W49" s="1"/>
-      <c r="Y49" s="15"/>
+      <c r="W49" s="8">
+        <v>1</v>
+      </c>
+      <c r="X49" s="15" t="s">
+        <v>98</v>
+      </c>
+      <c r="Y49" s="13">
+        <v>0</v>
+      </c>
       <c r="Z49" s="1"/>
       <c r="AA49" s="1"/>
-      <c r="AB49" s="1"/>
-      <c r="AC49" s="1"/>
+      <c r="AB49" s="1">
+        <v>13</v>
+      </c>
+      <c r="AC49" s="1">
+        <v>70</v>
+      </c>
       <c r="AD49" s="1"/>
       <c r="AE49" s="1"/>
       <c r="AF49" s="1"/>
@@ -18805,48 +18827,80 @@
         <v>49</v>
       </c>
       <c r="C50" s="1" t="s">
-        <v>227</v>
+        <v>230</v>
       </c>
       <c r="D50" s="1" t="s">
-        <v>223</v>
+        <v>231</v>
       </c>
       <c r="E50" s="1" t="s">
-        <v>224</v>
+        <v>232</v>
       </c>
       <c r="F50" s="1">
         <v>2023</v>
       </c>
       <c r="G50" s="1" t="s">
-        <v>225</v>
+        <v>233</v>
       </c>
       <c r="H50" s="1">
-        <v>3</v>
+        <v>1</v>
       </c>
       <c r="I50" s="1">
-        <v>3</v>
-      </c>
-      <c r="J50" s="1"/>
-      <c r="K50" s="1"/>
-      <c r="L50" s="1"/>
-      <c r="M50" s="1"/>
-      <c r="N50" s="1"/>
-      <c r="O50" s="1"/>
-      <c r="P50" s="1"/>
-      <c r="Q50" s="1"/>
-      <c r="R50" s="1"/>
-      <c r="S50" s="1"/>
+        <v>1</v>
+      </c>
+      <c r="J50" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="K50" s="1" t="s">
+        <v>69</v>
+      </c>
+      <c r="L50" s="1" t="s">
+        <v>54</v>
+      </c>
+      <c r="M50" s="1">
+        <v>20</v>
+      </c>
+      <c r="N50" s="1">
+        <v>12</v>
+      </c>
+      <c r="O50" s="1" t="s">
+        <v>38</v>
+      </c>
+      <c r="P50" s="1">
+        <v>960</v>
+      </c>
+      <c r="Q50" s="1">
+        <v>16</v>
+      </c>
+      <c r="R50" s="1">
+        <v>0</v>
+      </c>
+      <c r="S50" s="1">
+        <v>20</v>
+      </c>
       <c r="T50" s="1"/>
       <c r="U50" s="1"/>
       <c r="V50" s="1"/>
-      <c r="W50" s="1"/>
-      <c r="X50" s="15"/>
-      <c r="Y50" s="15"/>
+      <c r="W50" s="8">
+        <v>1</v>
+      </c>
+      <c r="X50" s="13">
+        <v>0</v>
+      </c>
+      <c r="Y50" s="8">
+        <v>1</v>
+      </c>
       <c r="Z50" s="1"/>
       <c r="AA50" s="1"/>
-      <c r="AB50" s="1"/>
-      <c r="AC50" s="1"/>
+      <c r="AB50" s="1">
+        <v>12</v>
+      </c>
+      <c r="AC50" s="1">
+        <v>8</v>
+      </c>
       <c r="AD50" s="1"/>
-      <c r="AE50" s="1"/>
+      <c r="AE50" s="19" t="s">
+        <v>234</v>
+      </c>
       <c r="AF50" s="1"/>
       <c r="AG50" s="1"/>
       <c r="AH50" s="1"/>
@@ -19115,19 +19169,19 @@
         <v>50</v>
       </c>
       <c r="C51" s="1" t="s">
-        <v>228</v>
+        <v>235</v>
       </c>
       <c r="D51" s="1" t="s">
-        <v>229</v>
+        <v>236</v>
       </c>
       <c r="E51" s="1" t="s">
-        <v>230</v>
+        <v>237</v>
       </c>
       <c r="F51" s="1">
-        <v>2021</v>
+        <v>2024</v>
       </c>
       <c r="G51" s="1" t="s">
-        <v>231</v>
+        <v>233</v>
       </c>
       <c r="H51" s="1">
         <v>1</v>
@@ -19145,25 +19199,25 @@
         <v>54</v>
       </c>
       <c r="M51" s="1">
-        <v>84</v>
-      </c>
-      <c r="N51" s="1" t="s">
-        <v>38</v>
+        <v>32</v>
+      </c>
+      <c r="N51" s="1">
+        <v>20</v>
       </c>
       <c r="O51" s="1">
-        <v>3</v>
+        <v>1</v>
       </c>
       <c r="P51" s="1">
-        <v>320</v>
+        <v>240</v>
       </c>
       <c r="Q51" s="1">
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="R51" s="1">
         <v>0</v>
       </c>
       <c r="S51" s="1">
-        <v>84</v>
+        <v>32</v>
       </c>
       <c r="T51" s="1"/>
       <c r="U51" s="1"/>
@@ -19171,22 +19225,28 @@
       <c r="W51" s="8">
         <v>1</v>
       </c>
-      <c r="X51" s="15" t="s">
-        <v>98</v>
+      <c r="X51" s="13">
+        <v>0</v>
       </c>
       <c r="Y51" s="13">
         <v>0</v>
       </c>
-      <c r="Z51" s="1"/>
-      <c r="AA51" s="1"/>
+      <c r="Z51" s="1" t="s">
+        <v>238</v>
+      </c>
+      <c r="AA51" s="1" t="s">
+        <v>239</v>
+      </c>
       <c r="AB51" s="1">
-        <v>13</v>
+        <v>5</v>
       </c>
       <c r="AC51" s="1">
-        <v>70</v>
+        <v>27</v>
       </c>
       <c r="AD51" s="1"/>
-      <c r="AE51" s="1"/>
+      <c r="AE51" s="19" t="s">
+        <v>240</v>
+      </c>
       <c r="AF51" s="1"/>
       <c r="AG51" s="1"/>
       <c r="AH51" s="1"/>
@@ -19455,48 +19515,76 @@
         <v>51</v>
       </c>
       <c r="C52" s="1" t="s">
-        <v>232</v>
+        <v>241</v>
       </c>
       <c r="D52" s="1" t="s">
-        <v>229</v>
+        <v>242</v>
       </c>
       <c r="E52" s="1" t="s">
-        <v>230</v>
+        <v>243</v>
       </c>
       <c r="F52" s="1">
-        <v>2021</v>
+        <v>2024</v>
       </c>
       <c r="G52" s="1" t="s">
-        <v>231</v>
+        <v>244</v>
       </c>
       <c r="H52" s="1">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="I52" s="1">
-        <v>2</v>
-      </c>
-      <c r="J52" s="1"/>
-      <c r="K52" s="1"/>
-      <c r="L52" s="1"/>
-      <c r="M52" s="1"/>
-      <c r="N52" s="1"/>
-      <c r="O52" s="1"/>
-      <c r="P52" s="1"/>
-      <c r="Q52" s="1"/>
+        <v>1</v>
+      </c>
+      <c r="J52" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="K52" s="1" t="s">
+        <v>245</v>
+      </c>
+      <c r="L52" s="1" t="s">
+        <v>54</v>
+      </c>
+      <c r="M52" s="1">
+        <v>70</v>
+      </c>
+      <c r="N52" s="1">
+        <v>24</v>
+      </c>
+      <c r="O52" s="1">
+        <v>1</v>
+      </c>
+      <c r="P52" s="1">
+        <v>360</v>
+      </c>
+      <c r="Q52" s="1">
+        <v>0</v>
+      </c>
       <c r="R52" s="1"/>
       <c r="S52" s="1"/>
       <c r="T52" s="1"/>
       <c r="U52" s="1"/>
       <c r="V52" s="1"/>
-      <c r="W52" s="1"/>
-      <c r="X52" s="15"/>
-      <c r="Y52" s="15"/>
+      <c r="W52" s="8">
+        <v>1</v>
+      </c>
+      <c r="X52" s="15" t="s">
+        <v>98</v>
+      </c>
+      <c r="Y52" s="8">
+        <v>1</v>
+      </c>
       <c r="Z52" s="1"/>
       <c r="AA52" s="1"/>
-      <c r="AB52" s="1"/>
-      <c r="AC52" s="1"/>
+      <c r="AB52" s="1">
+        <v>49</v>
+      </c>
+      <c r="AC52" s="1">
+        <v>21</v>
+      </c>
       <c r="AD52" s="1"/>
-      <c r="AE52" s="1"/>
+      <c r="AE52" s="17" t="s">
+        <v>246</v>
+      </c>
       <c r="AF52" s="1"/>
       <c r="AG52" s="1"/>
       <c r="AH52" s="1"/>
@@ -19759,32 +19847,16 @@
       <c r="KE52" s="1"/>
       <c r="KF52" s="1"/>
     </row>
-    <row r="53" ht="18" customHeight="1" spans="1:292">
+    <row r="53" ht="15.5" spans="1:292">
       <c r="A53" s="1"/>
-      <c r="B53" s="1">
-        <v>52</v>
-      </c>
-      <c r="C53" s="1" t="s">
-        <v>233</v>
-      </c>
-      <c r="D53" s="1" t="s">
-        <v>229</v>
-      </c>
-      <c r="E53" s="1" t="s">
-        <v>230</v>
-      </c>
-      <c r="F53" s="1">
-        <v>2021</v>
-      </c>
-      <c r="G53" s="1" t="s">
-        <v>231</v>
-      </c>
-      <c r="H53" s="1">
-        <v>3</v>
-      </c>
-      <c r="I53" s="1">
-        <v>3</v>
-      </c>
+      <c r="B53" s="1"/>
+      <c r="C53" s="1"/>
+      <c r="D53" s="1"/>
+      <c r="E53" s="1"/>
+      <c r="F53" s="1"/>
+      <c r="G53" s="1"/>
+      <c r="H53" s="1"/>
+      <c r="I53" s="1"/>
       <c r="J53" s="1"/>
       <c r="K53" s="1"/>
       <c r="L53" s="1"/>
@@ -19799,8 +19871,8 @@
       <c r="U53" s="1"/>
       <c r="V53" s="1"/>
       <c r="W53" s="1"/>
-      <c r="X53" s="15"/>
-      <c r="Y53" s="15"/>
+      <c r="X53" s="1"/>
+      <c r="Y53" s="1"/>
       <c r="Z53" s="1"/>
       <c r="AA53" s="1"/>
       <c r="AB53" s="1"/>
@@ -20071,84 +20143,36 @@
     </row>
     <row r="54" ht="15.5" spans="1:292">
       <c r="A54" s="1"/>
-      <c r="B54" s="1">
-        <v>53</v>
-      </c>
-      <c r="C54" s="1" t="s">
-        <v>234</v>
-      </c>
-      <c r="D54" s="1" t="s">
-        <v>235</v>
-      </c>
-      <c r="E54" s="1" t="s">
-        <v>236</v>
-      </c>
-      <c r="F54" s="1">
-        <v>2023</v>
-      </c>
-      <c r="G54" s="1" t="s">
-        <v>237</v>
-      </c>
-      <c r="H54" s="1">
-        <v>1</v>
-      </c>
-      <c r="I54" s="1">
-        <v>1</v>
-      </c>
-      <c r="J54" s="1" t="s">
-        <v>9</v>
-      </c>
-      <c r="K54" s="1" t="s">
-        <v>69</v>
-      </c>
-      <c r="L54" s="1" t="s">
-        <v>54</v>
-      </c>
-      <c r="M54" s="1">
-        <v>20</v>
-      </c>
-      <c r="N54" s="1">
-        <v>12</v>
-      </c>
-      <c r="O54" s="1" t="s">
-        <v>38</v>
-      </c>
-      <c r="P54" s="1">
-        <v>960</v>
-      </c>
-      <c r="Q54" s="1">
-        <v>16</v>
-      </c>
-      <c r="R54" s="1">
-        <v>0</v>
-      </c>
-      <c r="S54" s="1">
-        <v>20</v>
-      </c>
+      <c r="B54" s="1"/>
+      <c r="C54" s="1"/>
+      <c r="D54" s="1"/>
+      <c r="E54" s="1"/>
+      <c r="F54" s="1"/>
+      <c r="G54" s="1"/>
+      <c r="H54" s="1"/>
+      <c r="I54" s="1"/>
+      <c r="J54" s="1"/>
+      <c r="K54" s="1"/>
+      <c r="L54" s="1"/>
+      <c r="M54" s="1"/>
+      <c r="N54" s="1"/>
+      <c r="O54" s="1"/>
+      <c r="P54" s="1"/>
+      <c r="Q54" s="1"/>
+      <c r="R54" s="1"/>
+      <c r="S54" s="1"/>
       <c r="T54" s="1"/>
       <c r="U54" s="1"/>
       <c r="V54" s="1"/>
-      <c r="W54" s="8">
-        <v>1</v>
-      </c>
-      <c r="X54" s="13">
-        <v>0</v>
-      </c>
-      <c r="Y54" s="8">
-        <v>1</v>
-      </c>
+      <c r="W54" s="1"/>
+      <c r="X54" s="1"/>
+      <c r="Y54" s="1"/>
       <c r="Z54" s="1"/>
       <c r="AA54" s="1"/>
-      <c r="AB54" s="1">
-        <v>12</v>
-      </c>
-      <c r="AC54" s="1">
-        <v>8</v>
-      </c>
+      <c r="AB54" s="1"/>
+      <c r="AC54" s="1"/>
       <c r="AD54" s="1"/>
-      <c r="AE54" s="19" t="s">
-        <v>238</v>
-      </c>
+      <c r="AE54" s="1"/>
       <c r="AF54" s="1"/>
       <c r="AG54" s="1"/>
       <c r="AH54" s="1"/>
@@ -20413,88 +20437,36 @@
     </row>
     <row r="55" ht="15.5" spans="1:292">
       <c r="A55" s="1"/>
-      <c r="B55" s="1">
-        <v>54</v>
-      </c>
-      <c r="C55" s="1" t="s">
-        <v>239</v>
-      </c>
-      <c r="D55" s="1" t="s">
-        <v>240</v>
-      </c>
-      <c r="E55" s="1" t="s">
-        <v>241</v>
-      </c>
-      <c r="F55" s="1">
-        <v>2024</v>
-      </c>
-      <c r="G55" s="1" t="s">
-        <v>237</v>
-      </c>
-      <c r="H55" s="1">
-        <v>1</v>
-      </c>
-      <c r="I55" s="1">
-        <v>1</v>
-      </c>
-      <c r="J55" s="1" t="s">
-        <v>9</v>
-      </c>
-      <c r="K55" s="1" t="s">
-        <v>69</v>
-      </c>
-      <c r="L55" s="1" t="s">
-        <v>54</v>
-      </c>
-      <c r="M55" s="1">
-        <v>32</v>
-      </c>
-      <c r="N55" s="1">
-        <v>20</v>
-      </c>
-      <c r="O55" s="1">
-        <v>1</v>
-      </c>
-      <c r="P55" s="1">
-        <v>240</v>
-      </c>
-      <c r="Q55" s="1">
-        <v>5</v>
-      </c>
-      <c r="R55" s="1">
-        <v>0</v>
-      </c>
-      <c r="S55" s="1">
-        <v>32</v>
-      </c>
+      <c r="B55" s="1"/>
+      <c r="C55" s="1"/>
+      <c r="D55" s="1"/>
+      <c r="E55" s="1"/>
+      <c r="F55" s="1"/>
+      <c r="G55" s="1"/>
+      <c r="H55" s="1"/>
+      <c r="I55" s="1"/>
+      <c r="J55" s="1"/>
+      <c r="K55" s="1"/>
+      <c r="L55" s="1"/>
+      <c r="M55" s="1"/>
+      <c r="N55" s="1"/>
+      <c r="O55" s="1"/>
+      <c r="P55" s="1"/>
+      <c r="Q55" s="1"/>
+      <c r="R55" s="1"/>
+      <c r="S55" s="1"/>
       <c r="T55" s="1"/>
       <c r="U55" s="1"/>
       <c r="V55" s="1"/>
-      <c r="W55" s="8">
-        <v>1</v>
-      </c>
-      <c r="X55" s="13">
-        <v>0</v>
-      </c>
-      <c r="Y55" s="13">
-        <v>0</v>
-      </c>
-      <c r="Z55" s="1" t="s">
-        <v>242</v>
-      </c>
-      <c r="AA55" s="1" t="s">
-        <v>243</v>
-      </c>
-      <c r="AB55" s="1">
-        <v>5</v>
-      </c>
-      <c r="AC55" s="1">
-        <v>27</v>
-      </c>
+      <c r="W55" s="1"/>
+      <c r="X55" s="1"/>
+      <c r="Y55" s="1"/>
+      <c r="Z55" s="1"/>
+      <c r="AA55" s="1"/>
+      <c r="AB55" s="1"/>
+      <c r="AC55" s="1"/>
       <c r="AD55" s="1"/>
-      <c r="AE55" s="19" t="s">
-        <v>244</v>
-      </c>
+      <c r="AE55" s="1"/>
       <c r="AF55" s="1"/>
       <c r="AG55" s="1"/>
       <c r="AH55" s="1"/>
@@ -20759,80 +20731,36 @@
     </row>
     <row r="56" ht="15.5" spans="1:292">
       <c r="A56" s="1"/>
-      <c r="B56" s="1">
-        <v>55</v>
-      </c>
-      <c r="C56" s="1" t="s">
-        <v>245</v>
-      </c>
-      <c r="D56" s="1" t="s">
-        <v>246</v>
-      </c>
-      <c r="E56" s="1" t="s">
-        <v>247</v>
-      </c>
-      <c r="F56" s="1">
-        <v>2024</v>
-      </c>
-      <c r="G56" s="1" t="s">
-        <v>248</v>
-      </c>
-      <c r="H56" s="1">
-        <v>1</v>
-      </c>
-      <c r="I56" s="1">
-        <v>1</v>
-      </c>
-      <c r="J56" s="1" t="s">
-        <v>9</v>
-      </c>
-      <c r="K56" s="1" t="s">
-        <v>249</v>
-      </c>
-      <c r="L56" s="1" t="s">
-        <v>54</v>
-      </c>
-      <c r="M56" s="1">
-        <v>70</v>
-      </c>
-      <c r="N56" s="1">
-        <v>24</v>
-      </c>
-      <c r="O56" s="1">
-        <v>1</v>
-      </c>
-      <c r="P56" s="1">
-        <v>360</v>
-      </c>
-      <c r="Q56" s="1">
-        <v>0</v>
-      </c>
+      <c r="B56" s="1"/>
+      <c r="C56" s="1"/>
+      <c r="D56" s="1"/>
+      <c r="E56" s="1"/>
+      <c r="F56" s="1"/>
+      <c r="G56" s="1"/>
+      <c r="H56" s="1"/>
+      <c r="I56" s="1"/>
+      <c r="J56" s="1"/>
+      <c r="K56" s="1"/>
+      <c r="L56" s="1"/>
+      <c r="M56" s="1"/>
+      <c r="N56" s="1"/>
+      <c r="O56" s="1"/>
+      <c r="P56" s="1"/>
+      <c r="Q56" s="1"/>
       <c r="R56" s="1"/>
       <c r="S56" s="1"/>
       <c r="T56" s="1"/>
       <c r="U56" s="1"/>
       <c r="V56" s="1"/>
-      <c r="W56" s="8">
-        <v>1</v>
-      </c>
-      <c r="X56" s="15" t="s">
-        <v>98</v>
-      </c>
-      <c r="Y56" s="8">
-        <v>1</v>
-      </c>
+      <c r="W56" s="1"/>
+      <c r="X56" s="1"/>
+      <c r="Y56" s="1"/>
       <c r="Z56" s="1"/>
       <c r="AA56" s="1"/>
-      <c r="AB56" s="1">
-        <v>49</v>
-      </c>
-      <c r="AC56" s="1">
-        <v>21</v>
-      </c>
+      <c r="AB56" s="1"/>
+      <c r="AC56" s="1"/>
       <c r="AD56" s="1"/>
-      <c r="AE56" s="17" t="s">
-        <v>250</v>
-      </c>
+      <c r="AE56" s="1"/>
       <c r="AF56" s="1"/>
       <c r="AG56" s="1"/>
       <c r="AH56" s="1"/>
@@ -24329,7 +24257,7 @@
       <c r="KE67" s="1"/>
       <c r="KF67" s="1"/>
     </row>
-    <row r="68" ht="15.5" spans="1:292">
+    <row r="68" ht="15.5" spans="1:12">
       <c r="A68" s="1"/>
       <c r="B68" s="1"/>
       <c r="C68" s="1"/>
@@ -24342,1185 +24270,9 @@
       <c r="J68" s="1"/>
       <c r="K68" s="1"/>
       <c r="L68" s="1"/>
-      <c r="M68" s="1"/>
-      <c r="N68" s="1"/>
-      <c r="O68" s="1"/>
-      <c r="P68" s="1"/>
-      <c r="Q68" s="1"/>
-      <c r="R68" s="1"/>
-      <c r="S68" s="1"/>
-      <c r="T68" s="1"/>
-      <c r="U68" s="1"/>
-      <c r="V68" s="1"/>
-      <c r="W68" s="1"/>
-      <c r="X68" s="1"/>
-      <c r="Y68" s="1"/>
-      <c r="Z68" s="1"/>
-      <c r="AA68" s="1"/>
-      <c r="AB68" s="1"/>
-      <c r="AC68" s="1"/>
-      <c r="AD68" s="1"/>
-      <c r="AE68" s="1"/>
-      <c r="AF68" s="1"/>
-      <c r="AG68" s="1"/>
-      <c r="AH68" s="1"/>
-      <c r="AI68" s="1"/>
-      <c r="AJ68" s="1"/>
-      <c r="AK68" s="1"/>
-      <c r="AL68" s="1"/>
-      <c r="AM68" s="1"/>
-      <c r="AN68" s="1"/>
-      <c r="AO68" s="1"/>
-      <c r="AP68" s="1"/>
-      <c r="AQ68" s="1"/>
-      <c r="AR68" s="1"/>
-      <c r="AS68" s="1"/>
-      <c r="AT68" s="1"/>
-      <c r="AU68" s="1"/>
-      <c r="AV68" s="1"/>
-      <c r="AW68" s="1"/>
-      <c r="AX68" s="1"/>
-      <c r="AY68" s="1"/>
-      <c r="AZ68" s="1"/>
-      <c r="BA68" s="1"/>
-      <c r="BB68" s="1"/>
-      <c r="BC68" s="1"/>
-      <c r="BD68" s="1"/>
-      <c r="BE68" s="1"/>
-      <c r="BF68" s="1"/>
-      <c r="BG68" s="1"/>
-      <c r="BH68" s="1"/>
-      <c r="BI68" s="1"/>
-      <c r="BJ68" s="1"/>
-      <c r="BK68" s="1"/>
-      <c r="BL68" s="1"/>
-      <c r="BM68" s="1"/>
-      <c r="BN68" s="1"/>
-      <c r="BO68" s="1"/>
-      <c r="BP68" s="1"/>
-      <c r="BQ68" s="1"/>
-      <c r="BR68" s="1"/>
-      <c r="BS68" s="1"/>
-      <c r="BT68" s="1"/>
-      <c r="BU68" s="1"/>
-      <c r="BV68" s="1"/>
-      <c r="BW68" s="1"/>
-      <c r="BX68" s="1"/>
-      <c r="BY68" s="1"/>
-      <c r="BZ68" s="1"/>
-      <c r="CA68" s="1"/>
-      <c r="CB68" s="1"/>
-      <c r="CC68" s="1"/>
-      <c r="CD68" s="1"/>
-      <c r="CE68" s="1"/>
-      <c r="CF68" s="1"/>
-      <c r="CG68" s="1"/>
-      <c r="CH68" s="1"/>
-      <c r="CI68" s="1"/>
-      <c r="CJ68" s="1"/>
-      <c r="CK68" s="1"/>
-      <c r="CL68" s="1"/>
-      <c r="CM68" s="1"/>
-      <c r="CN68" s="1"/>
-      <c r="CO68" s="1"/>
-      <c r="CP68" s="1"/>
-      <c r="CQ68" s="1"/>
-      <c r="CR68" s="1"/>
-      <c r="CS68" s="1"/>
-      <c r="CT68" s="1"/>
-      <c r="CU68" s="1"/>
-      <c r="CV68" s="1"/>
-      <c r="CW68" s="1"/>
-      <c r="CX68" s="1"/>
-      <c r="CY68" s="1"/>
-      <c r="CZ68" s="1"/>
-      <c r="DA68" s="1"/>
-      <c r="DB68" s="1"/>
-      <c r="DC68" s="1"/>
-      <c r="DD68" s="1"/>
-      <c r="DE68" s="1"/>
-      <c r="DF68" s="1"/>
-      <c r="DG68" s="1"/>
-      <c r="DH68" s="1"/>
-      <c r="DI68" s="1"/>
-      <c r="DJ68" s="1"/>
-      <c r="DK68" s="1"/>
-      <c r="DL68" s="1"/>
-      <c r="DM68" s="1"/>
-      <c r="DN68" s="1"/>
-      <c r="DO68" s="1"/>
-      <c r="DP68" s="1"/>
-      <c r="DQ68" s="1"/>
-      <c r="DR68" s="1"/>
-      <c r="DS68" s="1"/>
-      <c r="DT68" s="1"/>
-      <c r="DU68" s="1"/>
-      <c r="DV68" s="1"/>
-      <c r="DW68" s="1"/>
-      <c r="DX68" s="1"/>
-      <c r="DY68" s="1"/>
-      <c r="DZ68" s="1"/>
-      <c r="EA68" s="1"/>
-      <c r="EB68" s="1"/>
-      <c r="EC68" s="1"/>
-      <c r="ED68" s="1"/>
-      <c r="EE68" s="1"/>
-      <c r="EF68" s="1"/>
-      <c r="EG68" s="1"/>
-      <c r="EH68" s="1"/>
-      <c r="EI68" s="1"/>
-      <c r="EJ68" s="1"/>
-      <c r="EK68" s="1"/>
-      <c r="EL68" s="1"/>
-      <c r="EM68" s="1"/>
-      <c r="EN68" s="1"/>
-      <c r="EO68" s="1"/>
-      <c r="EP68" s="1"/>
-      <c r="EQ68" s="1"/>
-      <c r="ER68" s="1"/>
-      <c r="ES68" s="1"/>
-      <c r="ET68" s="1"/>
-      <c r="EU68" s="1"/>
-      <c r="EV68" s="1"/>
-      <c r="EW68" s="1"/>
-      <c r="EX68" s="1"/>
-      <c r="EY68" s="1"/>
-      <c r="EZ68" s="1"/>
-      <c r="FA68" s="1"/>
-      <c r="FB68" s="1"/>
-      <c r="FC68" s="1"/>
-      <c r="FD68" s="1"/>
-      <c r="FE68" s="1"/>
-      <c r="FF68" s="1"/>
-      <c r="FG68" s="1"/>
-      <c r="FH68" s="1"/>
-      <c r="FI68" s="1"/>
-      <c r="FJ68" s="1"/>
-      <c r="FK68" s="1"/>
-      <c r="FL68" s="1"/>
-      <c r="FM68" s="1"/>
-      <c r="FN68" s="1"/>
-      <c r="FO68" s="1"/>
-      <c r="FP68" s="1"/>
-      <c r="FQ68" s="1"/>
-      <c r="FR68" s="1"/>
-      <c r="FS68" s="1"/>
-      <c r="FT68" s="1"/>
-      <c r="FU68" s="1"/>
-      <c r="FV68" s="1"/>
-      <c r="FW68" s="1"/>
-      <c r="FX68" s="1"/>
-      <c r="FY68" s="1"/>
-      <c r="FZ68" s="1"/>
-      <c r="GA68" s="1"/>
-      <c r="GB68" s="1"/>
-      <c r="GC68" s="1"/>
-      <c r="GD68" s="1"/>
-      <c r="GE68" s="1"/>
-      <c r="GF68" s="1"/>
-      <c r="GG68" s="1"/>
-      <c r="GH68" s="1"/>
-      <c r="GI68" s="1"/>
-      <c r="GJ68" s="1"/>
-      <c r="GK68" s="1"/>
-      <c r="GL68" s="1"/>
-      <c r="GM68" s="1"/>
-      <c r="GN68" s="1"/>
-      <c r="GO68" s="1"/>
-      <c r="GP68" s="1"/>
-      <c r="GQ68" s="1"/>
-      <c r="GR68" s="1"/>
-      <c r="GS68" s="1"/>
-      <c r="GT68" s="1"/>
-      <c r="GU68" s="1"/>
-      <c r="GV68" s="1"/>
-      <c r="GW68" s="1"/>
-      <c r="GX68" s="1"/>
-      <c r="GY68" s="1"/>
-      <c r="GZ68" s="1"/>
-      <c r="HA68" s="1"/>
-      <c r="HB68" s="1"/>
-      <c r="HC68" s="1"/>
-      <c r="HD68" s="1"/>
-      <c r="HE68" s="1"/>
-      <c r="HF68" s="1"/>
-      <c r="HG68" s="1"/>
-      <c r="HH68" s="1"/>
-      <c r="HI68" s="1"/>
-      <c r="HJ68" s="1"/>
-      <c r="HK68" s="1"/>
-      <c r="HL68" s="1"/>
-      <c r="HM68" s="1"/>
-      <c r="HN68" s="1"/>
-      <c r="HO68" s="1"/>
-      <c r="HP68" s="1"/>
-      <c r="HQ68" s="1"/>
-      <c r="HR68" s="1"/>
-      <c r="HS68" s="1"/>
-      <c r="HT68" s="1"/>
-      <c r="HU68" s="1"/>
-      <c r="HV68" s="1"/>
-      <c r="HW68" s="1"/>
-      <c r="HX68" s="1"/>
-      <c r="HY68" s="1"/>
-      <c r="HZ68" s="1"/>
-      <c r="IA68" s="1"/>
-      <c r="IB68" s="1"/>
-      <c r="IC68" s="1"/>
-      <c r="ID68" s="1"/>
-      <c r="IE68" s="1"/>
-      <c r="IF68" s="1"/>
-      <c r="IG68" s="1"/>
-      <c r="IH68" s="1"/>
-      <c r="II68" s="1"/>
-      <c r="IJ68" s="1"/>
-      <c r="IK68" s="1"/>
-      <c r="IL68" s="1"/>
-      <c r="IM68" s="1"/>
-      <c r="IN68" s="1"/>
-      <c r="IO68" s="1"/>
-      <c r="IP68" s="1"/>
-      <c r="IQ68" s="1"/>
-      <c r="IR68" s="1"/>
-      <c r="IS68" s="1"/>
-      <c r="IT68" s="1"/>
-      <c r="IU68" s="1"/>
-      <c r="IV68" s="1"/>
-      <c r="IW68" s="1"/>
-      <c r="IX68" s="1"/>
-      <c r="IY68" s="1"/>
-      <c r="IZ68" s="1"/>
-      <c r="JA68" s="1"/>
-      <c r="JB68" s="1"/>
-      <c r="JC68" s="1"/>
-      <c r="JD68" s="1"/>
-      <c r="JE68" s="1"/>
-      <c r="JF68" s="1"/>
-      <c r="JG68" s="1"/>
-      <c r="JH68" s="1"/>
-      <c r="JI68" s="1"/>
-      <c r="JJ68" s="1"/>
-      <c r="JK68" s="1"/>
-      <c r="JL68" s="1"/>
-      <c r="JM68" s="1"/>
-      <c r="JN68" s="1"/>
-      <c r="JO68" s="1"/>
-      <c r="JP68" s="1"/>
-      <c r="JQ68" s="1"/>
-      <c r="JR68" s="1"/>
-      <c r="JS68" s="1"/>
-      <c r="JT68" s="1"/>
-      <c r="JU68" s="1"/>
-      <c r="JV68" s="1"/>
-      <c r="JW68" s="1"/>
-      <c r="JX68" s="1"/>
-      <c r="JY68" s="1"/>
-      <c r="JZ68" s="1"/>
-      <c r="KA68" s="1"/>
-      <c r="KB68" s="1"/>
-      <c r="KC68" s="1"/>
-      <c r="KD68" s="1"/>
-      <c r="KE68" s="1"/>
-      <c r="KF68" s="1"/>
-    </row>
-    <row r="69" ht="15.5" spans="1:292">
-      <c r="A69" s="1"/>
-      <c r="B69" s="1"/>
-      <c r="C69" s="1"/>
-      <c r="D69" s="1"/>
-      <c r="E69" s="1"/>
-      <c r="F69" s="1"/>
-      <c r="G69" s="1"/>
-      <c r="H69" s="1"/>
-      <c r="I69" s="1"/>
-      <c r="J69" s="1"/>
-      <c r="K69" s="1"/>
-      <c r="L69" s="1"/>
-      <c r="M69" s="1"/>
-      <c r="N69" s="1"/>
-      <c r="O69" s="1"/>
-      <c r="P69" s="1"/>
-      <c r="Q69" s="1"/>
-      <c r="R69" s="1"/>
-      <c r="S69" s="1"/>
-      <c r="T69" s="1"/>
-      <c r="U69" s="1"/>
-      <c r="V69" s="1"/>
-      <c r="W69" s="1"/>
-      <c r="X69" s="1"/>
-      <c r="Y69" s="1"/>
-      <c r="Z69" s="1"/>
-      <c r="AA69" s="1"/>
-      <c r="AB69" s="1"/>
-      <c r="AC69" s="1"/>
-      <c r="AD69" s="1"/>
-      <c r="AE69" s="1"/>
-      <c r="AF69" s="1"/>
-      <c r="AG69" s="1"/>
-      <c r="AH69" s="1"/>
-      <c r="AI69" s="1"/>
-      <c r="AJ69" s="1"/>
-      <c r="AK69" s="1"/>
-      <c r="AL69" s="1"/>
-      <c r="AM69" s="1"/>
-      <c r="AN69" s="1"/>
-      <c r="AO69" s="1"/>
-      <c r="AP69" s="1"/>
-      <c r="AQ69" s="1"/>
-      <c r="AR69" s="1"/>
-      <c r="AS69" s="1"/>
-      <c r="AT69" s="1"/>
-      <c r="AU69" s="1"/>
-      <c r="AV69" s="1"/>
-      <c r="AW69" s="1"/>
-      <c r="AX69" s="1"/>
-      <c r="AY69" s="1"/>
-      <c r="AZ69" s="1"/>
-      <c r="BA69" s="1"/>
-      <c r="BB69" s="1"/>
-      <c r="BC69" s="1"/>
-      <c r="BD69" s="1"/>
-      <c r="BE69" s="1"/>
-      <c r="BF69" s="1"/>
-      <c r="BG69" s="1"/>
-      <c r="BH69" s="1"/>
-      <c r="BI69" s="1"/>
-      <c r="BJ69" s="1"/>
-      <c r="BK69" s="1"/>
-      <c r="BL69" s="1"/>
-      <c r="BM69" s="1"/>
-      <c r="BN69" s="1"/>
-      <c r="BO69" s="1"/>
-      <c r="BP69" s="1"/>
-      <c r="BQ69" s="1"/>
-      <c r="BR69" s="1"/>
-      <c r="BS69" s="1"/>
-      <c r="BT69" s="1"/>
-      <c r="BU69" s="1"/>
-      <c r="BV69" s="1"/>
-      <c r="BW69" s="1"/>
-      <c r="BX69" s="1"/>
-      <c r="BY69" s="1"/>
-      <c r="BZ69" s="1"/>
-      <c r="CA69" s="1"/>
-      <c r="CB69" s="1"/>
-      <c r="CC69" s="1"/>
-      <c r="CD69" s="1"/>
-      <c r="CE69" s="1"/>
-      <c r="CF69" s="1"/>
-      <c r="CG69" s="1"/>
-      <c r="CH69" s="1"/>
-      <c r="CI69" s="1"/>
-      <c r="CJ69" s="1"/>
-      <c r="CK69" s="1"/>
-      <c r="CL69" s="1"/>
-      <c r="CM69" s="1"/>
-      <c r="CN69" s="1"/>
-      <c r="CO69" s="1"/>
-      <c r="CP69" s="1"/>
-      <c r="CQ69" s="1"/>
-      <c r="CR69" s="1"/>
-      <c r="CS69" s="1"/>
-      <c r="CT69" s="1"/>
-      <c r="CU69" s="1"/>
-      <c r="CV69" s="1"/>
-      <c r="CW69" s="1"/>
-      <c r="CX69" s="1"/>
-      <c r="CY69" s="1"/>
-      <c r="CZ69" s="1"/>
-      <c r="DA69" s="1"/>
-      <c r="DB69" s="1"/>
-      <c r="DC69" s="1"/>
-      <c r="DD69" s="1"/>
-      <c r="DE69" s="1"/>
-      <c r="DF69" s="1"/>
-      <c r="DG69" s="1"/>
-      <c r="DH69" s="1"/>
-      <c r="DI69" s="1"/>
-      <c r="DJ69" s="1"/>
-      <c r="DK69" s="1"/>
-      <c r="DL69" s="1"/>
-      <c r="DM69" s="1"/>
-      <c r="DN69" s="1"/>
-      <c r="DO69" s="1"/>
-      <c r="DP69" s="1"/>
-      <c r="DQ69" s="1"/>
-      <c r="DR69" s="1"/>
-      <c r="DS69" s="1"/>
-      <c r="DT69" s="1"/>
-      <c r="DU69" s="1"/>
-      <c r="DV69" s="1"/>
-      <c r="DW69" s="1"/>
-      <c r="DX69" s="1"/>
-      <c r="DY69" s="1"/>
-      <c r="DZ69" s="1"/>
-      <c r="EA69" s="1"/>
-      <c r="EB69" s="1"/>
-      <c r="EC69" s="1"/>
-      <c r="ED69" s="1"/>
-      <c r="EE69" s="1"/>
-      <c r="EF69" s="1"/>
-      <c r="EG69" s="1"/>
-      <c r="EH69" s="1"/>
-      <c r="EI69" s="1"/>
-      <c r="EJ69" s="1"/>
-      <c r="EK69" s="1"/>
-      <c r="EL69" s="1"/>
-      <c r="EM69" s="1"/>
-      <c r="EN69" s="1"/>
-      <c r="EO69" s="1"/>
-      <c r="EP69" s="1"/>
-      <c r="EQ69" s="1"/>
-      <c r="ER69" s="1"/>
-      <c r="ES69" s="1"/>
-      <c r="ET69" s="1"/>
-      <c r="EU69" s="1"/>
-      <c r="EV69" s="1"/>
-      <c r="EW69" s="1"/>
-      <c r="EX69" s="1"/>
-      <c r="EY69" s="1"/>
-      <c r="EZ69" s="1"/>
-      <c r="FA69" s="1"/>
-      <c r="FB69" s="1"/>
-      <c r="FC69" s="1"/>
-      <c r="FD69" s="1"/>
-      <c r="FE69" s="1"/>
-      <c r="FF69" s="1"/>
-      <c r="FG69" s="1"/>
-      <c r="FH69" s="1"/>
-      <c r="FI69" s="1"/>
-      <c r="FJ69" s="1"/>
-      <c r="FK69" s="1"/>
-      <c r="FL69" s="1"/>
-      <c r="FM69" s="1"/>
-      <c r="FN69" s="1"/>
-      <c r="FO69" s="1"/>
-      <c r="FP69" s="1"/>
-      <c r="FQ69" s="1"/>
-      <c r="FR69" s="1"/>
-      <c r="FS69" s="1"/>
-      <c r="FT69" s="1"/>
-      <c r="FU69" s="1"/>
-      <c r="FV69" s="1"/>
-      <c r="FW69" s="1"/>
-      <c r="FX69" s="1"/>
-      <c r="FY69" s="1"/>
-      <c r="FZ69" s="1"/>
-      <c r="GA69" s="1"/>
-      <c r="GB69" s="1"/>
-      <c r="GC69" s="1"/>
-      <c r="GD69" s="1"/>
-      <c r="GE69" s="1"/>
-      <c r="GF69" s="1"/>
-      <c r="GG69" s="1"/>
-      <c r="GH69" s="1"/>
-      <c r="GI69" s="1"/>
-      <c r="GJ69" s="1"/>
-      <c r="GK69" s="1"/>
-      <c r="GL69" s="1"/>
-      <c r="GM69" s="1"/>
-      <c r="GN69" s="1"/>
-      <c r="GO69" s="1"/>
-      <c r="GP69" s="1"/>
-      <c r="GQ69" s="1"/>
-      <c r="GR69" s="1"/>
-      <c r="GS69" s="1"/>
-      <c r="GT69" s="1"/>
-      <c r="GU69" s="1"/>
-      <c r="GV69" s="1"/>
-      <c r="GW69" s="1"/>
-      <c r="GX69" s="1"/>
-      <c r="GY69" s="1"/>
-      <c r="GZ69" s="1"/>
-      <c r="HA69" s="1"/>
-      <c r="HB69" s="1"/>
-      <c r="HC69" s="1"/>
-      <c r="HD69" s="1"/>
-      <c r="HE69" s="1"/>
-      <c r="HF69" s="1"/>
-      <c r="HG69" s="1"/>
-      <c r="HH69" s="1"/>
-      <c r="HI69" s="1"/>
-      <c r="HJ69" s="1"/>
-      <c r="HK69" s="1"/>
-      <c r="HL69" s="1"/>
-      <c r="HM69" s="1"/>
-      <c r="HN69" s="1"/>
-      <c r="HO69" s="1"/>
-      <c r="HP69" s="1"/>
-      <c r="HQ69" s="1"/>
-      <c r="HR69" s="1"/>
-      <c r="HS69" s="1"/>
-      <c r="HT69" s="1"/>
-      <c r="HU69" s="1"/>
-      <c r="HV69" s="1"/>
-      <c r="HW69" s="1"/>
-      <c r="HX69" s="1"/>
-      <c r="HY69" s="1"/>
-      <c r="HZ69" s="1"/>
-      <c r="IA69" s="1"/>
-      <c r="IB69" s="1"/>
-      <c r="IC69" s="1"/>
-      <c r="ID69" s="1"/>
-      <c r="IE69" s="1"/>
-      <c r="IF69" s="1"/>
-      <c r="IG69" s="1"/>
-      <c r="IH69" s="1"/>
-      <c r="II69" s="1"/>
-      <c r="IJ69" s="1"/>
-      <c r="IK69" s="1"/>
-      <c r="IL69" s="1"/>
-      <c r="IM69" s="1"/>
-      <c r="IN69" s="1"/>
-      <c r="IO69" s="1"/>
-      <c r="IP69" s="1"/>
-      <c r="IQ69" s="1"/>
-      <c r="IR69" s="1"/>
-      <c r="IS69" s="1"/>
-      <c r="IT69" s="1"/>
-      <c r="IU69" s="1"/>
-      <c r="IV69" s="1"/>
-      <c r="IW69" s="1"/>
-      <c r="IX69" s="1"/>
-      <c r="IY69" s="1"/>
-      <c r="IZ69" s="1"/>
-      <c r="JA69" s="1"/>
-      <c r="JB69" s="1"/>
-      <c r="JC69" s="1"/>
-      <c r="JD69" s="1"/>
-      <c r="JE69" s="1"/>
-      <c r="JF69" s="1"/>
-      <c r="JG69" s="1"/>
-      <c r="JH69" s="1"/>
-      <c r="JI69" s="1"/>
-      <c r="JJ69" s="1"/>
-      <c r="JK69" s="1"/>
-      <c r="JL69" s="1"/>
-      <c r="JM69" s="1"/>
-      <c r="JN69" s="1"/>
-      <c r="JO69" s="1"/>
-      <c r="JP69" s="1"/>
-      <c r="JQ69" s="1"/>
-      <c r="JR69" s="1"/>
-      <c r="JS69" s="1"/>
-      <c r="JT69" s="1"/>
-      <c r="JU69" s="1"/>
-      <c r="JV69" s="1"/>
-      <c r="JW69" s="1"/>
-      <c r="JX69" s="1"/>
-      <c r="JY69" s="1"/>
-      <c r="JZ69" s="1"/>
-      <c r="KA69" s="1"/>
-      <c r="KB69" s="1"/>
-      <c r="KC69" s="1"/>
-      <c r="KD69" s="1"/>
-      <c r="KE69" s="1"/>
-      <c r="KF69" s="1"/>
-    </row>
-    <row r="70" ht="15.5" spans="1:292">
-      <c r="A70" s="1"/>
-      <c r="B70" s="1"/>
-      <c r="C70" s="1"/>
-      <c r="D70" s="1"/>
-      <c r="E70" s="1"/>
-      <c r="F70" s="1"/>
-      <c r="G70" s="1"/>
-      <c r="H70" s="1"/>
-      <c r="I70" s="1"/>
-      <c r="J70" s="1"/>
-      <c r="K70" s="1"/>
-      <c r="L70" s="1"/>
-      <c r="M70" s="1"/>
-      <c r="N70" s="1"/>
-      <c r="O70" s="1"/>
-      <c r="P70" s="1"/>
-      <c r="Q70" s="1"/>
-      <c r="R70" s="1"/>
-      <c r="S70" s="1"/>
-      <c r="T70" s="1"/>
-      <c r="U70" s="1"/>
-      <c r="V70" s="1"/>
-      <c r="W70" s="1"/>
-      <c r="X70" s="1"/>
-      <c r="Y70" s="1"/>
-      <c r="Z70" s="1"/>
-      <c r="AA70" s="1"/>
-      <c r="AB70" s="1"/>
-      <c r="AC70" s="1"/>
-      <c r="AD70" s="1"/>
-      <c r="AE70" s="1"/>
-      <c r="AF70" s="1"/>
-      <c r="AG70" s="1"/>
-      <c r="AH70" s="1"/>
-      <c r="AI70" s="1"/>
-      <c r="AJ70" s="1"/>
-      <c r="AK70" s="1"/>
-      <c r="AL70" s="1"/>
-      <c r="AM70" s="1"/>
-      <c r="AN70" s="1"/>
-      <c r="AO70" s="1"/>
-      <c r="AP70" s="1"/>
-      <c r="AQ70" s="1"/>
-      <c r="AR70" s="1"/>
-      <c r="AS70" s="1"/>
-      <c r="AT70" s="1"/>
-      <c r="AU70" s="1"/>
-      <c r="AV70" s="1"/>
-      <c r="AW70" s="1"/>
-      <c r="AX70" s="1"/>
-      <c r="AY70" s="1"/>
-      <c r="AZ70" s="1"/>
-      <c r="BA70" s="1"/>
-      <c r="BB70" s="1"/>
-      <c r="BC70" s="1"/>
-      <c r="BD70" s="1"/>
-      <c r="BE70" s="1"/>
-      <c r="BF70" s="1"/>
-      <c r="BG70" s="1"/>
-      <c r="BH70" s="1"/>
-      <c r="BI70" s="1"/>
-      <c r="BJ70" s="1"/>
-      <c r="BK70" s="1"/>
-      <c r="BL70" s="1"/>
-      <c r="BM70" s="1"/>
-      <c r="BN70" s="1"/>
-      <c r="BO70" s="1"/>
-      <c r="BP70" s="1"/>
-      <c r="BQ70" s="1"/>
-      <c r="BR70" s="1"/>
-      <c r="BS70" s="1"/>
-      <c r="BT70" s="1"/>
-      <c r="BU70" s="1"/>
-      <c r="BV70" s="1"/>
-      <c r="BW70" s="1"/>
-      <c r="BX70" s="1"/>
-      <c r="BY70" s="1"/>
-      <c r="BZ70" s="1"/>
-      <c r="CA70" s="1"/>
-      <c r="CB70" s="1"/>
-      <c r="CC70" s="1"/>
-      <c r="CD70" s="1"/>
-      <c r="CE70" s="1"/>
-      <c r="CF70" s="1"/>
-      <c r="CG70" s="1"/>
-      <c r="CH70" s="1"/>
-      <c r="CI70" s="1"/>
-      <c r="CJ70" s="1"/>
-      <c r="CK70" s="1"/>
-      <c r="CL70" s="1"/>
-      <c r="CM70" s="1"/>
-      <c r="CN70" s="1"/>
-      <c r="CO70" s="1"/>
-      <c r="CP70" s="1"/>
-      <c r="CQ70" s="1"/>
-      <c r="CR70" s="1"/>
-      <c r="CS70" s="1"/>
-      <c r="CT70" s="1"/>
-      <c r="CU70" s="1"/>
-      <c r="CV70" s="1"/>
-      <c r="CW70" s="1"/>
-      <c r="CX70" s="1"/>
-      <c r="CY70" s="1"/>
-      <c r="CZ70" s="1"/>
-      <c r="DA70" s="1"/>
-      <c r="DB70" s="1"/>
-      <c r="DC70" s="1"/>
-      <c r="DD70" s="1"/>
-      <c r="DE70" s="1"/>
-      <c r="DF70" s="1"/>
-      <c r="DG70" s="1"/>
-      <c r="DH70" s="1"/>
-      <c r="DI70" s="1"/>
-      <c r="DJ70" s="1"/>
-      <c r="DK70" s="1"/>
-      <c r="DL70" s="1"/>
-      <c r="DM70" s="1"/>
-      <c r="DN70" s="1"/>
-      <c r="DO70" s="1"/>
-      <c r="DP70" s="1"/>
-      <c r="DQ70" s="1"/>
-      <c r="DR70" s="1"/>
-      <c r="DS70" s="1"/>
-      <c r="DT70" s="1"/>
-      <c r="DU70" s="1"/>
-      <c r="DV70" s="1"/>
-      <c r="DW70" s="1"/>
-      <c r="DX70" s="1"/>
-      <c r="DY70" s="1"/>
-      <c r="DZ70" s="1"/>
-      <c r="EA70" s="1"/>
-      <c r="EB70" s="1"/>
-      <c r="EC70" s="1"/>
-      <c r="ED70" s="1"/>
-      <c r="EE70" s="1"/>
-      <c r="EF70" s="1"/>
-      <c r="EG70" s="1"/>
-      <c r="EH70" s="1"/>
-      <c r="EI70" s="1"/>
-      <c r="EJ70" s="1"/>
-      <c r="EK70" s="1"/>
-      <c r="EL70" s="1"/>
-      <c r="EM70" s="1"/>
-      <c r="EN70" s="1"/>
-      <c r="EO70" s="1"/>
-      <c r="EP70" s="1"/>
-      <c r="EQ70" s="1"/>
-      <c r="ER70" s="1"/>
-      <c r="ES70" s="1"/>
-      <c r="ET70" s="1"/>
-      <c r="EU70" s="1"/>
-      <c r="EV70" s="1"/>
-      <c r="EW70" s="1"/>
-      <c r="EX70" s="1"/>
-      <c r="EY70" s="1"/>
-      <c r="EZ70" s="1"/>
-      <c r="FA70" s="1"/>
-      <c r="FB70" s="1"/>
-      <c r="FC70" s="1"/>
-      <c r="FD70" s="1"/>
-      <c r="FE70" s="1"/>
-      <c r="FF70" s="1"/>
-      <c r="FG70" s="1"/>
-      <c r="FH70" s="1"/>
-      <c r="FI70" s="1"/>
-      <c r="FJ70" s="1"/>
-      <c r="FK70" s="1"/>
-      <c r="FL70" s="1"/>
-      <c r="FM70" s="1"/>
-      <c r="FN70" s="1"/>
-      <c r="FO70" s="1"/>
-      <c r="FP70" s="1"/>
-      <c r="FQ70" s="1"/>
-      <c r="FR70" s="1"/>
-      <c r="FS70" s="1"/>
-      <c r="FT70" s="1"/>
-      <c r="FU70" s="1"/>
-      <c r="FV70" s="1"/>
-      <c r="FW70" s="1"/>
-      <c r="FX70" s="1"/>
-      <c r="FY70" s="1"/>
-      <c r="FZ70" s="1"/>
-      <c r="GA70" s="1"/>
-      <c r="GB70" s="1"/>
-      <c r="GC70" s="1"/>
-      <c r="GD70" s="1"/>
-      <c r="GE70" s="1"/>
-      <c r="GF70" s="1"/>
-      <c r="GG70" s="1"/>
-      <c r="GH70" s="1"/>
-      <c r="GI70" s="1"/>
-      <c r="GJ70" s="1"/>
-      <c r="GK70" s="1"/>
-      <c r="GL70" s="1"/>
-      <c r="GM70" s="1"/>
-      <c r="GN70" s="1"/>
-      <c r="GO70" s="1"/>
-      <c r="GP70" s="1"/>
-      <c r="GQ70" s="1"/>
-      <c r="GR70" s="1"/>
-      <c r="GS70" s="1"/>
-      <c r="GT70" s="1"/>
-      <c r="GU70" s="1"/>
-      <c r="GV70" s="1"/>
-      <c r="GW70" s="1"/>
-      <c r="GX70" s="1"/>
-      <c r="GY70" s="1"/>
-      <c r="GZ70" s="1"/>
-      <c r="HA70" s="1"/>
-      <c r="HB70" s="1"/>
-      <c r="HC70" s="1"/>
-      <c r="HD70" s="1"/>
-      <c r="HE70" s="1"/>
-      <c r="HF70" s="1"/>
-      <c r="HG70" s="1"/>
-      <c r="HH70" s="1"/>
-      <c r="HI70" s="1"/>
-      <c r="HJ70" s="1"/>
-      <c r="HK70" s="1"/>
-      <c r="HL70" s="1"/>
-      <c r="HM70" s="1"/>
-      <c r="HN70" s="1"/>
-      <c r="HO70" s="1"/>
-      <c r="HP70" s="1"/>
-      <c r="HQ70" s="1"/>
-      <c r="HR70" s="1"/>
-      <c r="HS70" s="1"/>
-      <c r="HT70" s="1"/>
-      <c r="HU70" s="1"/>
-      <c r="HV70" s="1"/>
-      <c r="HW70" s="1"/>
-      <c r="HX70" s="1"/>
-      <c r="HY70" s="1"/>
-      <c r="HZ70" s="1"/>
-      <c r="IA70" s="1"/>
-      <c r="IB70" s="1"/>
-      <c r="IC70" s="1"/>
-      <c r="ID70" s="1"/>
-      <c r="IE70" s="1"/>
-      <c r="IF70" s="1"/>
-      <c r="IG70" s="1"/>
-      <c r="IH70" s="1"/>
-      <c r="II70" s="1"/>
-      <c r="IJ70" s="1"/>
-      <c r="IK70" s="1"/>
-      <c r="IL70" s="1"/>
-      <c r="IM70" s="1"/>
-      <c r="IN70" s="1"/>
-      <c r="IO70" s="1"/>
-      <c r="IP70" s="1"/>
-      <c r="IQ70" s="1"/>
-      <c r="IR70" s="1"/>
-      <c r="IS70" s="1"/>
-      <c r="IT70" s="1"/>
-      <c r="IU70" s="1"/>
-      <c r="IV70" s="1"/>
-      <c r="IW70" s="1"/>
-      <c r="IX70" s="1"/>
-      <c r="IY70" s="1"/>
-      <c r="IZ70" s="1"/>
-      <c r="JA70" s="1"/>
-      <c r="JB70" s="1"/>
-      <c r="JC70" s="1"/>
-      <c r="JD70" s="1"/>
-      <c r="JE70" s="1"/>
-      <c r="JF70" s="1"/>
-      <c r="JG70" s="1"/>
-      <c r="JH70" s="1"/>
-      <c r="JI70" s="1"/>
-      <c r="JJ70" s="1"/>
-      <c r="JK70" s="1"/>
-      <c r="JL70" s="1"/>
-      <c r="JM70" s="1"/>
-      <c r="JN70" s="1"/>
-      <c r="JO70" s="1"/>
-      <c r="JP70" s="1"/>
-      <c r="JQ70" s="1"/>
-      <c r="JR70" s="1"/>
-      <c r="JS70" s="1"/>
-      <c r="JT70" s="1"/>
-      <c r="JU70" s="1"/>
-      <c r="JV70" s="1"/>
-      <c r="JW70" s="1"/>
-      <c r="JX70" s="1"/>
-      <c r="JY70" s="1"/>
-      <c r="JZ70" s="1"/>
-      <c r="KA70" s="1"/>
-      <c r="KB70" s="1"/>
-      <c r="KC70" s="1"/>
-      <c r="KD70" s="1"/>
-      <c r="KE70" s="1"/>
-      <c r="KF70" s="1"/>
-    </row>
-    <row r="71" ht="15.5" spans="1:292">
-      <c r="A71" s="1"/>
-      <c r="B71" s="1"/>
-      <c r="C71" s="1"/>
-      <c r="D71" s="1"/>
-      <c r="E71" s="1"/>
-      <c r="F71" s="1"/>
-      <c r="G71" s="1"/>
-      <c r="H71" s="1"/>
-      <c r="I71" s="1"/>
-      <c r="J71" s="1"/>
-      <c r="K71" s="1"/>
-      <c r="L71" s="1"/>
-      <c r="M71" s="1"/>
-      <c r="N71" s="1"/>
-      <c r="O71" s="1"/>
-      <c r="P71" s="1"/>
-      <c r="Q71" s="1"/>
-      <c r="R71" s="1"/>
-      <c r="S71" s="1"/>
-      <c r="T71" s="1"/>
-      <c r="U71" s="1"/>
-      <c r="V71" s="1"/>
-      <c r="W71" s="1"/>
-      <c r="X71" s="1"/>
-      <c r="Y71" s="1"/>
-      <c r="Z71" s="1"/>
-      <c r="AA71" s="1"/>
-      <c r="AB71" s="1"/>
-      <c r="AC71" s="1"/>
-      <c r="AD71" s="1"/>
-      <c r="AE71" s="1"/>
-      <c r="AF71" s="1"/>
-      <c r="AG71" s="1"/>
-      <c r="AH71" s="1"/>
-      <c r="AI71" s="1"/>
-      <c r="AJ71" s="1"/>
-      <c r="AK71" s="1"/>
-      <c r="AL71" s="1"/>
-      <c r="AM71" s="1"/>
-      <c r="AN71" s="1"/>
-      <c r="AO71" s="1"/>
-      <c r="AP71" s="1"/>
-      <c r="AQ71" s="1"/>
-      <c r="AR71" s="1"/>
-      <c r="AS71" s="1"/>
-      <c r="AT71" s="1"/>
-      <c r="AU71" s="1"/>
-      <c r="AV71" s="1"/>
-      <c r="AW71" s="1"/>
-      <c r="AX71" s="1"/>
-      <c r="AY71" s="1"/>
-      <c r="AZ71" s="1"/>
-      <c r="BA71" s="1"/>
-      <c r="BB71" s="1"/>
-      <c r="BC71" s="1"/>
-      <c r="BD71" s="1"/>
-      <c r="BE71" s="1"/>
-      <c r="BF71" s="1"/>
-      <c r="BG71" s="1"/>
-      <c r="BH71" s="1"/>
-      <c r="BI71" s="1"/>
-      <c r="BJ71" s="1"/>
-      <c r="BK71" s="1"/>
-      <c r="BL71" s="1"/>
-      <c r="BM71" s="1"/>
-      <c r="BN71" s="1"/>
-      <c r="BO71" s="1"/>
-      <c r="BP71" s="1"/>
-      <c r="BQ71" s="1"/>
-      <c r="BR71" s="1"/>
-      <c r="BS71" s="1"/>
-      <c r="BT71" s="1"/>
-      <c r="BU71" s="1"/>
-      <c r="BV71" s="1"/>
-      <c r="BW71" s="1"/>
-      <c r="BX71" s="1"/>
-      <c r="BY71" s="1"/>
-      <c r="BZ71" s="1"/>
-      <c r="CA71" s="1"/>
-      <c r="CB71" s="1"/>
-      <c r="CC71" s="1"/>
-      <c r="CD71" s="1"/>
-      <c r="CE71" s="1"/>
-      <c r="CF71" s="1"/>
-      <c r="CG71" s="1"/>
-      <c r="CH71" s="1"/>
-      <c r="CI71" s="1"/>
-      <c r="CJ71" s="1"/>
-      <c r="CK71" s="1"/>
-      <c r="CL71" s="1"/>
-      <c r="CM71" s="1"/>
-      <c r="CN71" s="1"/>
-      <c r="CO71" s="1"/>
-      <c r="CP71" s="1"/>
-      <c r="CQ71" s="1"/>
-      <c r="CR71" s="1"/>
-      <c r="CS71" s="1"/>
-      <c r="CT71" s="1"/>
-      <c r="CU71" s="1"/>
-      <c r="CV71" s="1"/>
-      <c r="CW71" s="1"/>
-      <c r="CX71" s="1"/>
-      <c r="CY71" s="1"/>
-      <c r="CZ71" s="1"/>
-      <c r="DA71" s="1"/>
-      <c r="DB71" s="1"/>
-      <c r="DC71" s="1"/>
-      <c r="DD71" s="1"/>
-      <c r="DE71" s="1"/>
-      <c r="DF71" s="1"/>
-      <c r="DG71" s="1"/>
-      <c r="DH71" s="1"/>
-      <c r="DI71" s="1"/>
-      <c r="DJ71" s="1"/>
-      <c r="DK71" s="1"/>
-      <c r="DL71" s="1"/>
-      <c r="DM71" s="1"/>
-      <c r="DN71" s="1"/>
-      <c r="DO71" s="1"/>
-      <c r="DP71" s="1"/>
-      <c r="DQ71" s="1"/>
-      <c r="DR71" s="1"/>
-      <c r="DS71" s="1"/>
-      <c r="DT71" s="1"/>
-      <c r="DU71" s="1"/>
-      <c r="DV71" s="1"/>
-      <c r="DW71" s="1"/>
-      <c r="DX71" s="1"/>
-      <c r="DY71" s="1"/>
-      <c r="DZ71" s="1"/>
-      <c r="EA71" s="1"/>
-      <c r="EB71" s="1"/>
-      <c r="EC71" s="1"/>
-      <c r="ED71" s="1"/>
-      <c r="EE71" s="1"/>
-      <c r="EF71" s="1"/>
-      <c r="EG71" s="1"/>
-      <c r="EH71" s="1"/>
-      <c r="EI71" s="1"/>
-      <c r="EJ71" s="1"/>
-      <c r="EK71" s="1"/>
-      <c r="EL71" s="1"/>
-      <c r="EM71" s="1"/>
-      <c r="EN71" s="1"/>
-      <c r="EO71" s="1"/>
-      <c r="EP71" s="1"/>
-      <c r="EQ71" s="1"/>
-      <c r="ER71" s="1"/>
-      <c r="ES71" s="1"/>
-      <c r="ET71" s="1"/>
-      <c r="EU71" s="1"/>
-      <c r="EV71" s="1"/>
-      <c r="EW71" s="1"/>
-      <c r="EX71" s="1"/>
-      <c r="EY71" s="1"/>
-      <c r="EZ71" s="1"/>
-      <c r="FA71" s="1"/>
-      <c r="FB71" s="1"/>
-      <c r="FC71" s="1"/>
-      <c r="FD71" s="1"/>
-      <c r="FE71" s="1"/>
-      <c r="FF71" s="1"/>
-      <c r="FG71" s="1"/>
-      <c r="FH71" s="1"/>
-      <c r="FI71" s="1"/>
-      <c r="FJ71" s="1"/>
-      <c r="FK71" s="1"/>
-      <c r="FL71" s="1"/>
-      <c r="FM71" s="1"/>
-      <c r="FN71" s="1"/>
-      <c r="FO71" s="1"/>
-      <c r="FP71" s="1"/>
-      <c r="FQ71" s="1"/>
-      <c r="FR71" s="1"/>
-      <c r="FS71" s="1"/>
-      <c r="FT71" s="1"/>
-      <c r="FU71" s="1"/>
-      <c r="FV71" s="1"/>
-      <c r="FW71" s="1"/>
-      <c r="FX71" s="1"/>
-      <c r="FY71" s="1"/>
-      <c r="FZ71" s="1"/>
-      <c r="GA71" s="1"/>
-      <c r="GB71" s="1"/>
-      <c r="GC71" s="1"/>
-      <c r="GD71" s="1"/>
-      <c r="GE71" s="1"/>
-      <c r="GF71" s="1"/>
-      <c r="GG71" s="1"/>
-      <c r="GH71" s="1"/>
-      <c r="GI71" s="1"/>
-      <c r="GJ71" s="1"/>
-      <c r="GK71" s="1"/>
-      <c r="GL71" s="1"/>
-      <c r="GM71" s="1"/>
-      <c r="GN71" s="1"/>
-      <c r="GO71" s="1"/>
-      <c r="GP71" s="1"/>
-      <c r="GQ71" s="1"/>
-      <c r="GR71" s="1"/>
-      <c r="GS71" s="1"/>
-      <c r="GT71" s="1"/>
-      <c r="GU71" s="1"/>
-      <c r="GV71" s="1"/>
-      <c r="GW71" s="1"/>
-      <c r="GX71" s="1"/>
-      <c r="GY71" s="1"/>
-      <c r="GZ71" s="1"/>
-      <c r="HA71" s="1"/>
-      <c r="HB71" s="1"/>
-      <c r="HC71" s="1"/>
-      <c r="HD71" s="1"/>
-      <c r="HE71" s="1"/>
-      <c r="HF71" s="1"/>
-      <c r="HG71" s="1"/>
-      <c r="HH71" s="1"/>
-      <c r="HI71" s="1"/>
-      <c r="HJ71" s="1"/>
-      <c r="HK71" s="1"/>
-      <c r="HL71" s="1"/>
-      <c r="HM71" s="1"/>
-      <c r="HN71" s="1"/>
-      <c r="HO71" s="1"/>
-      <c r="HP71" s="1"/>
-      <c r="HQ71" s="1"/>
-      <c r="HR71" s="1"/>
-      <c r="HS71" s="1"/>
-      <c r="HT71" s="1"/>
-      <c r="HU71" s="1"/>
-      <c r="HV71" s="1"/>
-      <c r="HW71" s="1"/>
-      <c r="HX71" s="1"/>
-      <c r="HY71" s="1"/>
-      <c r="HZ71" s="1"/>
-      <c r="IA71" s="1"/>
-      <c r="IB71" s="1"/>
-      <c r="IC71" s="1"/>
-      <c r="ID71" s="1"/>
-      <c r="IE71" s="1"/>
-      <c r="IF71" s="1"/>
-      <c r="IG71" s="1"/>
-      <c r="IH71" s="1"/>
-      <c r="II71" s="1"/>
-      <c r="IJ71" s="1"/>
-      <c r="IK71" s="1"/>
-      <c r="IL71" s="1"/>
-      <c r="IM71" s="1"/>
-      <c r="IN71" s="1"/>
-      <c r="IO71" s="1"/>
-      <c r="IP71" s="1"/>
-      <c r="IQ71" s="1"/>
-      <c r="IR71" s="1"/>
-      <c r="IS71" s="1"/>
-      <c r="IT71" s="1"/>
-      <c r="IU71" s="1"/>
-      <c r="IV71" s="1"/>
-      <c r="IW71" s="1"/>
-      <c r="IX71" s="1"/>
-      <c r="IY71" s="1"/>
-      <c r="IZ71" s="1"/>
-      <c r="JA71" s="1"/>
-      <c r="JB71" s="1"/>
-      <c r="JC71" s="1"/>
-      <c r="JD71" s="1"/>
-      <c r="JE71" s="1"/>
-      <c r="JF71" s="1"/>
-      <c r="JG71" s="1"/>
-      <c r="JH71" s="1"/>
-      <c r="JI71" s="1"/>
-      <c r="JJ71" s="1"/>
-      <c r="JK71" s="1"/>
-      <c r="JL71" s="1"/>
-      <c r="JM71" s="1"/>
-      <c r="JN71" s="1"/>
-      <c r="JO71" s="1"/>
-      <c r="JP71" s="1"/>
-      <c r="JQ71" s="1"/>
-      <c r="JR71" s="1"/>
-      <c r="JS71" s="1"/>
-      <c r="JT71" s="1"/>
-      <c r="JU71" s="1"/>
-      <c r="JV71" s="1"/>
-      <c r="JW71" s="1"/>
-      <c r="JX71" s="1"/>
-      <c r="JY71" s="1"/>
-      <c r="JZ71" s="1"/>
-      <c r="KA71" s="1"/>
-      <c r="KB71" s="1"/>
-      <c r="KC71" s="1"/>
-      <c r="KD71" s="1"/>
-      <c r="KE71" s="1"/>
-      <c r="KF71" s="1"/>
-    </row>
-    <row r="72" ht="15.5" spans="1:12">
-      <c r="A72" s="1"/>
-      <c r="B72" s="1"/>
-      <c r="C72" s="1"/>
-      <c r="D72" s="1"/>
-      <c r="E72" s="1"/>
-      <c r="F72" s="1"/>
-      <c r="G72" s="1"/>
-      <c r="H72" s="1"/>
-      <c r="I72" s="1"/>
-      <c r="J72" s="1"/>
-      <c r="K72" s="1"/>
-      <c r="L72" s="1"/>
     </row>
   </sheetData>
-  <autoFilter xmlns:etc="http://www.wps.cn/officeDocument/2017/etCustomData" ref="A1:V56" etc:filterBottomFollowUsedRange="0">
+  <autoFilter xmlns:etc="http://www.wps.cn/officeDocument/2017/etCustomData" ref="A1:V52" etc:filterBottomFollowUsedRange="0">
     <extLst>
       <etc:autoFilterAnalysis etc:version="v1" etc:showPane="0">
         <etc:analysisCharts>
@@ -25535,7 +24287,7 @@
     </extLst>
   </autoFilter>
   <hyperlinks>
-    <hyperlink ref="G56" r:id="rId1" display="Cognitive, Affective, &amp; Behavioral Neuroscience" tooltip="https://link.springer.com/journal/13415"/>
+    <hyperlink ref="G52" r:id="rId1" display="Cognitive, Affective, &amp; Behavioral Neuroscience" tooltip="https://link.springer.com/journal/13415"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait"/>
@@ -25548,7 +24300,7 @@
   <sheetPr filterMode="1"/>
   <dimension ref="A1:H68"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
+    <sheetView topLeftCell="A83" workbookViewId="0">
       <selection activeCell="H20" sqref="H20"/>
     </sheetView>
   </sheetViews>
@@ -26068,10 +24820,10 @@
         <v>2023</v>
       </c>
       <c r="D26" s="3" t="s">
-        <v>229</v>
+        <v>227</v>
       </c>
       <c r="E26" s="3" t="s">
-        <v>251</v>
+        <v>247</v>
       </c>
       <c r="G26" s="1" t="s">
         <v>155</v>
@@ -26362,13 +25114,13 @@
     </row>
     <row r="47" ht="15.5" spans="1:8">
       <c r="A47" s="1" t="s">
-        <v>229</v>
+        <v>227</v>
       </c>
       <c r="B47" s="1">
         <v>2021</v>
       </c>
       <c r="G47" s="1" t="s">
-        <v>229</v>
+        <v>227</v>
       </c>
       <c r="H47" s="1">
         <v>2021</v>
@@ -26376,13 +25128,13 @@
     </row>
     <row r="48" ht="15.5" spans="1:8">
       <c r="A48" s="1" t="s">
-        <v>229</v>
+        <v>227</v>
       </c>
       <c r="B48" s="1">
         <v>2021</v>
       </c>
       <c r="G48" s="1" t="s">
-        <v>229</v>
+        <v>227</v>
       </c>
       <c r="H48" s="1">
         <v>2021</v>
@@ -26390,13 +25142,13 @@
     </row>
     <row r="49" ht="15.5" spans="1:8">
       <c r="A49" s="1" t="s">
-        <v>229</v>
+        <v>227</v>
       </c>
       <c r="B49" s="1">
         <v>2021</v>
       </c>
       <c r="G49" s="1" t="s">
-        <v>229</v>
+        <v>227</v>
       </c>
       <c r="H49" s="1">
         <v>2021</v>
@@ -26404,13 +25156,13 @@
     </row>
     <row r="50" ht="15.5" hidden="1" spans="1:8">
       <c r="A50" s="1" t="s">
-        <v>235</v>
+        <v>231</v>
       </c>
       <c r="B50" s="1">
         <v>2023</v>
       </c>
       <c r="G50" s="1" t="s">
-        <v>235</v>
+        <v>231</v>
       </c>
       <c r="H50" s="1">
         <v>2023</v>
@@ -26418,13 +25170,13 @@
     </row>
     <row r="51" ht="15.5" hidden="1" spans="1:8">
       <c r="A51" s="1" t="s">
-        <v>240</v>
+        <v>236</v>
       </c>
       <c r="B51" s="1">
         <v>2024</v>
       </c>
       <c r="G51" s="1" t="s">
-        <v>240</v>
+        <v>236</v>
       </c>
       <c r="H51" s="1">
         <v>2024</v>
@@ -26432,13 +25184,13 @@
     </row>
     <row r="52" ht="15.5" hidden="1" spans="1:8">
       <c r="A52" s="1" t="s">
-        <v>246</v>
+        <v>242</v>
       </c>
       <c r="B52" s="1">
         <v>2024</v>
       </c>
       <c r="G52" s="1" t="s">
-        <v>246</v>
+        <v>242</v>
       </c>
       <c r="H52" s="1">
         <v>2024</v>
@@ -26551,4 +25303,765 @@
   <headerFooter/>
   <drawing r:id="rId1"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:etc="http://www.wps.cn/officeDocument/2017/etCustomData">
+  <sheetPr/>
+  <dimension ref="A1:D56"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="A52" sqref="D1:D52 A1:A52"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultColWidth="8.66666666666667" defaultRowHeight="14" outlineLevelCol="3"/>
+  <cols>
+    <col min="2" max="2" width="11.8333333333333" customWidth="1"/>
+    <col min="3" max="3" width="11.25" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" ht="15.5" spans="1:4">
+      <c r="A1" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="B1" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="C1" t="s">
+        <v>12</v>
+      </c>
+      <c r="D1" s="1" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="2" ht="15.5" spans="1:4">
+      <c r="A2" s="1" t="s">
+        <v>33</v>
+      </c>
+      <c r="B2" s="1">
+        <v>96</v>
+      </c>
+      <c r="C2" s="1">
+        <v>28</v>
+      </c>
+      <c r="D2" s="1">
+        <v>2019</v>
+      </c>
+    </row>
+    <row r="3" ht="15.5" spans="1:4">
+      <c r="A3" s="1" t="s">
+        <v>33</v>
+      </c>
+      <c r="B3" s="1">
+        <v>96</v>
+      </c>
+      <c r="C3" s="1">
+        <v>28</v>
+      </c>
+      <c r="D3" s="1">
+        <v>2019</v>
+      </c>
+    </row>
+    <row r="4" ht="15.5" spans="1:4">
+      <c r="A4" s="1" t="s">
+        <v>33</v>
+      </c>
+      <c r="B4" s="1">
+        <v>96</v>
+      </c>
+      <c r="C4" s="1">
+        <v>28</v>
+      </c>
+      <c r="D4" s="1">
+        <v>2019</v>
+      </c>
+    </row>
+    <row r="5" ht="15.5" spans="1:4">
+      <c r="A5" s="1" t="s">
+        <v>33</v>
+      </c>
+      <c r="B5" s="1">
+        <v>80</v>
+      </c>
+      <c r="C5" s="1">
+        <v>40</v>
+      </c>
+      <c r="D5" s="1">
+        <v>2019</v>
+      </c>
+    </row>
+    <row r="6" ht="15.5" spans="1:4">
+      <c r="A6" s="1" t="s">
+        <v>50</v>
+      </c>
+      <c r="B6" s="1">
+        <v>240</v>
+      </c>
+      <c r="C6" s="1">
+        <v>92</v>
+      </c>
+      <c r="D6" s="1">
+        <v>2020</v>
+      </c>
+    </row>
+    <row r="7" ht="15.5" spans="1:4">
+      <c r="A7" s="1" t="s">
+        <v>59</v>
+      </c>
+      <c r="B7" s="1">
+        <v>312</v>
+      </c>
+      <c r="C7" s="1">
+        <v>46</v>
+      </c>
+      <c r="D7" s="1">
+        <v>2020</v>
+      </c>
+    </row>
+    <row r="8" ht="15.5" spans="1:4">
+      <c r="A8" s="1" t="s">
+        <v>66</v>
+      </c>
+      <c r="B8" s="1">
+        <v>100</v>
+      </c>
+      <c r="C8" s="1">
+        <v>31</v>
+      </c>
+      <c r="D8" s="1">
+        <v>2020</v>
+      </c>
+    </row>
+    <row r="9" ht="15.5" spans="1:4">
+      <c r="A9" s="1" t="s">
+        <v>72</v>
+      </c>
+      <c r="B9" s="1">
+        <v>960</v>
+      </c>
+      <c r="C9" s="1">
+        <v>40</v>
+      </c>
+      <c r="D9" s="1">
+        <v>2021</v>
+      </c>
+    </row>
+    <row r="10" ht="15.5" spans="1:4">
+      <c r="A10" s="1" t="s">
+        <v>78</v>
+      </c>
+      <c r="B10" s="1">
+        <v>192</v>
+      </c>
+      <c r="C10" s="1">
+        <v>56</v>
+      </c>
+      <c r="D10" s="1">
+        <v>2020</v>
+      </c>
+    </row>
+    <row r="11" ht="15.5" spans="1:4">
+      <c r="A11" s="1" t="s">
+        <v>83</v>
+      </c>
+      <c r="B11" s="1">
+        <v>144</v>
+      </c>
+      <c r="C11" s="1">
+        <v>26</v>
+      </c>
+      <c r="D11" s="1">
+        <v>2020</v>
+      </c>
+    </row>
+    <row r="12" ht="15.5" spans="1:4">
+      <c r="A12" s="1" t="s">
+        <v>83</v>
+      </c>
+      <c r="B12" s="1">
+        <v>100</v>
+      </c>
+      <c r="C12" s="1">
+        <v>26</v>
+      </c>
+      <c r="D12" s="1">
+        <v>2020</v>
+      </c>
+    </row>
+    <row r="13" ht="15.5" spans="1:4">
+      <c r="A13" s="1" t="s">
+        <v>93</v>
+      </c>
+      <c r="B13" s="1">
+        <v>144</v>
+      </c>
+      <c r="C13" s="1">
+        <v>103</v>
+      </c>
+      <c r="D13" s="1">
+        <v>2019</v>
+      </c>
+    </row>
+    <row r="14" ht="15.5" spans="1:4">
+      <c r="A14" s="1" t="s">
+        <v>103</v>
+      </c>
+      <c r="B14" s="1">
+        <v>672</v>
+      </c>
+      <c r="C14" s="1">
+        <v>19</v>
+      </c>
+      <c r="D14" s="1">
+        <v>2018</v>
+      </c>
+    </row>
+    <row r="15" ht="15.5" spans="1:4">
+      <c r="A15" s="1" t="s">
+        <v>103</v>
+      </c>
+      <c r="B15" s="1">
+        <v>672</v>
+      </c>
+      <c r="C15" s="1">
+        <v>20</v>
+      </c>
+      <c r="D15" s="1">
+        <v>2018</v>
+      </c>
+    </row>
+    <row r="16" ht="15.5" spans="1:4">
+      <c r="A16" s="1" t="s">
+        <v>109</v>
+      </c>
+      <c r="B16" s="1">
+        <v>360</v>
+      </c>
+      <c r="C16" s="1">
+        <v>30</v>
+      </c>
+      <c r="D16" s="1">
+        <v>2021</v>
+      </c>
+    </row>
+    <row r="17" ht="15.5" spans="1:4">
+      <c r="A17" s="1" t="s">
+        <v>109</v>
+      </c>
+      <c r="B17" s="1">
+        <v>360</v>
+      </c>
+      <c r="C17" s="1">
+        <v>30</v>
+      </c>
+      <c r="D17" s="1">
+        <v>2021</v>
+      </c>
+    </row>
+    <row r="18" ht="15.5" spans="1:4">
+      <c r="A18" s="1" t="s">
+        <v>115</v>
+      </c>
+      <c r="B18" s="1">
+        <v>360</v>
+      </c>
+      <c r="C18" s="1">
+        <v>13</v>
+      </c>
+      <c r="D18" s="1">
+        <v>2021</v>
+      </c>
+    </row>
+    <row r="19" ht="15.5" spans="1:4">
+      <c r="A19" s="1" t="s">
+        <v>115</v>
+      </c>
+      <c r="B19" s="1">
+        <v>360</v>
+      </c>
+      <c r="C19" s="1">
+        <v>27</v>
+      </c>
+      <c r="D19" s="1">
+        <v>2021</v>
+      </c>
+    </row>
+    <row r="20" ht="15.5" spans="1:4">
+      <c r="A20" s="1" t="s">
+        <v>115</v>
+      </c>
+      <c r="B20" s="1">
+        <v>360</v>
+      </c>
+      <c r="C20" s="1">
+        <v>27</v>
+      </c>
+      <c r="D20" s="1">
+        <v>2021</v>
+      </c>
+    </row>
+    <row r="21" ht="15.5" spans="1:4">
+      <c r="A21" s="1" t="s">
+        <v>115</v>
+      </c>
+      <c r="B21" s="1">
+        <v>360</v>
+      </c>
+      <c r="C21" s="1">
+        <v>26</v>
+      </c>
+      <c r="D21" s="1">
+        <v>2021</v>
+      </c>
+    </row>
+    <row r="22" ht="15.5" spans="1:4">
+      <c r="A22" s="1" t="s">
+        <v>124</v>
+      </c>
+      <c r="B22" s="1">
+        <v>128</v>
+      </c>
+      <c r="C22" s="1">
+        <v>38</v>
+      </c>
+      <c r="D22" s="1">
+        <v>2020</v>
+      </c>
+    </row>
+    <row r="23" ht="15.5" spans="1:4">
+      <c r="A23" s="1" t="s">
+        <v>124</v>
+      </c>
+      <c r="B23" s="1">
+        <v>240</v>
+      </c>
+      <c r="C23" s="1">
+        <v>33</v>
+      </c>
+      <c r="D23" s="1">
+        <v>2020</v>
+      </c>
+    </row>
+    <row r="24" ht="15.5" spans="1:4">
+      <c r="A24" s="1" t="s">
+        <v>124</v>
+      </c>
+      <c r="B24" s="1">
+        <v>240</v>
+      </c>
+      <c r="C24" s="1">
+        <v>36</v>
+      </c>
+      <c r="D24" s="1">
+        <v>2020</v>
+      </c>
+    </row>
+    <row r="25" ht="15.5" spans="1:4">
+      <c r="A25" s="1" t="s">
+        <v>133</v>
+      </c>
+      <c r="B25" s="1">
+        <v>200</v>
+      </c>
+      <c r="C25" s="1">
+        <v>20</v>
+      </c>
+      <c r="D25" s="1">
+        <v>2022</v>
+      </c>
+    </row>
+    <row r="26" ht="15.5" spans="1:4">
+      <c r="A26" s="1" t="s">
+        <v>133</v>
+      </c>
+      <c r="B26" s="1">
+        <v>400</v>
+      </c>
+      <c r="C26" s="1">
+        <v>24</v>
+      </c>
+      <c r="D26" s="1">
+        <v>2022</v>
+      </c>
+    </row>
+    <row r="27" ht="15.5" spans="1:4">
+      <c r="A27" s="1" t="s">
+        <v>133</v>
+      </c>
+      <c r="B27" s="1">
+        <v>400</v>
+      </c>
+      <c r="C27" s="1">
+        <v>25</v>
+      </c>
+      <c r="D27" s="1">
+        <v>2022</v>
+      </c>
+    </row>
+    <row r="28" ht="15.5" spans="1:4">
+      <c r="A28" s="1" t="s">
+        <v>144</v>
+      </c>
+      <c r="B28" s="1">
+        <v>360</v>
+      </c>
+      <c r="C28" s="1">
+        <v>105</v>
+      </c>
+      <c r="D28" s="1">
+        <v>2021</v>
+      </c>
+    </row>
+    <row r="29" ht="15.5" spans="1:4">
+      <c r="A29" s="1" t="s">
+        <v>149</v>
+      </c>
+      <c r="B29" s="1">
+        <v>64</v>
+      </c>
+      <c r="C29" s="1">
+        <v>302</v>
+      </c>
+      <c r="D29" s="1">
+        <v>2023</v>
+      </c>
+    </row>
+    <row r="30" ht="15.5" spans="1:4">
+      <c r="A30" s="1" t="s">
+        <v>155</v>
+      </c>
+      <c r="B30" s="1">
+        <v>90</v>
+      </c>
+      <c r="C30" s="1">
+        <v>23</v>
+      </c>
+      <c r="D30" s="1">
+        <v>2023</v>
+      </c>
+    </row>
+    <row r="31" ht="15.5" spans="1:4">
+      <c r="A31" s="1" t="s">
+        <v>162</v>
+      </c>
+      <c r="B31" s="1">
+        <v>40</v>
+      </c>
+      <c r="C31" s="1">
+        <v>24</v>
+      </c>
+      <c r="D31" s="1">
+        <v>2014</v>
+      </c>
+    </row>
+    <row r="32" ht="15.5" spans="1:4">
+      <c r="A32" s="1" t="s">
+        <v>165</v>
+      </c>
+      <c r="B32" s="1">
+        <v>40</v>
+      </c>
+      <c r="C32" s="1">
+        <v>20</v>
+      </c>
+      <c r="D32" s="1">
+        <v>2015</v>
+      </c>
+    </row>
+    <row r="33" ht="15.5" spans="1:4">
+      <c r="A33" s="1" t="s">
+        <v>165</v>
+      </c>
+      <c r="B33" s="1">
+        <v>40</v>
+      </c>
+      <c r="C33" s="1">
+        <v>21</v>
+      </c>
+      <c r="D33" s="1">
+        <v>2015</v>
+      </c>
+    </row>
+    <row r="34" ht="15.5" spans="1:4">
+      <c r="A34" s="1" t="s">
+        <v>169</v>
+      </c>
+      <c r="B34" s="1">
+        <v>60</v>
+      </c>
+      <c r="C34" s="1">
+        <v>24</v>
+      </c>
+      <c r="D34" s="1">
+        <v>2014</v>
+      </c>
+    </row>
+    <row r="35" ht="15.5" spans="1:4">
+      <c r="A35" s="1" t="s">
+        <v>169</v>
+      </c>
+      <c r="B35" s="1">
+        <v>60</v>
+      </c>
+      <c r="C35" s="1">
+        <v>18</v>
+      </c>
+      <c r="D35" s="1">
+        <v>2014</v>
+      </c>
+    </row>
+    <row r="36" ht="15.5" spans="1:4">
+      <c r="A36" s="1" t="s">
+        <v>169</v>
+      </c>
+      <c r="B36" s="1">
+        <v>60</v>
+      </c>
+      <c r="C36" s="1">
+        <v>22</v>
+      </c>
+      <c r="D36" s="1">
+        <v>2014</v>
+      </c>
+    </row>
+    <row r="37" ht="15.5" spans="1:4">
+      <c r="A37" s="1" t="s">
+        <v>169</v>
+      </c>
+      <c r="B37" s="1">
+        <v>60</v>
+      </c>
+      <c r="C37" s="1">
+        <v>20</v>
+      </c>
+      <c r="D37" s="1">
+        <v>2014</v>
+      </c>
+    </row>
+    <row r="38" ht="15.5" spans="1:4">
+      <c r="A38" s="1" t="s">
+        <v>184</v>
+      </c>
+      <c r="B38" s="1">
+        <v>240</v>
+      </c>
+      <c r="C38" s="1">
+        <v>40</v>
+      </c>
+      <c r="D38" s="1">
+        <v>2023</v>
+      </c>
+    </row>
+    <row r="39" ht="15.5" spans="1:4">
+      <c r="A39" s="1" t="s">
+        <v>189</v>
+      </c>
+      <c r="B39" s="1">
+        <v>60</v>
+      </c>
+      <c r="C39" s="1">
+        <v>144</v>
+      </c>
+      <c r="D39" s="1">
+        <v>2023</v>
+      </c>
+    </row>
+    <row r="40" ht="15.5" spans="1:4">
+      <c r="A40" s="1" t="s">
+        <v>193</v>
+      </c>
+      <c r="B40" s="1">
+        <v>360</v>
+      </c>
+      <c r="C40" s="1">
+        <v>109</v>
+      </c>
+      <c r="D40" s="1">
+        <v>2021</v>
+      </c>
+    </row>
+    <row r="41" ht="15.5" spans="1:4">
+      <c r="A41" s="1" t="s">
+        <v>199</v>
+      </c>
+      <c r="B41" s="1">
+        <v>300</v>
+      </c>
+      <c r="C41" s="1">
+        <v>40</v>
+      </c>
+      <c r="D41" s="1">
+        <v>2023</v>
+      </c>
+    </row>
+    <row r="42" ht="15.5" spans="1:4">
+      <c r="A42" s="1" t="s">
+        <v>203</v>
+      </c>
+      <c r="B42" s="1">
+        <v>240</v>
+      </c>
+      <c r="C42" s="1">
+        <v>30</v>
+      </c>
+      <c r="D42" s="1">
+        <v>2022</v>
+      </c>
+    </row>
+    <row r="43" ht="15.5" spans="1:4">
+      <c r="A43" s="1" t="s">
+        <v>203</v>
+      </c>
+      <c r="B43" s="1">
+        <v>240</v>
+      </c>
+      <c r="C43" s="1">
+        <v>104</v>
+      </c>
+      <c r="D43" s="1">
+        <v>2022</v>
+      </c>
+    </row>
+    <row r="44" ht="15.5" spans="1:4">
+      <c r="A44" s="1" t="s">
+        <v>213</v>
+      </c>
+      <c r="B44" s="1">
+        <v>360</v>
+      </c>
+      <c r="C44" s="1">
+        <v>328</v>
+      </c>
+      <c r="D44" s="1">
+        <v>2022</v>
+      </c>
+    </row>
+    <row r="45" ht="15.5" spans="1:4">
+      <c r="A45" s="1" t="s">
+        <v>217</v>
+      </c>
+      <c r="B45" s="1">
+        <v>360</v>
+      </c>
+      <c r="C45" s="1">
+        <v>23</v>
+      </c>
+      <c r="D45" s="1">
+        <v>2020</v>
+      </c>
+    </row>
+    <row r="46" ht="15.5" spans="1:4">
+      <c r="A46" s="1" t="s">
+        <v>217</v>
+      </c>
+      <c r="B46" s="1">
+        <v>360</v>
+      </c>
+      <c r="C46" s="1">
+        <v>21</v>
+      </c>
+      <c r="D46" s="1">
+        <v>2020</v>
+      </c>
+    </row>
+    <row r="47" ht="15.5" spans="1:4">
+      <c r="A47" s="1" t="s">
+        <v>217</v>
+      </c>
+      <c r="B47" s="1">
+        <v>360</v>
+      </c>
+      <c r="C47" s="1">
+        <v>18</v>
+      </c>
+      <c r="D47" s="1">
+        <v>2020</v>
+      </c>
+    </row>
+    <row r="48" ht="15.5" spans="1:4">
+      <c r="A48" s="1" t="s">
+        <v>223</v>
+      </c>
+      <c r="B48" s="1">
+        <v>96</v>
+      </c>
+      <c r="C48" s="1">
+        <v>380</v>
+      </c>
+      <c r="D48" s="1">
+        <v>2023</v>
+      </c>
+    </row>
+    <row r="49" ht="15.5" spans="1:4">
+      <c r="A49" s="1" t="s">
+        <v>227</v>
+      </c>
+      <c r="B49" s="1">
+        <v>320</v>
+      </c>
+      <c r="C49" s="1">
+        <v>84</v>
+      </c>
+      <c r="D49" s="1">
+        <v>2021</v>
+      </c>
+    </row>
+    <row r="50" ht="15.5" spans="1:4">
+      <c r="A50" s="1" t="s">
+        <v>231</v>
+      </c>
+      <c r="B50" s="1">
+        <v>960</v>
+      </c>
+      <c r="C50" s="1">
+        <v>20</v>
+      </c>
+      <c r="D50" s="1">
+        <v>2023</v>
+      </c>
+    </row>
+    <row r="51" ht="15.5" spans="1:4">
+      <c r="A51" s="1" t="s">
+        <v>236</v>
+      </c>
+      <c r="B51" s="1">
+        <v>240</v>
+      </c>
+      <c r="C51" s="1">
+        <v>32</v>
+      </c>
+      <c r="D51" s="1">
+        <v>2024</v>
+      </c>
+    </row>
+    <row r="52" ht="15.5" spans="1:4">
+      <c r="A52" s="1" t="s">
+        <v>242</v>
+      </c>
+      <c r="B52" s="1">
+        <v>360</v>
+      </c>
+      <c r="C52" s="1">
+        <v>70</v>
+      </c>
+      <c r="D52" s="1">
+        <v>2024</v>
+      </c>
+    </row>
+    <row r="53" ht="15.5" spans="1:1">
+      <c r="A53" s="1"/>
+    </row>
+    <row r="54" ht="15.5" spans="1:1">
+      <c r="A54" s="1"/>
+    </row>
+    <row r="55" ht="15.5" spans="1:1">
+      <c r="A55" s="1"/>
+    </row>
+    <row r="56" ht="15.5" spans="1:1">
+      <c r="A56" s="1"/>
+    </row>
+  </sheetData>
+  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+  <headerFooter/>
+</worksheet>
 </file>
</xml_diff>

<commit_message>
Update Process_Data_v2 and Draw_pic_v2
</commit_message>
<xml_diff>
--- a/Label.xlsx
+++ b/Label.xlsx
@@ -1029,7 +1029,7 @@
     <t>E-prime 3</t>
   </si>
   <si>
-    <t xml:space="preserve"> Spanish</t>
+    <t>Spanish</t>
   </si>
   <si>
     <t>2(match:matching,non-matching)*3(labelcondition:you,friend,stranger)</t>
@@ -1057,6 +1057,12 @@
   </si>
   <si>
     <r>
+      <rPr>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="Times New Roman"/>
+        <charset val="134"/>
+      </rPr>
       <t>2(Group:Autism,Neuro</t>
     </r>
     <r>
@@ -2166,7 +2172,7 @@
     <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
       <pane xSplit="5" topLeftCell="AB1" activePane="topRight" state="frozen"/>
       <selection/>
-      <selection pane="topRight" activeCell="AH52" sqref="AH52"/>
+      <selection pane="topRight" activeCell="AD52" sqref="AD52"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9" defaultRowHeight="14"/>

</xml_diff>

<commit_message>
Update Process_Data_v2 and Label
</commit_message>
<xml_diff>
--- a/Label.xlsx
+++ b/Label.xlsx
@@ -30,7 +30,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="819" uniqueCount="380">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="839" uniqueCount="390">
   <si>
     <t>Note</t>
   </si>
@@ -1035,6 +1035,9 @@
     <t>Psychological Medicine</t>
   </si>
   <si>
+    <t>Bath</t>
+  </si>
+  <si>
     <t>Hobbs_2023_PM</t>
   </si>
   <si>
@@ -1115,9 +1118,18 @@
     </r>
   </si>
   <si>
+    <t>Beijing</t>
+  </si>
+  <si>
     <t>Liang_2021_HBM</t>
   </si>
   <si>
+    <t>https://osf.io/u9ty6/?view_only=9bdbbaf95f9a4d9c8bc53dd1a29563ae.</t>
+  </si>
+  <si>
+    <t>This is an open access article under the terms of the Creative Commons Attribution-NonCommercial-NoDerivs License, which permits use and distribution in any medium, provided the original work is properly cited, the use is non-commercial and no modifications or adaptations are made.</t>
+  </si>
+  <si>
     <t>Non-trial level</t>
   </si>
   <si>
@@ -1157,6 +1169,12 @@
     <t>PsychoPy3</t>
   </si>
   <si>
+    <t>Italy</t>
+  </si>
+  <si>
+    <t>Padova</t>
+  </si>
+  <si>
     <t>Italian</t>
   </si>
   <si>
@@ -1166,6 +1184,9 @@
     <t>Vicovaro_2022_EPHPP</t>
   </si>
   <si>
+    <t>https://doi.org/10.17605/OSF.IO/FE3JW</t>
+  </si>
+  <si>
     <t>Pt6E2</t>
   </si>
   <si>
@@ -1190,9 +1211,15 @@
     <t>BMC Psychology</t>
   </si>
   <si>
+    <t>Clayton</t>
+  </si>
+  <si>
     <t>Perrykkad_2022_BMC</t>
   </si>
   <si>
+    <t>https://doi.org/10.26180/20011142</t>
+  </si>
+  <si>
     <t>Pt9E1</t>
   </si>
   <si>
@@ -1209,6 +1236,9 @@
   </si>
   <si>
     <t>Wozniak_2022_PR</t>
+  </si>
+  <si>
+    <t>https://osf.io/35wp9</t>
   </si>
   <si>
     <t>Pt9E2</t>
@@ -2040,7 +2070,7 @@
       <alignment vertical="center"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="21">
+  <cellXfs count="22">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0">
       <alignment vertical="center"/>
     </xf>
@@ -2102,6 +2132,9 @@
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="6" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
@@ -2430,10 +2463,10 @@
   <sheetPr/>
   <dimension ref="A1:KK68"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="76" zoomScaleNormal="76" topLeftCell="A16" workbookViewId="0">
-      <pane xSplit="5" topLeftCell="AA1" activePane="topRight" state="frozen"/>
+    <sheetView tabSelected="1" zoomScale="76" zoomScaleNormal="76" topLeftCell="A35" workbookViewId="0">
+      <pane xSplit="5" topLeftCell="Z1" activePane="topRight" state="frozen"/>
       <selection/>
-      <selection pane="topRight" activeCell="AK39" sqref="AK39"/>
+      <selection pane="topRight" activeCell="AE47" sqref="AE47"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9" defaultRowHeight="14"/>
@@ -15963,8 +15996,12 @@
         <v>0</v>
       </c>
       <c r="AC39" s="2"/>
-      <c r="AD39" s="2"/>
-      <c r="AE39" s="2"/>
+      <c r="AD39" s="2" t="s">
+        <v>71</v>
+      </c>
+      <c r="AE39" s="2" t="s">
+        <v>297</v>
+      </c>
       <c r="AF39" s="2" t="s">
         <v>61</v>
       </c>
@@ -15977,13 +16014,13 @@
       <c r="AI39" s="2"/>
       <c r="AJ39" s="2"/>
       <c r="AK39" s="2" t="s">
-        <v>297</v>
-      </c>
-      <c r="AL39" s="4" t="s">
         <v>298</v>
       </c>
+      <c r="AL39" s="9" t="s">
+        <v>299</v>
+      </c>
       <c r="AM39" s="2" t="s">
-        <v>299</v>
+        <v>300</v>
       </c>
       <c r="AN39" s="2"/>
       <c r="AO39" s="2"/>
@@ -16244,28 +16281,28 @@
       <c r="KJ39" s="2"/>
       <c r="KK39" s="2"/>
     </row>
-    <row r="40" ht="15.5" spans="1:297">
+    <row r="40" ht="62" spans="1:297">
       <c r="A40" s="2"/>
       <c r="B40" s="2">
         <v>39</v>
       </c>
       <c r="C40" s="2" t="s">
-        <v>300</v>
+        <v>301</v>
       </c>
       <c r="D40" s="2" t="s">
-        <v>301</v>
+        <v>302</v>
       </c>
       <c r="E40" s="5" t="s">
         <v>64</v>
       </c>
       <c r="F40" s="2" t="s">
-        <v>302</v>
+        <v>303</v>
       </c>
       <c r="G40" s="4" t="s">
-        <v>303</v>
+        <v>304</v>
       </c>
       <c r="H40" s="2" t="s">
-        <v>304</v>
+        <v>305</v>
       </c>
       <c r="I40" s="2">
         <v>2021</v>
@@ -16311,10 +16348,10 @@
         <v>108</v>
       </c>
       <c r="W40" s="2" t="s">
-        <v>305</v>
+        <v>306</v>
       </c>
       <c r="X40" s="2" t="s">
-        <v>306</v>
+        <v>307</v>
       </c>
       <c r="Y40" s="2"/>
       <c r="Z40" s="15">
@@ -16323,14 +16360,18 @@
       <c r="AA40" s="17">
         <v>0</v>
       </c>
-      <c r="AB40" s="17">
-        <v>0</v>
+      <c r="AB40" s="15">
+        <v>1</v>
       </c>
       <c r="AC40" s="2" t="s">
         <v>109</v>
       </c>
-      <c r="AD40" s="2"/>
-      <c r="AE40" s="2"/>
+      <c r="AD40" s="2" t="s">
+        <v>84</v>
+      </c>
+      <c r="AE40" s="2" t="s">
+        <v>308</v>
+      </c>
       <c r="AF40" s="2" t="s">
         <v>61</v>
       </c>
@@ -16343,10 +16384,14 @@
       <c r="AI40" s="2"/>
       <c r="AJ40" s="2"/>
       <c r="AK40" s="2" t="s">
-        <v>307</v>
-      </c>
-      <c r="AL40" s="2"/>
-      <c r="AM40" s="2"/>
+        <v>309</v>
+      </c>
+      <c r="AL40" s="9" t="s">
+        <v>310</v>
+      </c>
+      <c r="AM40" s="21" t="s">
+        <v>311</v>
+      </c>
       <c r="AN40" s="2"/>
       <c r="AO40" s="2"/>
       <c r="AP40" s="2"/>
@@ -16608,22 +16653,22 @@
     </row>
     <row r="41" ht="15.5" spans="1:297">
       <c r="A41" s="6" t="s">
-        <v>308</v>
+        <v>312</v>
       </c>
       <c r="B41" s="2">
         <v>40</v>
       </c>
       <c r="C41" s="2" t="s">
-        <v>309</v>
+        <v>313</v>
       </c>
       <c r="D41" s="2" t="s">
-        <v>310</v>
+        <v>314</v>
       </c>
       <c r="E41" s="2"/>
       <c r="F41" s="2"/>
       <c r="G41" s="4"/>
       <c r="H41" s="2" t="s">
-        <v>311</v>
+        <v>315</v>
       </c>
       <c r="I41" s="2">
         <v>2023</v>
@@ -16694,7 +16739,7 @@
       </c>
       <c r="AI41" s="2"/>
       <c r="AJ41" s="2" t="s">
-        <v>312</v>
+        <v>316</v>
       </c>
       <c r="AK41" s="2"/>
       <c r="AL41" s="2"/>
@@ -16964,28 +17009,28 @@
         <v>41</v>
       </c>
       <c r="C42" s="2" t="s">
-        <v>313</v>
+        <v>317</v>
       </c>
       <c r="D42" s="2" t="s">
-        <v>314</v>
+        <v>318</v>
       </c>
       <c r="E42" s="5" t="s">
         <v>64</v>
       </c>
       <c r="F42" s="2" t="s">
-        <v>315</v>
+        <v>319</v>
       </c>
       <c r="G42" s="4" t="s">
-        <v>316</v>
+        <v>320</v>
       </c>
       <c r="H42" s="2" t="s">
-        <v>317</v>
+        <v>321</v>
       </c>
       <c r="I42" s="2">
         <v>2022</v>
       </c>
       <c r="J42" s="2" t="s">
-        <v>318</v>
+        <v>322</v>
       </c>
       <c r="K42" s="2">
         <v>1</v>
@@ -17023,7 +17068,7 @@
         <v>27</v>
       </c>
       <c r="W42" s="2" t="s">
-        <v>319</v>
+        <v>323</v>
       </c>
       <c r="X42" s="2"/>
       <c r="Y42" s="2"/>
@@ -17037,12 +17082,16 @@
         <v>0</v>
       </c>
       <c r="AC42" s="2" t="s">
-        <v>320</v>
-      </c>
-      <c r="AD42" s="2"/>
-      <c r="AE42" s="2"/>
+        <v>324</v>
+      </c>
+      <c r="AD42" s="2" t="s">
+        <v>325</v>
+      </c>
+      <c r="AE42" s="2" t="s">
+        <v>326</v>
+      </c>
       <c r="AF42" s="2" t="s">
-        <v>321</v>
+        <v>327</v>
       </c>
       <c r="AG42" s="2">
         <v>14</v>
@@ -17052,13 +17101,17 @@
       </c>
       <c r="AI42" s="2"/>
       <c r="AJ42" s="2" t="s">
-        <v>322</v>
+        <v>328</v>
       </c>
       <c r="AK42" s="2" t="s">
-        <v>323</v>
-      </c>
-      <c r="AL42" s="2"/>
-      <c r="AM42" s="2"/>
+        <v>329</v>
+      </c>
+      <c r="AL42" s="4" t="s">
+        <v>330</v>
+      </c>
+      <c r="AM42" s="2" t="s">
+        <v>290</v>
+      </c>
       <c r="AN42" s="2"/>
       <c r="AO42" s="2"/>
       <c r="AP42" s="2"/>
@@ -17324,10 +17377,10 @@
         <v>42</v>
       </c>
       <c r="C43" s="2" t="s">
-        <v>324</v>
+        <v>331</v>
       </c>
       <c r="D43" s="2" t="s">
-        <v>314</v>
+        <v>318</v>
       </c>
       <c r="E43" s="5" t="s">
         <v>64</v>
@@ -17335,13 +17388,13 @@
       <c r="F43" s="2"/>
       <c r="G43" s="4"/>
       <c r="H43" s="2" t="s">
-        <v>317</v>
+        <v>321</v>
       </c>
       <c r="I43" s="2">
         <v>2022</v>
       </c>
       <c r="J43" s="2" t="s">
-        <v>318</v>
+        <v>322</v>
       </c>
       <c r="K43" s="2">
         <v>2</v>
@@ -17379,7 +17432,7 @@
         <v>102</v>
       </c>
       <c r="W43" s="2" t="s">
-        <v>319</v>
+        <v>323</v>
       </c>
       <c r="X43" s="2"/>
       <c r="Y43" s="2"/>
@@ -17393,12 +17446,16 @@
         <v>0</v>
       </c>
       <c r="AC43" s="2" t="s">
-        <v>320</v>
-      </c>
-      <c r="AD43" s="2"/>
-      <c r="AE43" s="2"/>
+        <v>324</v>
+      </c>
+      <c r="AD43" s="2" t="s">
+        <v>325</v>
+      </c>
+      <c r="AE43" s="2" t="s">
+        <v>326</v>
+      </c>
       <c r="AF43" s="2" t="s">
-        <v>321</v>
+        <v>327</v>
       </c>
       <c r="AG43" s="2">
         <v>14</v>
@@ -17408,13 +17465,17 @@
       </c>
       <c r="AI43" s="2"/>
       <c r="AJ43" s="2" t="s">
-        <v>322</v>
+        <v>328</v>
       </c>
       <c r="AK43" s="2" t="s">
-        <v>323</v>
-      </c>
-      <c r="AL43" s="2"/>
-      <c r="AM43" s="2"/>
+        <v>329</v>
+      </c>
+      <c r="AL43" s="4" t="s">
+        <v>330</v>
+      </c>
+      <c r="AM43" s="2" t="s">
+        <v>290</v>
+      </c>
       <c r="AN43" s="2"/>
       <c r="AO43" s="2"/>
       <c r="AP43" s="2"/>
@@ -17676,34 +17737,34 @@
     </row>
     <row r="44" ht="15.5" spans="1:297">
       <c r="A44" s="2" t="s">
-        <v>325</v>
+        <v>332</v>
       </c>
       <c r="B44" s="2">
         <v>43</v>
       </c>
       <c r="C44" s="2" t="s">
-        <v>326</v>
+        <v>333</v>
       </c>
       <c r="D44" s="2" t="s">
-        <v>327</v>
+        <v>334</v>
       </c>
       <c r="E44" s="5" t="s">
         <v>64</v>
       </c>
       <c r="F44" s="7" t="s">
-        <v>328</v>
+        <v>335</v>
       </c>
       <c r="G44" s="4" t="s">
-        <v>329</v>
+        <v>336</v>
       </c>
       <c r="H44" s="2" t="s">
-        <v>330</v>
+        <v>337</v>
       </c>
       <c r="I44" s="2">
         <v>2022</v>
       </c>
       <c r="J44" s="2" t="s">
-        <v>331</v>
+        <v>338</v>
       </c>
       <c r="K44" s="2">
         <v>1</v>
@@ -17748,8 +17809,8 @@
       <c r="Z44" s="15">
         <v>1</v>
       </c>
-      <c r="AA44" s="18" t="s">
-        <v>108</v>
+      <c r="AA44" s="15">
+        <v>1</v>
       </c>
       <c r="AB44" s="17">
         <v>0</v>
@@ -17757,8 +17818,12 @@
       <c r="AC44" s="2" t="s">
         <v>83</v>
       </c>
-      <c r="AD44" s="2"/>
-      <c r="AE44" s="2"/>
+      <c r="AD44" s="2" t="s">
+        <v>162</v>
+      </c>
+      <c r="AE44" s="2" t="s">
+        <v>339</v>
+      </c>
       <c r="AF44" s="2" t="s">
         <v>61</v>
       </c>
@@ -17769,10 +17834,14 @@
       </c>
       <c r="AJ44" s="2"/>
       <c r="AK44" s="2" t="s">
-        <v>332</v>
-      </c>
-      <c r="AL44" s="2"/>
-      <c r="AM44" s="2"/>
+        <v>340</v>
+      </c>
+      <c r="AL44" s="9" t="s">
+        <v>341</v>
+      </c>
+      <c r="AM44" s="2" t="s">
+        <v>300</v>
+      </c>
       <c r="AN44" s="2"/>
       <c r="AO44" s="2"/>
       <c r="AP44" s="2"/>
@@ -18038,17 +18107,17 @@
         <v>44</v>
       </c>
       <c r="C45" s="2" t="s">
-        <v>333</v>
+        <v>342</v>
       </c>
       <c r="D45" s="2" t="s">
-        <v>334</v>
+        <v>343</v>
       </c>
       <c r="E45" s="2"/>
       <c r="F45" s="2" t="s">
         <v>157</v>
       </c>
       <c r="G45" s="4" t="s">
-        <v>335</v>
+        <v>344</v>
       </c>
       <c r="H45" s="2" t="s">
         <v>159</v>
@@ -18109,7 +18178,7 @@
         <v>0</v>
       </c>
       <c r="AC45" s="2" t="s">
-        <v>336</v>
+        <v>345</v>
       </c>
       <c r="AD45" s="2"/>
       <c r="AE45" s="2"/>
@@ -18124,12 +18193,14 @@
       </c>
       <c r="AI45" s="2"/>
       <c r="AJ45" s="2" t="s">
-        <v>337</v>
+        <v>346</v>
       </c>
       <c r="AK45" s="2" t="s">
-        <v>338</v>
-      </c>
-      <c r="AL45" s="2"/>
+        <v>347</v>
+      </c>
+      <c r="AL45" s="4" t="s">
+        <v>348</v>
+      </c>
       <c r="AM45" s="2"/>
       <c r="AN45" s="2"/>
       <c r="AO45" s="2"/>
@@ -18396,10 +18467,10 @@
         <v>45</v>
       </c>
       <c r="C46" s="2" t="s">
-        <v>339</v>
+        <v>349</v>
       </c>
       <c r="D46" s="2" t="s">
-        <v>334</v>
+        <v>343</v>
       </c>
       <c r="E46" s="2"/>
       <c r="F46" s="2"/>
@@ -18463,7 +18534,7 @@
         <v>0</v>
       </c>
       <c r="AC46" s="2" t="s">
-        <v>336</v>
+        <v>345</v>
       </c>
       <c r="AD46" s="2"/>
       <c r="AE46" s="2"/>
@@ -18478,12 +18549,14 @@
       </c>
       <c r="AI46" s="2"/>
       <c r="AJ46" s="2" t="s">
-        <v>337</v>
+        <v>346</v>
       </c>
       <c r="AK46" s="2" t="s">
-        <v>338</v>
-      </c>
-      <c r="AL46" s="2"/>
+        <v>347</v>
+      </c>
+      <c r="AL46" s="4" t="s">
+        <v>348</v>
+      </c>
       <c r="AM46" s="2"/>
       <c r="AN46" s="2"/>
       <c r="AO46" s="2"/>
@@ -18750,10 +18823,10 @@
         <v>46</v>
       </c>
       <c r="C47" s="2" t="s">
-        <v>340</v>
+        <v>350</v>
       </c>
       <c r="D47" s="2" t="s">
-        <v>334</v>
+        <v>343</v>
       </c>
       <c r="E47" s="2"/>
       <c r="F47" s="2"/>
@@ -18817,7 +18890,7 @@
         <v>0</v>
       </c>
       <c r="AC47" s="2" t="s">
-        <v>336</v>
+        <v>345</v>
       </c>
       <c r="AD47" s="2"/>
       <c r="AE47" s="2"/>
@@ -18832,12 +18905,14 @@
       </c>
       <c r="AI47" s="2"/>
       <c r="AJ47" s="2" t="s">
-        <v>337</v>
+        <v>346</v>
       </c>
       <c r="AK47" s="2" t="s">
-        <v>338</v>
-      </c>
-      <c r="AL47" s="2"/>
+        <v>347</v>
+      </c>
+      <c r="AL47" s="4" t="s">
+        <v>348</v>
+      </c>
       <c r="AM47" s="2"/>
       <c r="AN47" s="2"/>
       <c r="AO47" s="2"/>
@@ -19104,28 +19179,28 @@
         <v>47</v>
       </c>
       <c r="C48" s="2" t="s">
-        <v>341</v>
+        <v>351</v>
       </c>
       <c r="D48" s="2" t="s">
-        <v>342</v>
+        <v>352</v>
       </c>
       <c r="E48" s="5" t="s">
         <v>64</v>
       </c>
       <c r="F48" s="8" t="s">
-        <v>302</v>
+        <v>303</v>
       </c>
       <c r="G48" s="4" t="s">
-        <v>303</v>
+        <v>304</v>
       </c>
       <c r="H48" s="2" t="s">
-        <v>343</v>
+        <v>353</v>
       </c>
       <c r="I48" s="2">
         <v>2023</v>
       </c>
       <c r="J48" s="2" t="s">
-        <v>344</v>
+        <v>354</v>
       </c>
       <c r="K48" s="2">
         <v>1</v>
@@ -19189,7 +19264,7 @@
       </c>
       <c r="AJ48" s="2"/>
       <c r="AK48" s="2" t="s">
-        <v>345</v>
+        <v>355</v>
       </c>
       <c r="AL48" s="2"/>
       <c r="AM48" s="2"/>
@@ -19458,28 +19533,28 @@
         <v>48</v>
       </c>
       <c r="C49" s="2" t="s">
-        <v>346</v>
+        <v>356</v>
       </c>
       <c r="D49" s="2" t="s">
-        <v>347</v>
+        <v>357</v>
       </c>
       <c r="E49" s="5" t="s">
         <v>64</v>
       </c>
       <c r="F49" s="2" t="s">
-        <v>348</v>
+        <v>358</v>
       </c>
       <c r="G49" s="4" t="s">
-        <v>349</v>
+        <v>359</v>
       </c>
       <c r="H49" s="2" t="s">
-        <v>350</v>
+        <v>360</v>
       </c>
       <c r="I49" s="2">
         <v>2021</v>
       </c>
       <c r="J49" s="2" t="s">
-        <v>351</v>
+        <v>361</v>
       </c>
       <c r="K49" s="2">
         <v>1</v>
@@ -19542,7 +19617,7 @@
       <c r="AI49" s="2"/>
       <c r="AJ49" s="2"/>
       <c r="AK49" s="2" t="s">
-        <v>352</v>
+        <v>362</v>
       </c>
       <c r="AL49" s="2"/>
       <c r="AM49" s="2"/>
@@ -19811,28 +19886,28 @@
         <v>49</v>
       </c>
       <c r="C50" s="2" t="s">
-        <v>353</v>
+        <v>363</v>
       </c>
       <c r="D50" s="2" t="s">
-        <v>354</v>
+        <v>364</v>
       </c>
       <c r="E50" s="5" t="s">
         <v>64</v>
       </c>
       <c r="F50" s="8" t="s">
-        <v>355</v>
+        <v>365</v>
       </c>
       <c r="G50" s="9" t="s">
-        <v>356</v>
+        <v>366</v>
       </c>
       <c r="H50" s="2" t="s">
-        <v>357</v>
+        <v>367</v>
       </c>
       <c r="I50" s="2">
         <v>2023</v>
       </c>
       <c r="J50" s="2" t="s">
-        <v>358</v>
+        <v>368</v>
       </c>
       <c r="K50" s="2">
         <v>1</v>
@@ -19894,10 +19969,10 @@
       </c>
       <c r="AI50" s="2"/>
       <c r="AJ50" s="2" t="s">
-        <v>359</v>
+        <v>369</v>
       </c>
       <c r="AK50" s="2" t="s">
-        <v>360</v>
+        <v>370</v>
       </c>
       <c r="AL50" s="2"/>
       <c r="AM50" s="2"/>
@@ -20166,28 +20241,28 @@
         <v>50</v>
       </c>
       <c r="C51" s="2" t="s">
-        <v>361</v>
+        <v>371</v>
       </c>
       <c r="D51" s="2" t="s">
-        <v>362</v>
+        <v>372</v>
       </c>
       <c r="E51" s="5" t="s">
         <v>64</v>
       </c>
       <c r="F51" s="8" t="s">
-        <v>363</v>
+        <v>373</v>
       </c>
       <c r="G51" s="4" t="s">
-        <v>364</v>
+        <v>374</v>
       </c>
       <c r="H51" s="2" t="s">
-        <v>365</v>
+        <v>375</v>
       </c>
       <c r="I51" s="2">
         <v>2024</v>
       </c>
       <c r="J51" s="2" t="s">
-        <v>358</v>
+        <v>368</v>
       </c>
       <c r="K51" s="2">
         <v>1</v>
@@ -20238,12 +20313,12 @@
         <v>0</v>
       </c>
       <c r="AC51" s="2" t="s">
-        <v>366</v>
+        <v>376</v>
       </c>
       <c r="AD51" s="2"/>
       <c r="AE51" s="2"/>
       <c r="AF51" s="2" t="s">
-        <v>367</v>
+        <v>377</v>
       </c>
       <c r="AG51" s="2">
         <v>5</v>
@@ -20253,10 +20328,10 @@
       </c>
       <c r="AI51" s="2"/>
       <c r="AJ51" s="2" t="s">
-        <v>368</v>
+        <v>378</v>
       </c>
       <c r="AK51" s="2" t="s">
-        <v>369</v>
+        <v>379</v>
       </c>
       <c r="AL51" s="2"/>
       <c r="AM51" s="2"/>
@@ -20525,28 +20600,28 @@
         <v>51</v>
       </c>
       <c r="C52" s="2" t="s">
-        <v>370</v>
+        <v>380</v>
       </c>
       <c r="D52" s="2" t="s">
-        <v>371</v>
+        <v>381</v>
       </c>
       <c r="E52" s="5" t="s">
         <v>64</v>
       </c>
       <c r="F52" s="2" t="s">
-        <v>372</v>
+        <v>382</v>
       </c>
       <c r="G52" s="4" t="s">
-        <v>373</v>
+        <v>383</v>
       </c>
       <c r="H52" s="2" t="s">
-        <v>374</v>
+        <v>384</v>
       </c>
       <c r="I52" s="2">
         <v>2024</v>
       </c>
       <c r="J52" s="2" t="s">
-        <v>375</v>
+        <v>385</v>
       </c>
       <c r="K52" s="2">
         <v>1</v>
@@ -20558,7 +20633,7 @@
         <v>11</v>
       </c>
       <c r="N52" s="2" t="s">
-        <v>376</v>
+        <v>386</v>
       </c>
       <c r="O52" s="2" t="s">
         <v>68</v>
@@ -20604,10 +20679,10 @@
       </c>
       <c r="AI52" s="2"/>
       <c r="AJ52" s="2" t="s">
-        <v>377</v>
+        <v>387</v>
       </c>
       <c r="AK52" s="2" t="s">
-        <v>378</v>
+        <v>388</v>
       </c>
       <c r="AL52" s="2"/>
       <c r="AM52" s="2"/>
@@ -20908,7 +20983,7 @@
       <c r="AI53" s="2"/>
       <c r="AJ53" s="2"/>
       <c r="AK53" s="2" t="s">
-        <v>379</v>
+        <v>389</v>
       </c>
       <c r="AL53" s="2"/>
       <c r="AM53" s="2"/>
@@ -25420,6 +25495,13 @@
     <hyperlink ref="AL27" r:id="rId24" display="https://osf.io/cj7fp/"/>
     <hyperlink ref="AL29" r:id="rId25" display="https://osf.io/4n6j7/"/>
     <hyperlink ref="AL30" r:id="rId26" display="https://zenodo.org/records/8031086"/>
+    <hyperlink ref="AL40" r:id="rId27" display="https://osf.io/u9ty6/?view_only=9bdbbaf95f9a4d9c8bc53dd1a29563ae."/>
+    <hyperlink ref="AL42" r:id="rId28" display="https://doi.org/10.17605/OSF.IO/FE3JW"/>
+    <hyperlink ref="AL43" r:id="rId28" display="https://doi.org/10.17605/OSF.IO/FE3JW"/>
+    <hyperlink ref="AL44" r:id="rId29" display="https://doi.org/10.26180/20011142"/>
+    <hyperlink ref="AL45" r:id="rId30" display="https://osf.io/35wp9" tooltip="https://osf.io/35wp9"/>
+    <hyperlink ref="AL46" r:id="rId30" display="https://osf.io/35wp9" tooltip="https://osf.io/35wp9"/>
+    <hyperlink ref="AL47" r:id="rId30" display="https://osf.io/35wp9" tooltip="https://osf.io/35wp9"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait"/>

</xml_diff>